<commit_message>
updating scripts + sheets for reproductive content
</commit_message>
<xml_diff>
--- a/input/images/IJE_File_Layouts_and_FHIR_Mapping_24-06-21.xlsx
+++ b/input/images/IJE_File_Layouts_and_FHIR_Mapping_24-06-21.xlsx
@@ -6292,7 +6292,7 @@
 U = Unknown</t>
   </si>
   <si>
-    <t>ProcedureArtificialInsemination</t>
+    <t>ProcedureFertilityEnhancingDrugTherapyArtificialInsemination</t>
   </si>
   <si>
     <t>Remove Observation-pregnancy-risk-factor</t>
@@ -6307,7 +6307,7 @@
     <t>Y, N, X, U  (BLANK IF NOT ADDED)</t>
   </si>
   <si>
-    <t>ProcedureAssistedFertilization</t>
+    <t>ProcedureAssistedReproductiveTechnology</t>
   </si>
   <si>
     <t>4 digit year; &gt;=year of delivery, Blank (Date of Registration must be a valid date or entirely blank; no portions of the date may be unknown)</t>
@@ -9639,7 +9639,7 @@
   <sheetPr>
     <tabColor rgb="FFCCFFCC"/>
   </sheetPr>
-  <dimension ref="A1:S277"/>
+  <dimension ref="A1:R277"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -9656,7 +9656,7 @@
     <col min="15" max="18" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:18">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -9711,9 +9711,8 @@
       <c r="R1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="S1" s="3"/>
-    </row>
-    <row r="2" spans="1:19">
+    </row>
+    <row r="2" spans="1:18">
       <c r="A2">
         <v>1</v>
       </c>
@@ -9756,7 +9755,7 @@
       </c>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:18">
       <c r="A3">
         <v>2</v>
       </c>
@@ -9799,7 +9798,7 @@
       </c>
       <c r="P3" s="1"/>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:18">
       <c r="A4">
         <v>6</v>
       </c>
@@ -9842,7 +9841,7 @@
       </c>
       <c r="P4" s="1"/>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:18">
       <c r="A5">
         <v>6</v>
       </c>
@@ -9882,7 +9881,7 @@
       <c r="N5" s="1"/>
       <c r="P5" s="1"/>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:18">
       <c r="A6">
         <v>7</v>
       </c>
@@ -9925,7 +9924,7 @@
       </c>
       <c r="P6" s="1"/>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:18">
       <c r="A7">
         <v>8</v>
       </c>
@@ -9968,7 +9967,7 @@
       </c>
       <c r="P7" s="1"/>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:18">
       <c r="A8">
         <v>9</v>
       </c>
@@ -10011,7 +10010,7 @@
       </c>
       <c r="P8" s="1"/>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:18">
       <c r="A9">
         <v>9</v>
       </c>
@@ -10050,7 +10049,7 @@
       </c>
       <c r="P9" s="1"/>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:18">
       <c r="A10">
         <v>10</v>
       </c>
@@ -10093,7 +10092,7 @@
       </c>
       <c r="P10" s="1"/>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:18">
       <c r="A11">
         <v>11</v>
       </c>
@@ -10136,7 +10135,7 @@
       </c>
       <c r="P11" s="1"/>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:18">
       <c r="A12">
         <v>12</v>
       </c>
@@ -10179,7 +10178,7 @@
       </c>
       <c r="P12" s="1"/>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:18">
       <c r="A13">
         <v>13</v>
       </c>
@@ -10222,7 +10221,7 @@
       </c>
       <c r="P13" s="1"/>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:18">
       <c r="A14">
         <v>13</v>
       </c>
@@ -10265,7 +10264,7 @@
       </c>
       <c r="P14" s="1"/>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:18">
       <c r="A15">
         <v>14</v>
       </c>
@@ -10306,7 +10305,7 @@
       </c>
       <c r="P15" s="1"/>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:18">
       <c r="A16">
         <v>15</v>
       </c>
@@ -21119,7 +21118,7 @@
   <sheetPr>
     <tabColor rgb="FFFF99CC"/>
   </sheetPr>
-  <dimension ref="A1:S46"/>
+  <dimension ref="A1:R46"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -21136,7 +21135,7 @@
     <col min="15" max="18" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:18">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
@@ -21191,9 +21190,8 @@
       <c r="R1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="S1" s="5"/>
-    </row>
-    <row r="2" spans="1:19">
+    </row>
+    <row r="2" spans="1:18">
       <c r="B2">
         <v>1</v>
       </c>
@@ -21230,7 +21228,7 @@
       <c r="N2" s="1"/>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:18">
       <c r="B3" t="s">
         <v>42</v>
       </c>
@@ -21265,7 +21263,7 @@
       <c r="N3" s="1"/>
       <c r="P3" s="1"/>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:18">
       <c r="B4" t="s">
         <v>42</v>
       </c>
@@ -21300,7 +21298,7 @@
       <c r="N4" s="1"/>
       <c r="P4" s="1"/>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:18">
       <c r="B5" t="s">
         <v>42</v>
       </c>
@@ -21335,7 +21333,7 @@
       <c r="N5" s="1"/>
       <c r="P5" s="1"/>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:18">
       <c r="B6" t="s">
         <v>42</v>
       </c>
@@ -21372,7 +21370,7 @@
       <c r="N6" s="1"/>
       <c r="P6" s="1"/>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:18">
       <c r="B7" t="s">
         <v>946</v>
       </c>
@@ -21409,7 +21407,7 @@
       </c>
       <c r="P7" s="1"/>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:18">
       <c r="B8" t="s">
         <v>42</v>
       </c>
@@ -21446,7 +21444,7 @@
       <c r="N8" s="1"/>
       <c r="P8" s="1"/>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:18">
       <c r="B9" t="s">
         <v>42</v>
       </c>
@@ -21483,7 +21481,7 @@
       <c r="N9" s="1"/>
       <c r="P9" s="1"/>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:18">
       <c r="B10" t="s">
         <v>42</v>
       </c>
@@ -21520,7 +21518,7 @@
       <c r="N10" s="1"/>
       <c r="P10" s="1"/>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:18">
       <c r="B11" t="s">
         <v>42</v>
       </c>
@@ -21557,7 +21555,7 @@
       <c r="N11" s="1"/>
       <c r="P11" s="1"/>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:18">
       <c r="B12" t="s">
         <v>42</v>
       </c>
@@ -21594,7 +21592,7 @@
       <c r="N12" s="1"/>
       <c r="P12" s="1"/>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:18">
       <c r="A13">
         <v>431</v>
       </c>
@@ -21634,7 +21632,7 @@
       <c r="N13" s="1"/>
       <c r="P13" s="1"/>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:18">
       <c r="A14">
         <v>432</v>
       </c>
@@ -21674,7 +21672,7 @@
       <c r="N14" s="1"/>
       <c r="P14" s="1"/>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:18">
       <c r="A15">
         <v>433</v>
       </c>
@@ -21714,7 +21712,7 @@
       <c r="N15" s="1"/>
       <c r="P15" s="1"/>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:18">
       <c r="A16">
         <v>434</v>
       </c>
@@ -22972,7 +22970,7 @@
   <sheetPr>
     <tabColor rgb="FFCCFFCC"/>
   </sheetPr>
-  <dimension ref="A1:S160"/>
+  <dimension ref="A1:R160"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -22989,7 +22987,7 @@
     <col min="15" max="18" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:18">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -23044,9 +23042,8 @@
       <c r="R1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="S1" s="3"/>
-    </row>
-    <row r="2" spans="1:19">
+    </row>
+    <row r="2" spans="1:18">
       <c r="A2">
         <v>272</v>
       </c>
@@ -23089,7 +23086,7 @@
       </c>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:18">
       <c r="A3">
         <v>430</v>
       </c>
@@ -23129,7 +23126,7 @@
       <c r="N3" s="1"/>
       <c r="P3" s="1"/>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:18">
       <c r="A4">
         <v>273</v>
       </c>
@@ -23172,7 +23169,7 @@
       </c>
       <c r="P4" s="1"/>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:18">
       <c r="A5">
         <v>275</v>
       </c>
@@ -23215,7 +23212,7 @@
       </c>
       <c r="P5" s="1"/>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:18">
       <c r="A6">
         <v>276</v>
       </c>
@@ -23258,7 +23255,7 @@
       </c>
       <c r="P6" s="1"/>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:18">
       <c r="A7">
         <v>277</v>
       </c>
@@ -23299,7 +23296,7 @@
       </c>
       <c r="P7" s="1"/>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:18">
       <c r="A8">
         <v>278</v>
       </c>
@@ -23340,7 +23337,7 @@
       </c>
       <c r="P8" s="1"/>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:18">
       <c r="A9">
         <v>279</v>
       </c>
@@ -23383,7 +23380,7 @@
       </c>
       <c r="P9" s="1"/>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:18">
       <c r="A10">
         <v>280</v>
       </c>
@@ -23424,7 +23421,7 @@
       </c>
       <c r="P10" s="1"/>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:18">
       <c r="A11">
         <v>281</v>
       </c>
@@ -23465,7 +23462,7 @@
       </c>
       <c r="P11" s="1"/>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:18">
       <c r="A12">
         <v>282</v>
       </c>
@@ -23508,7 +23505,7 @@
       </c>
       <c r="P12" s="1"/>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:18">
       <c r="A13">
         <v>283</v>
       </c>
@@ -23551,7 +23548,7 @@
       </c>
       <c r="P13" s="1"/>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:18">
       <c r="A14">
         <v>284</v>
       </c>
@@ -23594,7 +23591,7 @@
       </c>
       <c r="P14" s="1"/>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:18">
       <c r="A15">
         <v>285</v>
       </c>
@@ -23637,7 +23634,7 @@
       </c>
       <c r="P15" s="1"/>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:18">
       <c r="A16">
         <v>286</v>
       </c>
@@ -29770,7 +29767,7 @@
   <sheetPr>
     <tabColor rgb="FFCC99FF"/>
   </sheetPr>
-  <dimension ref="A1:S160"/>
+  <dimension ref="A1:R160"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -29787,7 +29784,7 @@
     <col min="15" max="18" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:18">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -29842,9 +29839,8 @@
       <c r="R1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="S1" s="6"/>
-    </row>
-    <row r="2" spans="1:19">
+    </row>
+    <row r="2" spans="1:18">
       <c r="A2">
         <v>1183</v>
       </c>
@@ -29877,7 +29873,7 @@
       <c r="N2" s="1"/>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:18">
       <c r="A3">
         <v>1184</v>
       </c>
@@ -29910,7 +29906,7 @@
       <c r="N3" s="1"/>
       <c r="P3" s="1"/>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:18">
       <c r="A4">
         <v>1185</v>
       </c>
@@ -29943,7 +29939,7 @@
       <c r="N4" s="1"/>
       <c r="P4" s="1"/>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:18">
       <c r="A5">
         <v>1186</v>
       </c>
@@ -29976,7 +29972,7 @@
       <c r="N5" s="1"/>
       <c r="P5" s="1"/>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:18">
       <c r="A6">
         <v>1187</v>
       </c>
@@ -30009,7 +30005,7 @@
       <c r="N6" s="1"/>
       <c r="P6" s="1"/>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:18">
       <c r="A7">
         <v>1188</v>
       </c>
@@ -30042,7 +30038,7 @@
       <c r="N7" s="1"/>
       <c r="P7" s="1"/>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:18">
       <c r="A8">
         <v>1189</v>
       </c>
@@ -30075,7 +30071,7 @@
       <c r="N8" s="1"/>
       <c r="P8" s="1"/>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:18">
       <c r="A9">
         <v>1190</v>
       </c>
@@ -30108,7 +30104,7 @@
       <c r="N9" s="1"/>
       <c r="P9" s="1"/>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:18">
       <c r="A10">
         <v>1191</v>
       </c>
@@ -30141,7 +30137,7 @@
       <c r="N10" s="1"/>
       <c r="P10" s="1"/>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:18">
       <c r="A11">
         <v>1192</v>
       </c>
@@ -30174,7 +30170,7 @@
       <c r="N11" s="1"/>
       <c r="P11" s="1"/>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:18">
       <c r="A12">
         <v>1193</v>
       </c>
@@ -30207,7 +30203,7 @@
       <c r="N12" s="1"/>
       <c r="P12" s="1"/>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:18">
       <c r="A13">
         <v>1194</v>
       </c>
@@ -30240,7 +30236,7 @@
       <c r="N13" s="1"/>
       <c r="P13" s="1"/>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:18">
       <c r="A14">
         <v>1195</v>
       </c>
@@ -30273,7 +30269,7 @@
       <c r="N14" s="1"/>
       <c r="P14" s="1"/>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:18">
       <c r="A15">
         <v>1196</v>
       </c>
@@ -30306,7 +30302,7 @@
       <c r="N15" s="1"/>
       <c r="P15" s="1"/>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:18">
       <c r="A16">
         <v>1197</v>
       </c>
@@ -35102,7 +35098,7 @@
   <sheetPr>
     <tabColor rgb="FFFFCC99"/>
   </sheetPr>
-  <dimension ref="A1:S370"/>
+  <dimension ref="A1:R370"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -35119,7 +35115,7 @@
     <col min="15" max="18" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:18">
       <c r="A1" s="7" t="s">
         <v>1</v>
       </c>
@@ -35174,9 +35170,8 @@
       <c r="R1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="S1" s="7"/>
-    </row>
-    <row r="2" spans="1:19">
+    </row>
+    <row r="2" spans="1:18">
       <c r="A2">
         <v>818</v>
       </c>
@@ -35218,7 +35213,7 @@
       </c>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:18">
       <c r="A3">
         <v>819</v>
       </c>
@@ -35260,7 +35255,7 @@
       </c>
       <c r="P3" s="1"/>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:18">
       <c r="A4">
         <v>820</v>
       </c>
@@ -35299,7 +35294,7 @@
       </c>
       <c r="P4" s="1"/>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:18">
       <c r="A5">
         <v>820</v>
       </c>
@@ -35338,7 +35333,7 @@
       </c>
       <c r="P5" s="1"/>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:18">
       <c r="A6">
         <v>820</v>
       </c>
@@ -35377,7 +35372,7 @@
       </c>
       <c r="P6" s="1"/>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:18">
       <c r="A7">
         <v>821</v>
       </c>
@@ -35415,7 +35410,7 @@
       </c>
       <c r="P7" s="1"/>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:18">
       <c r="A8">
         <v>822</v>
       </c>
@@ -35454,7 +35449,7 @@
       </c>
       <c r="P8" s="1"/>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:18">
       <c r="A9">
         <v>822</v>
       </c>
@@ -35493,7 +35488,7 @@
       </c>
       <c r="P9" s="1"/>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:18">
       <c r="A10">
         <v>822</v>
       </c>
@@ -35532,7 +35527,7 @@
       </c>
       <c r="P10" s="1"/>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:18">
       <c r="A11">
         <v>823</v>
       </c>
@@ -35574,7 +35569,7 @@
       </c>
       <c r="P11" s="1"/>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:18">
       <c r="A12">
         <v>824</v>
       </c>
@@ -35616,7 +35611,7 @@
       </c>
       <c r="P12" s="1"/>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:18">
       <c r="A13">
         <v>825</v>
       </c>
@@ -35658,7 +35653,7 @@
       </c>
       <c r="P13" s="1"/>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:18">
       <c r="A14">
         <v>826</v>
       </c>
@@ -35700,7 +35695,7 @@
       </c>
       <c r="P14" s="1"/>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:18">
       <c r="A15">
         <v>827</v>
       </c>
@@ -35742,7 +35737,7 @@
       </c>
       <c r="P15" s="1"/>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:18">
       <c r="A16">
         <v>828</v>
       </c>
@@ -49875,7 +49870,7 @@
   <sheetPr>
     <tabColor rgb="FFCCFFFF"/>
   </sheetPr>
-  <dimension ref="A1:S368"/>
+  <dimension ref="A1:R368"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -49892,7 +49887,7 @@
     <col min="15" max="18" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:18">
       <c r="A1" s="8" t="s">
         <v>1</v>
       </c>
@@ -49947,9 +49942,8 @@
       <c r="R1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="S1" s="8"/>
-    </row>
-    <row r="2" spans="1:19">
+    </row>
+    <row r="2" spans="1:18">
       <c r="A2">
         <v>465</v>
       </c>
@@ -49991,7 +49985,7 @@
       </c>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:18">
       <c r="A3">
         <v>466</v>
       </c>
@@ -50033,7 +50027,7 @@
       </c>
       <c r="P3" s="1"/>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:18">
       <c r="A4">
         <v>467</v>
       </c>
@@ -50072,7 +50066,7 @@
       </c>
       <c r="P4" s="1"/>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:18">
       <c r="A5">
         <v>467</v>
       </c>
@@ -50111,7 +50105,7 @@
       </c>
       <c r="P5" s="1"/>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:18">
       <c r="A6">
         <v>467</v>
       </c>
@@ -50150,7 +50144,7 @@
       </c>
       <c r="P6" s="1"/>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:18">
       <c r="A7">
         <v>468</v>
       </c>
@@ -50188,7 +50182,7 @@
       </c>
       <c r="P7" s="1"/>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:18">
       <c r="A8">
         <v>469</v>
       </c>
@@ -50227,7 +50221,7 @@
       </c>
       <c r="P8" s="1"/>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:18">
       <c r="A9">
         <v>469</v>
       </c>
@@ -50266,7 +50260,7 @@
       </c>
       <c r="P9" s="1"/>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:18">
       <c r="A10">
         <v>469</v>
       </c>
@@ -50305,7 +50299,7 @@
       </c>
       <c r="P10" s="1"/>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:18">
       <c r="A11" t="s">
         <v>42</v>
       </c>
@@ -50344,7 +50338,7 @@
       </c>
       <c r="P11" s="1"/>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:18">
       <c r="A12" t="s">
         <v>42</v>
       </c>
@@ -50383,7 +50377,7 @@
       </c>
       <c r="P12" s="1"/>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:18">
       <c r="A13" t="s">
         <v>42</v>
       </c>
@@ -50422,7 +50416,7 @@
       </c>
       <c r="P13" s="1"/>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:18">
       <c r="A14" t="s">
         <v>42</v>
       </c>
@@ -50461,7 +50455,7 @@
       </c>
       <c r="P14" s="1"/>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:18">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -50500,7 +50494,7 @@
       </c>
       <c r="P15" s="1"/>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:18">
       <c r="A16" t="s">
         <v>42</v>
       </c>
@@ -64828,7 +64822,7 @@
   <sheetPr>
     <tabColor rgb="FFC4BD97"/>
   </sheetPr>
-  <dimension ref="A1:S350"/>
+  <dimension ref="A1:R350"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -64845,7 +64839,7 @@
     <col min="15" max="18" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:18">
       <c r="A1" s="9" t="s">
         <v>1</v>
       </c>
@@ -64900,9 +64894,8 @@
       <c r="R1" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="S1" s="9"/>
-    </row>
-    <row r="2" spans="1:19">
+    </row>
+    <row r="2" spans="1:18">
       <c r="A2">
         <v>1342</v>
       </c>
@@ -64929,7 +64922,7 @@
       <c r="N2" s="1"/>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:18">
       <c r="A3">
         <v>1343</v>
       </c>
@@ -64956,7 +64949,7 @@
       <c r="N3" s="1"/>
       <c r="P3" s="1"/>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:18">
       <c r="A4">
         <v>1344</v>
       </c>
@@ -64983,7 +64976,7 @@
       <c r="N4" s="1"/>
       <c r="P4" s="1"/>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:18">
       <c r="A5">
         <v>1345</v>
       </c>
@@ -65010,7 +65003,7 @@
       <c r="N5" s="1"/>
       <c r="P5" s="1"/>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:18">
       <c r="A6">
         <v>1346</v>
       </c>
@@ -65037,7 +65030,7 @@
       <c r="N6" s="1"/>
       <c r="P6" s="1"/>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:18">
       <c r="A7">
         <v>1347</v>
       </c>
@@ -65064,7 +65057,7 @@
       <c r="N7" s="1"/>
       <c r="P7" s="1"/>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:18">
       <c r="A8">
         <v>1348</v>
       </c>
@@ -65091,7 +65084,7 @@
       <c r="N8" s="1"/>
       <c r="P8" s="1"/>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:18">
       <c r="A9">
         <v>1349</v>
       </c>
@@ -65118,7 +65111,7 @@
       <c r="N9" s="1"/>
       <c r="P9" s="1"/>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:18">
       <c r="A10">
         <v>1350</v>
       </c>
@@ -65145,7 +65138,7 @@
       <c r="N10" s="1"/>
       <c r="P10" s="1"/>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:18">
       <c r="A11">
         <v>1351</v>
       </c>
@@ -65172,7 +65165,7 @@
       <c r="N11" s="1"/>
       <c r="P11" s="1"/>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:18">
       <c r="A12">
         <v>1352</v>
       </c>
@@ -65199,7 +65192,7 @@
       <c r="N12" s="1"/>
       <c r="P12" s="1"/>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:18">
       <c r="A13">
         <v>1353</v>
       </c>
@@ -65224,7 +65217,7 @@
       <c r="N13" s="1"/>
       <c r="P13" s="1"/>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:18">
       <c r="A14">
         <v>1354</v>
       </c>
@@ -65249,7 +65242,7 @@
       <c r="N14" s="1"/>
       <c r="P14" s="1"/>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:18">
       <c r="A15">
         <v>1355</v>
       </c>
@@ -65276,7 +65269,7 @@
       <c r="N15" s="1"/>
       <c r="P15" s="1"/>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:18">
       <c r="A16">
         <v>1356</v>
       </c>

</xml_diff>

<commit_message>
final route VS note
</commit_message>
<xml_diff>
--- a/input/images/IJE_File_Layouts_and_FHIR_Mapping_24-06-21.xlsx
+++ b/input/images/IJE_File_Layouts_and_FHIR_Mapping_24-06-21.xlsx
@@ -125,26 +125,26 @@
     <t>DSTATE</t>
   </si>
   <si>
-    <t>NCHS Instruction Manual: Part 8
-For U.S. Territories:
-   MP  NORTHERN MARIANAS
-   AS  AMERICAN SAMOA
-   GU  GUAM
-   VI   VIRGIN ISLANDS
-   PR  PUERTO RICO
-For Canadian Provinces:
-   AB  ALBERTA  
-   BC  BRITISH COLUMBIA 
-   MB  MANITOBA 
-   NB  NEW BRUNSWICK  
-   NL  NEWFOUNDLAND AND LABRADOR  
-   NS  NOVA SCOTIA 
-   NT  NORTHWEST TERRITORIES
-   NU  NUNAVUT
-   ON  ONTARIO
-   PE  PRINCE EDWARD ISLAND 
-   QC  QUEBEC  
-   SK  SASKATCHEWAN
+    <t>NCHS Instruction Manual: Part 8_x000D_
+For U.S. Territories:_x000D_
+   MP  NORTHERN MARIANAS_x000D_
+   AS  AMERICAN SAMOA_x000D_
+   GU  GUAM_x000D_
+   VI   VIRGIN ISLANDS_x000D_
+   PR  PUERTO RICO_x000D_
+For Canadian Provinces:_x000D_
+   AB  ALBERTA  _x000D_
+   BC  BRITISH COLUMBIA _x000D_
+   MB  MANITOBA _x000D_
+   NB  NEW BRUNSWICK  _x000D_
+   NL  NEWFOUNDLAND AND LABRADOR  _x000D_
+   NS  NOVA SCOTIA _x000D_
+   NT  NORTHWEST TERRITORIES_x000D_
+   NU  NUNAVUT_x000D_
+   ON  ONTARIO_x000D_
+   PE  PRINCE EDWARD ISLAND _x000D_
+   QC  QUEBEC  _x000D_
+   SK  SASKATCHEWAN_x000D_
    YT  YUKON</t>
   </si>
   <si>
@@ -214,7 +214,7 @@
     <t>VOID</t>
   </si>
   <si>
-    <t>0 =Default; Valid Record
+    <t>0 =Default; Valid Record_x000D_
 1 = VOID record</t>
   </si>
   <si>
@@ -251,8 +251,8 @@
     <t>MFILED</t>
   </si>
   <si>
-    <t>0 = Electronic Mode
-1 = Paper Mode
+    <t>0 = Electronic Mode_x000D_
+1 = Paper Mode_x000D_
 2 = Mixed Mode</t>
   </si>
   <si>
@@ -316,7 +316,7 @@
     <t>ALIAS</t>
   </si>
   <si>
-    <t>0 = Original Record
+    <t>0 = Original Record_x000D_
 1 = Alias Record</t>
   </si>
   <si>
@@ -341,8 +341,8 @@
     <t>SEX</t>
   </si>
   <si>
-    <t>M = Male
-F = Female
+    <t>M = Male_x000D_
+F = Female_x000D_
 U = Unknown</t>
   </si>
   <si>
@@ -358,7 +358,7 @@
     <t>SEX_BYPASS</t>
   </si>
   <si>
-    <t>0 = Edit Passed
+    <t>0 = Edit Passed_x000D_
 1 = Edit Failed, Data Queried, and Verified</t>
   </si>
   <si>
@@ -380,11 +380,11 @@
     <t>AGETYPE</t>
   </si>
   <si>
-    <t>1 = Years
-2 = Months
-4 = Days
-5 = Hours
-6 = Minutes
+    <t>1 = Years_x000D_
+2 = Months_x000D_
+4 = Days_x000D_
+5 = Hours_x000D_
+6 = Minutes_x000D_
 9 = Unknown (not classifiable)</t>
   </si>
   <si>
@@ -403,12 +403,12 @@
     <t xml:space="preserve">AGE </t>
   </si>
   <si>
-    <t>001 - 135, 999
-Codes: If AGETYPE = 1 then 001-135, 999
-                                        2 then 001-011, 999
-                                        4 then 001-027, 999
-                                        5 then 001-023, 999
-                                        6 then 001-059, 999
+    <t>001 - 135, 999_x000D_
+Codes: If AGETYPE = 1 then 001-135, 999_x000D_
+                                        2 then 001-011, 999_x000D_
+                                        4 then 001-027, 999_x000D_
+                                        5 then 001-023, 999_x000D_
+                                        6 then 001-059, 999_x000D_
                                         9 then 999</t>
   </si>
   <si>
@@ -484,28 +484,28 @@
     <t>BPLACE_ST</t>
   </si>
   <si>
-    <t>NCHS Instruction Manual: Part 8
-   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY
-   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA 
-For U.S. Territories:
-   MP  NORTHERN MARIANAS
-   AS  AMERICAN SAMOA
-   GU  GUAM
-   VI   VIRGIN ISLANDS
-   PR  PUERTO RICO
-For Canadian Provinces:
-   AB  ALBERTA  
-   BC  BRITISH COLUMBIA 
-   MB  MANITOBA 
-   NB  NEW BRUNSWICK  
-   NL  NEWFOUNDLAND AND LABRADOR
-   NS  NOVA SCOTIA 
-   NT  NORTHWEST TERRITORIES
-   NU  NUNAVUT
-   ON  ONTARIO
-   PE  PRINCE EDWARD ISLAND 
-   QC  QUEBEC  
-   SK  SASKATCHEWAN
+    <t>NCHS Instruction Manual: Part 8_x000D_
+   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY_x000D_
+   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA _x000D_
+For U.S. Territories:_x000D_
+   MP  NORTHERN MARIANAS_x000D_
+   AS  AMERICAN SAMOA_x000D_
+   GU  GUAM_x000D_
+   VI   VIRGIN ISLANDS_x000D_
+   PR  PUERTO RICO_x000D_
+For Canadian Provinces:_x000D_
+   AB  ALBERTA  _x000D_
+   BC  BRITISH COLUMBIA _x000D_
+   MB  MANITOBA _x000D_
+   NB  NEW BRUNSWICK  _x000D_
+   NL  NEWFOUNDLAND AND LABRADOR_x000D_
+   NS  NOVA SCOTIA _x000D_
+   NT  NORTHWEST TERRITORIES_x000D_
+   NU  NUNAVUT_x000D_
+   ON  ONTARIO_x000D_
+   PE  PRINCE EDWARD ISLAND _x000D_
+   QC  QUEBEC  _x000D_
+   SK  SASKATCHEWAN_x000D_
    YT  YUKON</t>
   </si>
   <si>
@@ -548,28 +548,28 @@
     <t>STATEC</t>
   </si>
   <si>
-    <t>NCHS Instruction Manual: Part 8
-   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY
-   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA 
-For U.S. Territories:
-   MP  NORTHERN MARIANAS
-   AS  AMERICAN SAMOA
-   GU  GUAM
-   VI   VIRGIN ISLANDS
-   PR  PUERTO RICO
-For Canadian Provinces:
-   AB  ALBERTA  
-   BC  BRITISH COLUMBIA 
-   MB  MANITOBA 
-   NB  NEW BRUNSWICK  
-   NL  NEWFOUNDLAND AND LABRADOR  
-   NS  NOVA SCOTIA 
-   NT  NORTHWEST TERRITORIES
-   NU  NUNAVUT
-   ON  ONTARIO
-   PE  PRINCE EDWARD ISLAND 
-   QC  QUEBEC  
-   SK  SASKATCHEWAN
+    <t>NCHS Instruction Manual: Part 8_x000D_
+   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY_x000D_
+   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA _x000D_
+For U.S. Territories:_x000D_
+   MP  NORTHERN MARIANAS_x000D_
+   AS  AMERICAN SAMOA_x000D_
+   GU  GUAM_x000D_
+   VI   VIRGIN ISLANDS_x000D_
+   PR  PUERTO RICO_x000D_
+For Canadian Provinces:_x000D_
+   AB  ALBERTA  _x000D_
+   BC  BRITISH COLUMBIA _x000D_
+   MB  MANITOBA _x000D_
+   NB  NEW BRUNSWICK  _x000D_
+   NL  NEWFOUNDLAND AND LABRADOR  _x000D_
+   NS  NOVA SCOTIA _x000D_
+   NT  NORTHWEST TERRITORIES_x000D_
+   NU  NUNAVUT_x000D_
+   ON  ONTARIO_x000D_
+   PE  PRINCE EDWARD ISLAND _x000D_
+   QC  QUEBEC  _x000D_
+   SK  SASKATCHEWAN_x000D_
    YT  YUKON</t>
   </si>
   <si>
@@ -609,11 +609,11 @@
     <t>MARITAL</t>
   </si>
   <si>
-    <t>M = Married
-A = Married but Separated
-W = Widowed
-D = Divorced
-S = Never Married
+    <t>M = Married_x000D_
+A = Married but Separated_x000D_
+W = Widowed_x000D_
+D = Divorced_x000D_
+S = Never Married_x000D_
 U = Not Classifiable</t>
   </si>
   <si>
@@ -629,9 +629,9 @@
     <t>MARITAL_BYPASS</t>
   </si>
   <si>
-    <t>0 = Edit Passed
-1 = Edit Failed, Data Queried, and Verified
-2 = Edit Failed, Data Queried, but not Verified
+    <t>0 = Edit Passed_x000D_
+1 = Edit Failed, Data Queried, and Verified_x000D_
+2 = Edit Failed, Data Queried, but not Verified_x000D_
 4 = Edit Failed, Query Needed</t>
   </si>
   <si>
@@ -647,13 +647,13 @@
     <t>DPLACE</t>
   </si>
   <si>
-    <t>1 = Inpatient
-2 = Emergency Room/Outpatient
-3 = Dead on Arrival
-4 = Decedent's Home
-5 = Hospice Facility
-6 = Nursing Home/Long Term Care Facility
-7 = Other
+    <t>1 = Inpatient_x000D_
+2 = Emergency Room/Outpatient_x000D_
+3 = Dead on Arrival_x000D_
+4 = Decedent's Home_x000D_
+5 = Hospice Facility_x000D_
+6 = Nursing Home/Long Term Care Facility_x000D_
+7 = Other_x000D_
 9 = Unknown</t>
   </si>
   <si>
@@ -669,7 +669,7 @@
     <t>COD</t>
   </si>
   <si>
-    <t>NCHS Instruction Manual: Part 8
+    <t>NCHS Instruction Manual: Part 8_x000D_
 Variable description ("Contents") edited; same as NCHS "Facility Name--County"</t>
   </si>
   <si>
@@ -679,12 +679,12 @@
     <t>DISP</t>
   </si>
   <si>
-    <t>B = Burial
-C = Cremation
-D = Donation
-E = Entombment
-R = Removal from state
-O = Other
+    <t>B = Burial_x000D_
+C = Cremation_x000D_
+D = Donation_x000D_
+E = Entombment_x000D_
+R = Removal from state_x000D_
+O = Other_x000D_
 U = Unknown</t>
   </si>
   <si>
@@ -721,14 +721,14 @@
     <t>DEDUC</t>
   </si>
   <si>
-    <t>1 = 8th grade or less
-2 = 9th through 12th grade; no diploma
-3 = High School Graduate or GED Completed
-4 = Some college credit, but no degree
-5 = Associate Degree
-6 = Bachelor's Degree
-7 = Master's Degree
-8 = Doctorate Degree or Professional Degree
+    <t>1 = 8th grade or less_x000D_
+2 = 9th through 12th grade; no diploma_x000D_
+3 = High School Graduate or GED Completed_x000D_
+4 = Some college credit, but no degree_x000D_
+5 = Associate Degree_x000D_
+6 = Bachelor's Degree_x000D_
+7 = Master's Degree_x000D_
+8 = Doctorate Degree or Professional Degree_x000D_
 9 = Unknown</t>
   </si>
   <si>
@@ -744,10 +744,10 @@
     <t>DEDUC_BYPASS</t>
   </si>
   <si>
-    <t>0 = Edit Passed
-1 = Edit Failed, Data Queried, and Verified
-2 = Edit Failed, Data Queried, but not Verified
-3 = Edit Failed, Review Needed
+    <t>0 = Edit Passed_x000D_
+1 = Edit Failed, Data Queried, and Verified_x000D_
+2 = Edit Failed, Data Queried, but not Verified_x000D_
+3 = Edit Failed, Review Needed_x000D_
 4 = Edit Failed, Query Needed</t>
   </si>
   <si>
@@ -763,8 +763,8 @@
     <t>DETHNIC1</t>
   </si>
   <si>
-    <t>N = No, Not Mexican
-H = Yes, Mexican
+    <t>N = No, Not Mexican_x000D_
+H = Yes, Mexican_x000D_
 U = Unknown</t>
   </si>
   <si>
@@ -783,8 +783,8 @@
     <t>DETHNIC2</t>
   </si>
   <si>
-    <t>N = No, Not Puerto Rican
-H = Yes, Puerto Rican
+    <t>N = No, Not Puerto Rican_x000D_
+H = Yes, Puerto Rican_x000D_
 U = Unknown</t>
   </si>
   <si>
@@ -797,8 +797,8 @@
     <t>DETHNIC3</t>
   </si>
   <si>
-    <t>N = No, Not Cuban
-H = Yes, Cuban
+    <t>N = No, Not Cuban_x000D_
+H = Yes, Cuban_x000D_
 U = Unknown</t>
   </si>
   <si>
@@ -811,8 +811,8 @@
     <t>DETHNIC4</t>
   </si>
   <si>
-    <t>N = No, Not other Hispanic
-H = Yes, other Hispanic
+    <t>N = No, Not other Hispanic_x000D_
+H = Yes, other Hispanic_x000D_
 U = Unknown</t>
   </si>
   <si>
@@ -837,7 +837,7 @@
     <t>RACE1</t>
   </si>
   <si>
-    <t>Y = Yes, box for race checked
+    <t>Y = Yes, box for race checked_x000D_
 N = No, box for race not checked</t>
   </si>
   <si>
@@ -1213,8 +1213,8 @@
     <t>RACE_MVR</t>
   </si>
   <si>
-    <t>R = Refused
-S = Sought, but Unknown
+    <t>R = Refused_x000D_
+S = Sought, but Unknown_x000D_
 C = Not Obtainable</t>
   </si>
   <si>
@@ -1281,8 +1281,8 @@
     <t>IDOB_YR</t>
   </si>
   <si>
-    <t>4 digit year = year of death or (year of death - 1)
-9999 = unknown
+    <t>4 digit year = year of death or (year of death - 1)_x000D_
+9999 = unknown_x000D_
 Blank</t>
   </si>
   <si>
@@ -1298,29 +1298,30 @@
     <t>BSTATE</t>
   </si>
   <si>
-    <t>NCHS Instruction Manual: Part 8
-ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY
-XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA
-YC = NEW YORK CITY
-For US Territories:
-   MP  NORTHERN MARIANAS
-   AS  AMERICAN SAMOA
-   GU  GUAM
-   VI   VIRGIN ISLANDS
-   PR  PUERTO RICO
-For Canadian Provinces:
-   AB  ALBERTA  
-   BC  BRITISH COLUMBIA 
-   MB  MANITOBA 
-   NB  NEW BRUNSWICK  
-   NL  NEWFOUNDLAND AND LABRADOR  
-   NS  NOVA SCOTIA 
-   NT  NORTHWEST TERRITORIES
-   NU  NUNAVUT
-   ON  ONTARIO
-   PE  PRINCE EDWARD ISLAND 
-   QC  QUEBEC  
-   SK  SASKATCHEWAN
+    <t>NCHS Instruction Manual: Part 8_x000D_
+ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY_x000D_
+XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA_x000D_
+YC = NEW YORK CITY_x000D_
+_x000D_
+For US Territories:_x000D_
+   MP  NORTHERN MARIANAS_x000D_
+   AS  AMERICAN SAMOA_x000D_
+   GU  GUAM_x000D_
+   VI   VIRGIN ISLANDS_x000D_
+   PR  PUERTO RICO_x000D_
+For Canadian Provinces:_x000D_
+   AB  ALBERTA  _x000D_
+   BC  BRITISH COLUMBIA _x000D_
+   MB  MANITOBA _x000D_
+   NB  NEW BRUNSWICK  _x000D_
+   NL  NEWFOUNDLAND AND LABRADOR  _x000D_
+   NS  NOVA SCOTIA _x000D_
+   NT  NORTHWEST TERRITORIES_x000D_
+   NU  NUNAVUT_x000D_
+   ON  ONTARIO_x000D_
+   PE  PRINCE EDWARD ISLAND _x000D_
+   QC  QUEBEC  _x000D_
+   SK  SASKATCHEWAN_x000D_
    YT  YUKON</t>
   </si>
   <si>
@@ -1909,7 +1910,7 @@
     <t>SPOUSELV</t>
   </si>
   <si>
-    <t>1=yes; 2=no; 8=unmarried; 9=unknown;
+    <t>1=yes; 2=no; 8=unmarried; 9=unknown;_x000D_
 blank if not reported</t>
   </si>
   <si>
@@ -2042,7 +2043,7 @@
     <t>RESSTATE</t>
   </si>
   <si>
-    <t>See codes used before new 2003 codes -
+    <t>See codes used before new 2003 codes -_x000D_
 Receiving state will recode</t>
   </si>
   <si>
@@ -2058,8 +2059,8 @@
     <t xml:space="preserve">DETHNICE </t>
   </si>
   <si>
-    <t>100 = NonHispanic
-200-299 = Hispanic
+    <t>100 = NonHispanic_x000D_
+200-299 = Hispanic_x000D_
 996-999 = Unknown</t>
   </si>
   <si>
@@ -2183,9 +2184,9 @@
     <t>TRANSPRT</t>
   </si>
   <si>
-    <t>DR=Driver/Operator
-PA=Passenger
-PE=Pedestrian
+    <t>DR=Driver/Operator_x000D_
+PA=Passenger_x000D_
+PE=Pedestrian_x000D_
 Enter full text if it does not fit above (blank for natural death)</t>
   </si>
   <si>
@@ -2213,7 +2214,7 @@
     <t>COUNTYCODE_I</t>
   </si>
   <si>
-    <t>NCHS Instruction Manual: Part 8; 999=unknown; 
+    <t>NCHS Instruction Manual: Part 8; 999=unknown; _x000D_
 Blank for natural death.</t>
   </si>
   <si>
@@ -2247,27 +2248,27 @@
     <t>STATECODE_I</t>
   </si>
   <si>
-    <t>NCHS Instruction Manual: Part 8
-   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY
-   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA                                                                                 For U.S. Territories:
-   MP  NORTHERN MARIANAS
-   AS  AMERICAN SAMOA
-   GU  GUAM
-   VI   VIRGIN ISLANDS
-   PR  PUERTO RICO
-For Canadian Provinces:
-   AB  ALBERTA  
-   BC  BRITISH COLUMBIA 
-   MB  MANITOBA 
-   NB  NEW BRUNSWICK  
-   NL  NEWFOUNDLAND AND LABRADOR  
-   NS  NOVA SCOTIA 
-   NT  NORTHWEST TERRITORIES
-   NU  NUNAVUT
-   ON  ONTARIO
-   PE  PRINCE EDWARD ISLAND 
-   QC  QUEBEC  
-   SK  SASKATCHEWAN
+    <t>NCHS Instruction Manual: Part 8_x000D_
+   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY_x000D_
+   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA                                                                                 For U.S. Territories:_x000D_
+   MP  NORTHERN MARIANAS_x000D_
+   AS  AMERICAN SAMOA_x000D_
+   GU  GUAM_x000D_
+   VI   VIRGIN ISLANDS_x000D_
+   PR  PUERTO RICO_x000D_
+For Canadian Provinces:_x000D_
+   AB  ALBERTA  _x000D_
+   BC  BRITISH COLUMBIA _x000D_
+   MB  MANITOBA _x000D_
+   NB  NEW BRUNSWICK  _x000D_
+   NL  NEWFOUNDLAND AND LABRADOR  _x000D_
+   NS  NOVA SCOTIA _x000D_
+   NT  NORTHWEST TERRITORIES_x000D_
+   NU  NUNAVUT_x000D_
+   ON  ONTARIO_x000D_
+   PE  PRINCE EDWARD ISLAND _x000D_
+   QC  QUEBEC  _x000D_
+   SK  SASKATCHEWAN_x000D_
    YT  YUKON</t>
   </si>
   <si>
@@ -2499,27 +2500,27 @@
     <t>DISPSTATECD</t>
   </si>
   <si>
-    <t>NCHS Instruction Manual: Part 8
-   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY
-   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA                                                                                  For U.S. Territories:
-   MP  NORTHERN MARIANAS
-   AS  AMERICAN SAMOA
-   GU  GUAM
-   VI   VIRGIN ISLANDS
-   PR  PUERTO RICO
-For Canadian Provinces:
-   AB  ALBERTA  
-   BC  BRITISH COLUMBIA 
-   MB  MANITOBA 
-   NB  NEW BRUNSWICK  
-   NL NEWFOUNDLAND AND LABRADOR  
-   NS  NOVA SCOTIA 
-   NT  NORTHWEST TERRITORIES
-   NU  NUNAVUT
-   ON  ONTARIO
-   PE  PRINCE EDWARD ISLAND 
-   QC  QUEBEC  
-   SK  SASKATCHEWAN
+    <t>NCHS Instruction Manual: Part 8_x000D_
+   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY_x000D_
+   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA                                                                                  For U.S. Territories:_x000D_
+   MP  NORTHERN MARIANAS_x000D_
+   AS  AMERICAN SAMOA_x000D_
+   GU  GUAM_x000D_
+   VI   VIRGIN ISLANDS_x000D_
+   PR  PUERTO RICO_x000D_
+For Canadian Provinces:_x000D_
+   AB  ALBERTA  _x000D_
+   BC  BRITISH COLUMBIA _x000D_
+   MB  MANITOBA _x000D_
+   NB  NEW BRUNSWICK  _x000D_
+   NL NEWFOUNDLAND AND LABRADOR  _x000D_
+   NS  NOVA SCOTIA _x000D_
+   NT  NORTHWEST TERRITORIES_x000D_
+   NU  NUNAVUT_x000D_
+   ON  ONTARIO_x000D_
+   PE  PRINCE EDWARD ISLAND _x000D_
+   QC  QUEBEC  _x000D_
+   SK  SASKATCHEWAN_x000D_
    YT  YUKON</t>
   </si>
   <si>
@@ -2622,27 +2623,27 @@
     <t>FUNSTATECD</t>
   </si>
   <si>
-    <t>NCHS Instruction Manual: Part 8
-   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY
-   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA                                                                                       For U.S. Territories:
-   MP  NORTHERN MARIANAS
-   AS  AMERICAN SAMOA
-   GU  GUAM
-   VI   VIRGIN ISLANDS
-   PR  PUERTO RICO
-For Canadian Provinces:
-   AB  ALBERTA  
-   BC  BRITISH COLUMBIA 
-   MB  MANITOBA 
-   NB  NEW BRUNSWICK  
-   NL NEWFOUNDLAND AND LABRADOR
-   NS  NOVA SCOTIA 
-   NT  NORTHWEST TERRITORIES
-   NU  NUNAVUT
-   ON  ONTARIO
-   PE  PRINCE EDWARD ISLAND 
-   QC  QUEBEC  
-   SK  SASKATCHEWAN
+    <t>NCHS Instruction Manual: Part 8_x000D_
+   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY_x000D_
+   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA                                                                                       For U.S. Territories:_x000D_
+   MP  NORTHERN MARIANAS_x000D_
+   AS  AMERICAN SAMOA_x000D_
+   GU  GUAM_x000D_
+   VI   VIRGIN ISLANDS_x000D_
+   PR  PUERTO RICO_x000D_
+For Canadian Provinces:_x000D_
+   AB  ALBERTA  _x000D_
+   BC  BRITISH COLUMBIA _x000D_
+   MB  MANITOBA _x000D_
+   NB  NEW BRUNSWICK  _x000D_
+   NL NEWFOUNDLAND AND LABRADOR_x000D_
+   NS  NOVA SCOTIA _x000D_
+   NT  NORTHWEST TERRITORIES_x000D_
+   NU  NUNAVUT_x000D_
+   ON  ONTARIO_x000D_
+   PE  PRINCE EDWARD ISLAND _x000D_
+   QC  QUEBEC  _x000D_
+   SK  SASKATCHEWAN_x000D_
    YT  YUKON</t>
   </si>
   <si>
@@ -2775,27 +2776,27 @@
     <t>CERTSTATECD</t>
   </si>
   <si>
-    <t>NCHS Instruction Manual: Part 8
-   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY
-   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA                                                                                   For U.S. Territories:
-   MP  NORTHERN MARIANAS
-   AS  AMERICAN SAMOA
-   GU  GUAM
-   VI   VIRGIN ISLANDS
-   PR  PUERTO RICO
-For Canadian Provinces:
-   AB  ALBERTA  
-   BC  BRITISH COLUMBIA 
-   MB  MANITOBA 
-   NB  NEW BRUNSWICK  
-   NL NEWFOUNDLAND AND LABRADOR
-   NS  NOVA SCOTIA 
-   NT  NORTHWEST TERRITORIES
-   NU  NUNAVUT
-   ON  ONTARIO
-   PE  PRINCE EDWARD ISLAND 
-   QC  QUEBEC  
-   SK  SASKATCHEWAN
+    <t>NCHS Instruction Manual: Part 8_x000D_
+   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY_x000D_
+   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA                                                                                   For U.S. Territories:_x000D_
+   MP  NORTHERN MARIANAS_x000D_
+   AS  AMERICAN SAMOA_x000D_
+   GU  GUAM_x000D_
+   VI   VIRGIN ISLANDS_x000D_
+   PR  PUERTO RICO_x000D_
+For Canadian Provinces:_x000D_
+   AB  ALBERTA  _x000D_
+   BC  BRITISH COLUMBIA _x000D_
+   MB  MANITOBA _x000D_
+   NB  NEW BRUNSWICK  _x000D_
+   NL NEWFOUNDLAND AND LABRADOR_x000D_
+   NS  NOVA SCOTIA _x000D_
+   NT  NORTHWEST TERRITORIES_x000D_
+   NU  NUNAVUT_x000D_
+   ON  ONTARIO_x000D_
+   PE  PRINCE EDWARD ISLAND _x000D_
+   QC  QUEBEC  _x000D_
+   SK  SASKATCHEWAN_x000D_
    YT  YUKON</t>
   </si>
   <si>
@@ -2925,7 +2926,7 @@
     <t>MARITAL_DESCRIP</t>
   </si>
   <si>
-    <t>Free text for use of jurisdictions with domestic partnerships, other
+    <t>Free text for use of jurisdictions with domestic partnerships, other_x000D_
 types of relationships.</t>
   </si>
   <si>
@@ -3160,27 +3161,27 @@
     <t>BundleDocumentCodedCauseOfFetalDeath</t>
   </si>
   <si>
-    <t>NCHS Instruction Manual: Part 8
-   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY
-   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA                                                        For US Territories:
-   MP  NORTHERN MARIANAS
-   AS  AMERICAN SAMOA
-   GU  GUAM
-   VI   VIRGIN ISLANDS
-   PR  PUERTO RICO
-For Canadian Provinces:
-   AB  ALBERTA  
-   BC  BRITISH COLUMBIA 
-   MB  MANITOBA 
-   NB  NEW BRUNSWICK  
-   NL NEWFOUNDLAND AND LABRADOR  
-   NS  NOVA SCOTIA 
-   NT  NORTHWEST TERRITORIES
-   NU  NUNAVUT
-   ON  ONTARIO
-   PE  PRINCE EDWARD ISLAND 
-   QC  QUEBEC  
-   SK  SASKATCHEWAN
+    <t>NCHS Instruction Manual: Part 8_x000D_
+   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY_x000D_
+   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA                                                        For US Territories:_x000D_
+   MP  NORTHERN MARIANAS_x000D_
+   AS  AMERICAN SAMOA_x000D_
+   GU  GUAM_x000D_
+   VI   VIRGIN ISLANDS_x000D_
+   PR  PUERTO RICO_x000D_
+For Canadian Provinces:_x000D_
+   AB  ALBERTA  _x000D_
+   BC  BRITISH COLUMBIA _x000D_
+   MB  MANITOBA _x000D_
+   NB  NEW BRUNSWICK  _x000D_
+   NL NEWFOUNDLAND AND LABRADOR  _x000D_
+   NS  NOVA SCOTIA _x000D_
+   NT  NORTHWEST TERRITORIES_x000D_
+   NU  NUNAVUT_x000D_
+   ON  ONTARIO_x000D_
+   PE  PRINCE EDWARD ISLAND _x000D_
+   QC  QUEBEC  _x000D_
+   SK  SASKATCHEWAN_x000D_
    YT  YUKON</t>
   </si>
   <si>
@@ -3196,26 +3197,26 @@
     <t>State, U.S. Territory or Canadian Province of Death - literal</t>
   </si>
   <si>
-    <t>NCHS Instruction Manual: Part 8
-For U.S. Territories:
-   MP  NORTHERN MARIANAS
-   AS  AMERICAN SAMOA
-   GU  GUAM
-   VI   VIRGIN ISLANDS
-   PR  PUERTO RICO
-For Canadian Provinces:
-   AB  ALBERTA  
-   BC  BRITISH COLUMBIA 
-   MB  MANITOBA 
-   NB  NEW BRUNSWICK  
-   NL NEWFOUNDLAND AND LABRADOR  
-   NS  NOVA SCOTIA 
-   NT  NORTHWEST TERRITORIES
-   NU  NUNAVUT
-   ON  ONTARIO
-   PE  PRINCE EDWARD ISLAND 
-   QC  QUEBEC  
-   SK  SASKATCHEWAN
+    <t>NCHS Instruction Manual: Part 8_x000D_
+For U.S. Territories:_x000D_
+   MP  NORTHERN MARIANAS_x000D_
+   AS  AMERICAN SAMOA_x000D_
+   GU  GUAM_x000D_
+   VI   VIRGIN ISLANDS_x000D_
+   PR  PUERTO RICO_x000D_
+For Canadian Provinces:_x000D_
+   AB  ALBERTA  _x000D_
+   BC  BRITISH COLUMBIA _x000D_
+   MB  MANITOBA _x000D_
+   NB  NEW BRUNSWICK  _x000D_
+   NL NEWFOUNDLAND AND LABRADOR  _x000D_
+   NS  NOVA SCOTIA _x000D_
+   NT  NORTHWEST TERRITORIES_x000D_
+   NU  NUNAVUT_x000D_
+   ON  ONTARIO_x000D_
+   PE  PRINCE EDWARD ISLAND _x000D_
+   QC  QUEBEC  _x000D_
+   SK  SASKATCHEWAN_x000D_
    YT  YUKON</t>
   </si>
   <si>
@@ -3279,28 +3280,28 @@
     <t>State, U.S. Territory or Canadian Province of Decedent's Residence - code</t>
   </si>
   <si>
-    <t>NCHS Instruction Manual: Part 8
-   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY
-   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA 
-For US Territories:
-   MP  NORTHERN MARIANAS
-   AS  AMERICAN SAMOA
-   GU  GUAM
-   VI   VIRGIN ISLANDS
-   PR  PUERTO RICO
-For Canadian Provinces:
-   AB  ALBERTA  
-   BC  BRITISH COLUMBIA 
-   MB  MANITOBA 
-   NB  NEW BRUNSWICK  
-   NL NEWFOUNDLAND AND LABRADOR 
-   NS  NOVA SCOTIA 
-   NT  NORTHWEST TERRITORIES
-   NU  NUNAVUT
-   ON  ONTARIO
-   PE  PRINCE EDWARD ISLAND 
-   QC  QUEBEC  
-   SK  SASKATCHEWAN
+    <t>NCHS Instruction Manual: Part 8_x000D_
+   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY_x000D_
+   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA _x000D_
+For US Territories:_x000D_
+   MP  NORTHERN MARIANAS_x000D_
+   AS  AMERICAN SAMOA_x000D_
+   GU  GUAM_x000D_
+   VI   VIRGIN ISLANDS_x000D_
+   PR  PUERTO RICO_x000D_
+For Canadian Provinces:_x000D_
+   AB  ALBERTA  _x000D_
+   BC  BRITISH COLUMBIA _x000D_
+   MB  MANITOBA _x000D_
+   NB  NEW BRUNSWICK  _x000D_
+   NL NEWFOUNDLAND AND LABRADOR _x000D_
+   NS  NOVA SCOTIA _x000D_
+   NT  NORTHWEST TERRITORIES_x000D_
+   NU  NUNAVUT_x000D_
+   ON  ONTARIO_x000D_
+   PE  PRINCE EDWARD ISLAND _x000D_
+   QC  QUEBEC  _x000D_
+   SK  SASKATCHEWAN_x000D_
    YT  YUKON</t>
   </si>
   <si>
@@ -3547,26 +3548,26 @@
     <t>STATE_T</t>
   </si>
   <si>
-    <t>NCHS Instruction Manual: Part 8
-For US Territories:
-   MP  NORTHERN MARIANAS
-   AS  AMERICAN SAMOA
-   GU  GUAM
-   VI   VIRGIN ISLANDS
-   PR  PUERTO RICO
-For Canadian Provinces:
-   AB  ALBERTA  
-   BC  BRITISH COLUMBIA 
-   MB  MANITOBA 
-   NB  NEW BRUNSWICK  
-   NL  NEWFOUNDLAND AND LABRADOR  
-   NS  NOVA SCOTIA 
-   NT  NORTHWEST TERRITORIES
-   NU  NUNAVUT
-   ON  ONTARIO
-   PE  PRINCE EDWARD ISLAND 
-   QC  QUEBEC  
-   SK  SASKATCHEWAN
+    <t>NCHS Instruction Manual: Part 8_x000D_
+For US Territories:_x000D_
+   MP  NORTHERN MARIANAS_x000D_
+   AS  AMERICAN SAMOA_x000D_
+   GU  GUAM_x000D_
+   VI   VIRGIN ISLANDS_x000D_
+   PR  PUERTO RICO_x000D_
+For Canadian Provinces:_x000D_
+   AB  ALBERTA  _x000D_
+   BC  BRITISH COLUMBIA _x000D_
+   MB  MANITOBA _x000D_
+   NB  NEW BRUNSWICK  _x000D_
+   NL  NEWFOUNDLAND AND LABRADOR  _x000D_
+   NS  NOVA SCOTIA _x000D_
+   NT  NORTHWEST TERRITORIES_x000D_
+   NU  NUNAVUT_x000D_
+   ON  ONTARIO_x000D_
+   PE  PRINCE EDWARD ISLAND _x000D_
+   QC  QUEBEC  _x000D_
+   SK  SASKATCHEWAN_x000D_
    YT  YUKON</t>
   </si>
   <si>
@@ -3579,7 +3580,7 @@
     <t>Void Flag</t>
   </si>
   <si>
-    <t>0 = default; valid record
+    <t>0 = default; valid record_x000D_
 1 = VOID record</t>
   </si>
   <si>
@@ -3637,10 +3638,10 @@
     <t>TPLACE</t>
   </si>
   <si>
-    <t>1 = Hospital
-2 = Clinic
-3 = Doctor's Office
-4 = Other
+    <t>1 = Hospital_x000D_
+2 = Clinic_x000D_
+3 = Doctor's Office_x000D_
+4 = Other_x000D_
 9 = Unknown</t>
   </si>
   <si>
@@ -3668,7 +3669,7 @@
     <t>AGE</t>
   </si>
   <si>
-    <t>10-55
+    <t>10-55_x000D_
 99 = Unknown</t>
   </si>
   <si>
@@ -3681,27 +3682,27 @@
     <t>State, U.S. Territory or Canadian Province of Residence (Patient) - code</t>
   </si>
   <si>
-    <t>NCHS Instruction Manual: Part 8
-   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY
-   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA                     For U.S. Territories:
-   MP  NORTHERN MARIANAS
-   AS  AMERICAN SAMOA
-   GU  GUAM
-   VI   VIRGIN ISLANDS
-   PR  PUERTO RICO
-For Canadian Provinces:
-   AB  ALBERTA  
-   BC  BRITISH COLUMBIA 
-   MB  MANITOBA 
-   NB  NEW BRUNSWICK  
-   NL  NEWFOUNDLAND AND LABRADOR
-   NS  NOVA SCOTIA 
-   NT  NORTHWEST TERRITORIES
-   NU  NUNAVUT
-   ON  ONTARIO
-   PE  PRINCE EDWARD ISLAND 
-   QC  QUEBEC  
-   SK  SASKATCHEWAN
+    <t>NCHS Instruction Manual: Part 8_x000D_
+   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY_x000D_
+   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA                     For U.S. Territories:_x000D_
+   MP  NORTHERN MARIANAS_x000D_
+   AS  AMERICAN SAMOA_x000D_
+   GU  GUAM_x000D_
+   VI   VIRGIN ISLANDS_x000D_
+   PR  PUERTO RICO_x000D_
+For Canadian Provinces:_x000D_
+   AB  ALBERTA  _x000D_
+   BC  BRITISH COLUMBIA _x000D_
+   MB  MANITOBA _x000D_
+   NB  NEW BRUNSWICK  _x000D_
+   NL  NEWFOUNDLAND AND LABRADOR_x000D_
+   NS  NOVA SCOTIA _x000D_
+   NT  NORTHWEST TERRITORIES_x000D_
+   NU  NUNAVUT_x000D_
+   ON  ONTARIO_x000D_
+   PE  PRINCE EDWARD ISLAND _x000D_
+   QC  QUEBEC  _x000D_
+   SK  SASKATCHEWAN_x000D_
    YT  YUKON</t>
   </si>
   <si>
@@ -3771,12 +3772,12 @@
     <t>Patient's Marital Status</t>
   </si>
   <si>
-    <t>1 = Never Married
-2 = Now Married
-3 = Widowed
-4 = Divorced
-5 = Separated
-7 = Other (specify below)
+    <t>1 = Never Married_x000D_
+2 = Now Married_x000D_
+3 = Widowed_x000D_
+4 = Divorced_x000D_
+5 = Separated_x000D_
+7 = Other (specify below)_x000D_
 9 = Unknown or Not Stated</t>
   </si>
   <si>
@@ -3831,13 +3832,13 @@
     <t>ETHNIC_OLD</t>
   </si>
   <si>
-    <t>from single choice versus mark all
-0 = non-hispanic
-1 = Mexican
-2 = Puerto Rican
-3 = Cuban
-4 = Central of South American
-5 = Other or unknown hispanic
+    <t>from single choice versus mark all_x000D_
+0 = non-hispanic_x000D_
+1 = Mexican_x000D_
+2 = Puerto Rican_x000D_
+3 = Cuban_x000D_
+4 = Central of South American_x000D_
+5 = Other or unknown hispanic_x000D_
 9 = Not classifiable</t>
   </si>
   <si>
@@ -3847,15 +3848,15 @@
     <t>ETHNIC_OTH</t>
   </si>
   <si>
-    <t>Comma delimit multiple entries; 
+    <t>Comma delimit multiple entries; _x000D_
 Some states keep a version of multiple Hispanic origin that is not in the new format but something in between.</t>
   </si>
   <si>
     <t>Patient's Race--White</t>
   </si>
   <si>
-    <t>Y = Yes, box for race checked
-N = No, box for race not checked
+    <t>Y = Yes, box for race checked_x000D_
+N = No, box for race not checked_x000D_
 U = Unknown race (U in all race fields)</t>
   </si>
   <si>
@@ -3934,14 +3935,14 @@
     <t>RACE_OLD</t>
   </si>
   <si>
-    <t>From single choice versus mark all
-1 = white; 2 =  Black;
-3 = American Indian; 4 = Chinese
-5 = Japanese; 6 = Hawaiian;
-7 = Filipino; 8 = Other Asian/ Pac Islander;
-9 = not reported; A = Asian Indian; 
-B = Korean; C = Samoan;
-D = Vietnamese; E = Guamian;
+    <t>From single choice versus mark all_x000D_
+1 = white; 2 =  Black;_x000D_
+3 = American Indian; 4 = Chinese_x000D_
+5 = Japanese; 6 = Hawaiian;_x000D_
+7 = Filipino; 8 = Other Asian/ Pac Islander;_x000D_
+9 = not reported; A = Asian Indian; _x000D_
+B = Korean; C = Samoan;_x000D_
+D = Vietnamese; E = Guamian;_x000D_
 F = Multi-racial</t>
   </si>
   <si>
@@ -3951,7 +3952,7 @@
     <t>RACE_OTH</t>
   </si>
   <si>
-    <t xml:space="preserve">Comma delimit multiple entries;
+    <t xml:space="preserve">Comma delimit multiple entries;_x000D_
 Some states keep a version of multiple race that is not in the new format but something in between. </t>
   </si>
   <si>
@@ -3961,7 +3962,7 @@
     <t>PREV_PREG</t>
   </si>
   <si>
-    <t>00-30
+    <t>00-30_x000D_
 99 = Unknown</t>
   </si>
   <si>
@@ -3971,14 +3972,14 @@
     <t>PLBT</t>
   </si>
   <si>
-    <t>Previous live births,
+    <t>Previous live births,_x000D_
 Now living</t>
   </si>
   <si>
     <t>PLBL</t>
   </si>
   <si>
-    <t>Previous live births,
+    <t>Previous live births,_x000D_
 Now dead</t>
   </si>
   <si>
@@ -4009,7 +4010,7 @@
     <t>DLMP_MO</t>
   </si>
   <si>
-    <t>00-12
+    <t>00-12_x000D_
 99 = Unknown</t>
   </si>
   <si>
@@ -4019,7 +4020,7 @@
     <t>DLMP_DY</t>
   </si>
   <si>
-    <t>01-31 (based on month)
+    <t>01-31 (based on month)_x000D_
 99 = Unknown</t>
   </si>
   <si>
@@ -4029,7 +4030,7 @@
     <t>CWGEST</t>
   </si>
   <si>
-    <t>01-27
+    <t>01-27_x000D_
 99 = Unknown</t>
   </si>
   <si>
@@ -4099,18 +4100,18 @@
     <t>PROC_T</t>
   </si>
   <si>
-    <t>1 = Suction Curettage
-2 = Medical (Non-surgical; medication induced -- specify medication(s) in field below)
-3 = Dilation &amp; Evacuation (D&amp;E)
-4 = Intra-Uterine Instillation (Saline or Prostaglandin)
-5 = Vaginal Prostaglandin
-6 = Sharp Curettage (D&amp;C)
-7 = Hysterotomy/Hysterectomy
-8 = Other
+    <t>1 = Suction Curettage_x000D_
+2 = Medical (Non-surgical; medication induced -- specify medication(s) in field below)_x000D_
+3 = Dilation &amp; Evacuation (D&amp;E)_x000D_
+4 = Intra-Uterine Instillation (Saline or Prostaglandin)_x000D_
+5 = Vaginal Prostaglandin_x000D_
+6 = Sharp Curettage (D&amp;C)_x000D_
+7 = Hysterotomy/Hysterectomy_x000D_
+8 = Other_x000D_
 9 = Unknown</t>
   </si>
   <si>
-    <t xml:space="preserve">Medical (non-surgical) procedure medication(s) literal 
+    <t xml:space="preserve">Medical (non-surgical) procedure medication(s) literal _x000D_
 </t>
   </si>
   <si>
@@ -4120,7 +4121,7 @@
     <t>Free form literal specifing medication(s) that terminated this pregnancy.</t>
   </si>
   <si>
-    <t xml:space="preserve">Termination other procedure literal 
+    <t xml:space="preserve">Termination other procedure literal _x000D_
 </t>
   </si>
   <si>
@@ -4136,15 +4137,15 @@
     <t>PROC-OTH</t>
   </si>
   <si>
-    <t xml:space="preserve">Repeat up to 4 single digit codes                            
-0 = None                                                                                                                                                                                                                           1 = Suction Curettage
-2 = Medical (Non-surgical; medication induced)
-3 = Dilation &amp; Evacuation (D&amp;E)
-4 = Intra-Uterine Instillation (Saline or Prostaglandin)
-5 = Vaginal Prostaglandin
-6 = Sharp Curettage (D&amp;C)
-8 = Other
-9 = Unknown
+    <t xml:space="preserve">Repeat up to 4 single digit codes                            _x000D_
+0 = None                                                                                                                                                                                                                           1 = Suction Curettage_x000D_
+2 = Medical (Non-surgical; medication induced)_x000D_
+3 = Dilation &amp; Evacuation (D&amp;E)_x000D_
+4 = Intra-Uterine Instillation (Saline or Prostaglandin)_x000D_
+5 = Vaginal Prostaglandin_x000D_
+6 = Sharp Curettage (D&amp;C)_x000D_
+8 = Other_x000D_
+9 = Unknown_x000D_
 </t>
   </si>
   <si>
@@ -4154,7 +4155,7 @@
     <t>CALC_WGEST</t>
   </si>
   <si>
-    <t>00-95
+    <t>00-95_x000D_
 99 = Unknown</t>
   </si>
   <si>
@@ -4167,7 +4168,7 @@
     <t>Y, N, or U (if N or U, leave all other TP complications blank)</t>
   </si>
   <si>
-    <t>Hemorrhage
+    <t>Hemorrhage_x000D_
 (at time of procedure)</t>
   </si>
   <si>
@@ -4177,56 +4178,56 @@
     <t>Y, N, U (some jurisdictions may only collect hemorage data if above a certain volumn)</t>
   </si>
   <si>
-    <t>Infection
+    <t>Infection_x000D_
 (at time of procedure)</t>
   </si>
   <si>
     <t>INFECT_TP</t>
   </si>
   <si>
-    <t>Uterine perforation
+    <t>Uterine perforation_x000D_
 (at time of procedure)</t>
   </si>
   <si>
     <t>PERF_TP</t>
   </si>
   <si>
-    <t>Cervical laceration
+    <t>Cervical laceration_x000D_
 (at time of procedure)</t>
   </si>
   <si>
     <t>LACER_TP</t>
   </si>
   <si>
-    <t>Retained products
+    <t>Retained products_x000D_
 (at time of procedure)</t>
   </si>
   <si>
     <t>RETAN_TP</t>
   </si>
   <si>
-    <t>Death 
+    <t>Death _x000D_
 (at time of procedure)</t>
   </si>
   <si>
     <t>DEATH_TP</t>
   </si>
   <si>
-    <t>Failure of first method 
+    <t>Failure of first method _x000D_
 (at time of procedure)</t>
   </si>
   <si>
     <t>FAIL_TP</t>
   </si>
   <si>
-    <t>Other complications 
+    <t>Other complications _x000D_
 (at time of procedure)</t>
   </si>
   <si>
     <t>OTHER_TP</t>
   </si>
   <si>
-    <t>Other complications literal 
+    <t>Other complications literal _x000D_
 (at time of procedure)</t>
   </si>
   <si>
@@ -4245,49 +4246,49 @@
     <t>Y, N, or U (if N or U, leave all other F1 complications blank)</t>
   </si>
   <si>
-    <t>Complications at followup
+    <t>Complications at followup_x000D_
 at same facility</t>
   </si>
   <si>
     <t>COMP_F1</t>
   </si>
   <si>
-    <t>Hemorrhage
+    <t>Hemorrhage_x000D_
 (at time of followup at this facility)</t>
   </si>
   <si>
     <t>HEMOR_F1</t>
   </si>
   <si>
-    <t>Infection 
+    <t>Infection _x000D_
 (at time of  follow up at this facility)</t>
   </si>
   <si>
     <t>INFECT_F1</t>
   </si>
   <si>
-    <t>Uterine perforation 
+    <t>Uterine perforation _x000D_
 (at time of followup at this facility)</t>
   </si>
   <si>
     <t>PERF_F1</t>
   </si>
   <si>
-    <t>Cervical laceration 
+    <t>Cervical laceration _x000D_
 (at time of followup at this facility)</t>
   </si>
   <si>
     <t>LACER_F1</t>
   </si>
   <si>
-    <t>Retained products 
+    <t>Retained products _x000D_
 (at time of followup at this facility)</t>
   </si>
   <si>
     <t>RETAN_F1</t>
   </si>
   <si>
-    <t>Death 
+    <t>Death _x000D_
 (at time of followup at this facility)</t>
   </si>
   <si>
@@ -4306,7 +4307,7 @@
     <t>OTHER_F1</t>
   </si>
   <si>
-    <t>Other complications literal 
+    <t>Other complications literal _x000D_
 (at time of followup at this facility)</t>
   </si>
   <si>
@@ -4325,70 +4326,70 @@
     <t>Y, N, or U (if N or U, leave all other F2 complications blank)</t>
   </si>
   <si>
-    <t>Complications 
+    <t>Complications _x000D_
 (at time of followup at other facility)</t>
   </si>
   <si>
     <t>COMP_F2</t>
   </si>
   <si>
-    <t>Hemorrhage
+    <t>Hemorrhage_x000D_
 (at time of followup at other facility)</t>
   </si>
   <si>
     <t>HEMOR_F2</t>
   </si>
   <si>
-    <t>Infection 
+    <t>Infection _x000D_
 (at time of followup at other facility)</t>
   </si>
   <si>
     <t>INFECT_F2</t>
   </si>
   <si>
-    <t>Uterine perforation  
+    <t>Uterine perforation  _x000D_
 (at time of followup at other facility)</t>
   </si>
   <si>
     <t>PERF_F2</t>
   </si>
   <si>
-    <t>Cervical laceration  
+    <t>Cervical laceration  _x000D_
 (at time of followup at other facility)</t>
   </si>
   <si>
     <t>LACER_F2</t>
   </si>
   <si>
-    <t>Retained products 
+    <t>Retained products _x000D_
 (at time of followup at other facility)</t>
   </si>
   <si>
     <t>RETAN_F2</t>
   </si>
   <si>
-    <t>Death 
+    <t>Death _x000D_
 (at time of followup at other facility)</t>
   </si>
   <si>
     <t>DEATH_F2</t>
   </si>
   <si>
-    <t>Failure of first method 
+    <t>Failure of first method _x000D_
 (at time of followup at other facility)</t>
   </si>
   <si>
     <t>FAIL_F2</t>
   </si>
   <si>
-    <t xml:space="preserve">Other complications 
+    <t xml:space="preserve">Other complications _x000D_
 (at time of followup at other facility) </t>
   </si>
   <si>
     <t>OTHER_F2</t>
   </si>
   <si>
-    <t>Other complications literal 
+    <t>Other complications literal _x000D_
 (at time of followup at other facility)</t>
   </si>
   <si>
@@ -4398,17 +4399,17 @@
     <t>Free form literal of specified other complication at time of followup at other facility.</t>
   </si>
   <si>
-    <t>Site of follow-up visit 
+    <t>Site of follow-up visit _x000D_
 (at other facility)</t>
   </si>
   <si>
     <t>SITE_F2</t>
   </si>
   <si>
-    <t>1 = physician's office
-2 = clinic
-3 = hospital
-4 = other, specify
+    <t>1 = physician's office_x000D_
+2 = clinic_x000D_
+3 = hospital_x000D_
+4 = other, specify_x000D_
 9 = unknown</t>
   </si>
   <si>
@@ -4688,8 +4689,8 @@
     <t>FSEX</t>
   </si>
   <si>
-    <t xml:space="preserve">M = Male
-F = Female
+    <t xml:space="preserve">M = Male_x000D_
+F = Female_x000D_
 U = Unknown </t>
   </si>
   <si>
@@ -4726,13 +4727,13 @@
     <t>Place Where Delivery Occurred</t>
   </si>
   <si>
-    <t>1 = Hospital
-2 = Freestanding Birth Center
-3 = Home (Intended)
-4 = Home (Not Intended)
-5 = Home (Unknown if Intended)
-6 = Clinic/Doctor's Office
-7 = Other
+    <t>1 = Hospital_x000D_
+2 = Freestanding Birth Center_x000D_
+3 = Home (Intended)_x000D_
+4 = Home (Not Intended)_x000D_
+5 = Home (Unknown if Intended)_x000D_
+6 = Clinic/Doctor's Office_x000D_
+7 = Other_x000D_
 9 = Unknown</t>
   </si>
   <si>
@@ -4790,7 +4791,7 @@
     <t>MAGE_BYPASS</t>
   </si>
   <si>
-    <t xml:space="preserve">0 = Edit Passed
+    <t xml:space="preserve">0 = Edit Passed_x000D_
 1 = Data Queried </t>
   </si>
   <si>
@@ -4809,27 +4810,27 @@
     <t>BPLACEC_ST_TER</t>
   </si>
   <si>
-    <t>NCHS Instruction Manual: Part 8
-   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY
-   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA                                                                   For U.S. Territories:
-   MP  NORTHERN MARIANAS
-   AS  AMERICAN SAMOA
-   GU  GUAM
-   VI   VIRGIN ISLANDS
-   PR  PUERTO RICO
-For Canadian Provinces:
-   AB  ALBERTA  
-   BC  BRITISH COLUMBIA 
-   MB  MANITOBA 
-   NB  NEW BRUNSWICK  
-   NL  NEWFOUNDLAND AND LABRADOR  
-   NS  NOVA SCOTIA 
-   NT  NORTHWEST TERRITORIES
-   NU  NUNAVUT
-   ON  ONTARIO
-   PE  PRINCE EDWARD ISLAND 
-   QC  QUEBEC  
-   SK  SASKATCHEWAN
+    <t>NCHS Instruction Manual: Part 8_x000D_
+   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY_x000D_
+   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA                                                                   For U.S. Territories:_x000D_
+   MP  NORTHERN MARIANAS_x000D_
+   AS  AMERICAN SAMOA_x000D_
+   GU  GUAM_x000D_
+   VI   VIRGIN ISLANDS_x000D_
+   PR  PUERTO RICO_x000D_
+For Canadian Provinces:_x000D_
+   AB  ALBERTA  _x000D_
+   BC  BRITISH COLUMBIA _x000D_
+   MB  MANITOBA _x000D_
+   NB  NEW BRUNSWICK  _x000D_
+   NL  NEWFOUNDLAND AND LABRADOR  _x000D_
+   NS  NOVA SCOTIA _x000D_
+   NT  NORTHWEST TERRITORIES_x000D_
+   NU  NUNAVUT_x000D_
+   ON  ONTARIO_x000D_
+   PE  PRINCE EDWARD ISLAND _x000D_
+   QC  QUEBEC  _x000D_
+   SK  SASKATCHEWAN_x000D_
    YT  YUKON</t>
   </si>
   <si>
@@ -4854,27 +4855,27 @@
     <t>State, U.S. Territory or Canadian Province of Residence (Mother) - code</t>
   </si>
   <si>
-    <t>NCHS Instruction Manual: Part 8
-   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY
-   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA                                                                   For U.S. Territories:
-   MP  NORTHERN MARIANAS
-   AS  AMERICAN SAMOA
-   GU  GUAM
-   VI   VIRGIN ISLANDS
-   PR  PUERTO RICO
-For Canadian Provinces:
-   AB  ALBERTA  
-   BC  BRITISH COLUMBIA 
-   MB  MANITOBA 
-   NB  NEW BRUNSWICK  
-   NL  NEWFOUNDLAND AND LABRADOR
-   NS  NOVA SCOTIA 
-   NT  NORTHWEST TERRITORIES
-   NU  NUNAVUT
-   ON  ONTARIO
-   PE  PRINCE EDWARD ISLAND 
-   QC  QUEBEC  
-   SK  SASKATCHEWAN
+    <t>NCHS Instruction Manual: Part 8_x000D_
+   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY_x000D_
+   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA                                                                   For U.S. Territories:_x000D_
+   MP  NORTHERN MARIANAS_x000D_
+   AS  AMERICAN SAMOA_x000D_
+   GU  GUAM_x000D_
+   VI   VIRGIN ISLANDS_x000D_
+   PR  PUERTO RICO_x000D_
+For Canadian Provinces:_x000D_
+   AB  ALBERTA  _x000D_
+   BC  BRITISH COLUMBIA _x000D_
+   MB  MANITOBA _x000D_
+   NB  NEW BRUNSWICK  _x000D_
+   NL  NEWFOUNDLAND AND LABRADOR_x000D_
+   NS  NOVA SCOTIA _x000D_
+   NT  NORTHWEST TERRITORIES_x000D_
+   NU  NUNAVUT_x000D_
+   ON  ONTARIO_x000D_
+   PE  PRINCE EDWARD ISLAND _x000D_
+   QC  QUEBEC  _x000D_
+   SK  SASKATCHEWAN_x000D_
    YT  YUKON</t>
   </si>
   <si>
@@ -4884,8 +4885,8 @@
     <t>Residence of Mother--Inside City/Town Limits</t>
   </si>
   <si>
-    <t>Y = Yes
-N = No
+    <t>Y = Yes_x000D_
+N = No_x000D_
 U = Unknown</t>
   </si>
   <si>
@@ -4952,8 +4953,8 @@
     <t>MEDUC_BYPASS</t>
   </si>
   <si>
-    <t>0 = Edit Passed
-1 = Edit Failed, Data Queried and Verified
+    <t>0 = Edit Passed_x000D_
+1 = Edit Failed, Data Queried and Verified_x000D_
 2 = Edit Failed, Data Queried, but not Verified</t>
   </si>
   <si>
@@ -5374,11 +5375,11 @@
     <t>ATTEND</t>
   </si>
   <si>
-    <t>1 = MD
-2 = DO
-3 = CNM/CM
-4 = Other midwife
-5 = Other (specify)
+    <t>1 = MD_x000D_
+2 = DO_x000D_
+3 = CNM/CM_x000D_
+4 = Other midwife_x000D_
+5 = Other (specify)_x000D_
 9 = Unknown</t>
   </si>
   <si>
@@ -5430,7 +5431,7 @@
     <t>DOFP_YR</t>
   </si>
   <si>
-    <t>4 digit year; year of delivery or
+    <t>4 digit year; year of delivery or_x000D_
 (year of delivery - 1), 8888, 9999</t>
   </si>
   <si>
@@ -5467,8 +5468,8 @@
     <t>NPREV_BYPASS</t>
   </si>
   <si>
-    <t>0 = Edit Passed
-1 = Edit Failed, Number Verified
+    <t>0 = Edit Passed_x000D_
+1 = Edit Failed, Number Verified_x000D_
 2 = Edit Failed, Number not Verified</t>
   </si>
   <si>
@@ -5502,8 +5503,8 @@
     <t>HGT_BYPASS</t>
   </si>
   <si>
-    <t>0 = Edit Passed
-1 = Edit Failed, Number Verified
+    <t>0 = Edit Passed_x000D_
+1 = Edit Failed, Number Verified_x000D_
 2 = Edit Failed, Number not  Verified</t>
   </si>
   <si>
@@ -5531,8 +5532,8 @@
     <t>PWGT_BYPASS</t>
   </si>
   <si>
-    <t>0 = Edit Passed
-1 = Edit Failed, Verified
+    <t>0 = Edit Passed_x000D_
+1 = Edit Failed, Verified_x000D_
 2 = Edit Failed, not Verified</t>
   </si>
   <si>
@@ -5599,8 +5600,8 @@
     <t>YLLB</t>
   </si>
   <si>
-    <t>4 digit year;
-(year of mother's birth + 10) through
+    <t>4 digit year;_x000D_
+(year of mother's birth + 10) through_x000D_
 year of delivery, 8888, 9999</t>
   </si>
   <si>
@@ -5658,8 +5659,8 @@
     <t>Date Last Normal Menses Began--Year</t>
   </si>
   <si>
-    <t>4 digit year; year of delivery or
-(year of delivery - 1) or
+    <t>4 digit year; year of delivery or_x000D_
+(year of delivery - 1) or_x000D_
 (year of delivery - 2), 9999</t>
   </si>
   <si>
@@ -5684,9 +5685,9 @@
     <t>See [note on missing pregnancy risk factors data]</t>
   </si>
   <si>
-    <t>Update risk factors (old Observation-pregnancy-risk-factor)
-STU 1 listed:
-IJE Natality Data Elements: PDIAB, GDIAB, PHYPE, GHYPE, PPB, INFT, PCES, EHYPE, INFT_DRG, INFT_ART
+    <t>Update risk factors (old Observation-pregnancy-risk-factor)_x000D_
+STU 1 listed:_x000D_
+IJE Natality Data Elements: PDIAB, GDIAB, PHYPE, GHYPE, PPB, INFT, PCES, EHYPE, INFT_DRG, INFT_ART_x000D_
 IJE Fetal Death Data Elements: PDIAB, GDIAB, PHYPE, GHYPE, PPB, INFT, PCES, EHYPE, INFT_DRG, INFT_ART</t>
   </si>
   <si>
@@ -5777,7 +5778,7 @@
     <t>NPCES_BYPASS</t>
   </si>
   <si>
-    <t>0 = Edit Passed
+    <t>0 = Edit Passed_x000D_
 1 = Edit Failed, Verified</t>
   </si>
   <si>
@@ -5865,9 +5866,9 @@
     <t>PRES</t>
   </si>
   <si>
-    <t>1 = Cephalic
-2 = Breech
-3 = Other
+    <t>1 = Cephalic_x000D_
+2 = Breech_x000D_
+3 = Other_x000D_
 9 = Unknown</t>
   </si>
   <si>
@@ -5883,10 +5884,10 @@
     <t>ROUT</t>
   </si>
   <si>
-    <t>1 = Spontaneous
-2 = Forceps
-3 = Vacuum
-4 = Cesarean
+    <t>1 = Spontaneous_x000D_
+2 = Forceps_x000D_
+3 = Vacuum_x000D_
+4 = Cesarean_x000D_
 9 = Unknown</t>
   </si>
   <si>
@@ -5896,7 +5897,7 @@
     <t>code</t>
   </si>
   <si>
-    <t>See  [note on missing method of delivery data]</t>
+    <t>[DeliveryRoutesVS] unless unknown, &lt;br /&gt;See  [note on missing method of delivery data]</t>
   </si>
   <si>
     <t>Method of Delivery--Trial of Labor Attempted</t>
@@ -5905,9 +5906,9 @@
     <t>TLAB</t>
   </si>
   <si>
-    <t>Y = Yes
-N = No
-U = Unknown
+    <t>Y = Yes_x000D_
+N = No_x000D_
+U = Unknown_x000D_
 X = Not Applicable</t>
   </si>
   <si>
@@ -5926,9 +5927,9 @@
     <t>MTR</t>
   </si>
   <si>
-    <t>Update maternal morbidity (old Condition-maternal-morbidity)
-STU 1 listed:
-IJE Natality Data Elements: MTR, PLAC, RUT, UHYS, AINT
+    <t>Update maternal morbidity (old Condition-maternal-morbidity)_x000D_
+STU 1 listed:_x000D_
+IJE Natality Data Elements: MTR, PLAC, RUT, UHYS, AINT_x000D_
 IJE Fetal Death Data Elements: RUT, AINT</t>
   </si>
   <si>
@@ -5977,10 +5978,10 @@
     <t>UOPR</t>
   </si>
   <si>
-    <t>Update maternal morbidity (old Condition-maternal-morbidity)
-STU 1 listed:
-IJE Natality Data Elements: MTR, PLAC, RUT, UHYS, AINT
-IJE Fetal Death Data Elements: RUT, AINT
+    <t>Update maternal morbidity (old Condition-maternal-morbidity)_x000D_
+STU 1 listed:_x000D_
+IJE Natality Data Elements: MTR, PLAC, RUT, UHYS, AINT_x000D_
+IJE Fetal Death Data Elements: RUT, AINT_x000D_
 (new) UOPR</t>
   </si>
   <si>
@@ -5999,8 +6000,8 @@
     <t>FW_BYPASS</t>
   </si>
   <si>
-    <t>0 = Off
-1 = Queried data correct, out of range
+    <t>0 = Off_x000D_
+1 = Queried data correct, out of range_x000D_
 2 = Queried, failed  delivery weight/gestation edit</t>
   </si>
   <si>
@@ -6025,7 +6026,7 @@
     <t>OWGEST_BYPASS</t>
   </si>
   <si>
-    <t>0 = Off
+    <t>0 = Off_x000D_
 1 = Queried data correct, out of range</t>
   </si>
   <si>
@@ -6038,9 +6039,9 @@
     <t>ETIME</t>
   </si>
   <si>
-    <t>N = At assessment, no labor
-L = At assessment, labor
-A = Labor, no assessment
+    <t>N = At assessment, no labor_x000D_
+L = At assessment, labor_x000D_
+A = Labor, no assessment_x000D_
 U = Unknown</t>
   </si>
   <si>
@@ -6053,8 +6054,8 @@
     <t>Was an Autopsy Performed?</t>
   </si>
   <si>
-    <t>Y = Yes
-N = No
+    <t>Y = Yes_x000D_
+N = No_x000D_
 P = Planned</t>
   </si>
   <si>
@@ -6076,8 +6077,8 @@
     <t>Were Autopsy or Histological Placental Examination Results Used in Determining the Cause of Fetal Death?</t>
   </si>
   <si>
-    <t>Y = Yes
-N = No
+    <t>Y = Yes_x000D_
+N = No_x000D_
 X = Not Applicable</t>
   </si>
   <si>
@@ -6126,8 +6127,8 @@
     <t>PLUR_BYPASS</t>
   </si>
   <si>
-    <t>0 = Off
-1 = Queried, and Correct
+    <t>0 = Off_x000D_
+1 = Queried, and Correct_x000D_
 2 = Plurality/Set Order Queried, Inconsistent</t>
   </si>
   <si>
@@ -6197,9 +6198,9 @@
     <t>DOWT</t>
   </si>
   <si>
-    <t>C = Confirmed
-P = Pending
-N = No
+    <t>C = Confirmed_x000D_
+P = Pending_x000D_
+N = No_x000D_
 U = Unknown</t>
   </si>
   <si>
@@ -6221,10 +6222,10 @@
     <t>&gt;=year of delivery</t>
   </si>
   <si>
-    <t>Code used on 3 tabs: N, FD, &amp; BID
-Code structure description differs here
-Code sent back to state VRO
-For R_YR, R_MO, R_DY, VRDR uses CodingStatusValues  parameter[receiptDate].value   date    See [PartialDatesAndTimes]
+    <t>Code used on 3 tabs: N, FD, &amp; BID_x000D_
+Code structure description differs here_x000D_
+Code sent back to state VRO_x000D_
+For R_YR, R_MO, R_DY, VRDR uses CodingStatusValues  parameter[receiptDate].value   date    See [PartialDatesAndTimes]_x000D_
 Decision: Mimic VRDR</t>
   </si>
   <si>
@@ -6240,10 +6241,10 @@
     <t>NCHS USE ONLY: Receipt date -- Day</t>
   </si>
   <si>
-    <t>Code used on 3 tabs: N, FD, &amp; BID
-Code structure description differs here
-Code sent back to state VRO
-Note: Marked as NCHS USE ONLY, but VRDR does address this. For R_YR, R_MO, R_DY, VRDR uses CodingStatusValues  parameter[receiptDate].value   date    See [PartialDatesAndTimes]
+    <t>Code used on 3 tabs: N, FD, &amp; BID_x000D_
+Code structure description differs here_x000D_
+Code sent back to state VRO_x000D_
+Note: Marked as NCHS USE ONLY, but VRDR does address this. For R_YR, R_MO, R_DY, VRDR uses CodingStatusValues  parameter[receiptDate].value   date    See [PartialDatesAndTimes]_x000D_
 Decision: Mimic VRDR</t>
   </si>
   <si>
@@ -6286,9 +6287,9 @@
     <t>INFT_DRG</t>
   </si>
   <si>
-    <t>Y = Yes (BLANK IF NOT ADDED)
-N = No
-X = Not Applicable
+    <t>Y = Yes (BLANK IF NOT ADDED)_x000D_
+N = No_x000D_
+X = Not Applicable_x000D_
 U = Unknown</t>
   </si>
   <si>
@@ -6325,7 +6326,7 @@
     <t>COD18a1</t>
   </si>
   <si>
-    <t>Y = Yes
+    <t>Y = Yes_x000D_
 N = No</t>
   </si>
   <si>
@@ -7013,9 +7014,9 @@
     <t>string(25)</t>
   </si>
   <si>
-    <t>Code used on 3 tabs: N, FD, &amp; BID
-NCHS does not use
-BFDR defines "ObservationPresentJob" profile. 
+    <t>Code used on 3 tabs: N, FD, &amp; BID_x000D_
+NCHS does not use_x000D_
+BFDR defines "ObservationPresentJob" profile. _x000D_
 BFDR and VRDR use different profiles</t>
   </si>
   <si>
@@ -7577,24 +7578,24 @@
     <t>MRACEBG_C</t>
   </si>
   <si>
-    <t>01 = White
-02 = Black
-03 = American Indian/Alaskan Native
-04 = Asian Indian
-05 = Chinese
-06 = Filipino
-07 = Japanese
-08 = Korean
-09 = Vietnamese
-10 = Other Asian
-11 = Native Hawaiian
-12 = Guamanian
-13 = Samoan
-14 = Other Pacific Islander
-15 = Other
-21 = Bridged White
-22 = Bridged Black
-23 = Bridged American Indian/Alaskan Native
+    <t>01 = White_x000D_
+02 = Black_x000D_
+03 = American Indian/Alaskan Native_x000D_
+04 = Asian Indian_x000D_
+05 = Chinese_x000D_
+06 = Filipino_x000D_
+07 = Japanese_x000D_
+08 = Korean_x000D_
+09 = Vietnamese_x000D_
+10 = Other Asian_x000D_
+11 = Native Hawaiian_x000D_
+12 = Guamanian_x000D_
+13 = Samoan_x000D_
+14 = Other Pacific Islander_x000D_
+15 = Other_x000D_
+21 = Bridged White_x000D_
+22 = Bridged Black_x000D_
+23 = Bridged American Indian/Alaskan Native_x000D_
 24 = Bridged Asian &amp; Pacific Islander</t>
   </si>
   <si>
@@ -7715,24 +7716,24 @@
     <t>Informant's Relationship to Fetus</t>
   </si>
   <si>
-    <t>1 = Mother
-2 = Father
-3 = Sibling
-4 = Other relative
-5 = Other
+    <t>1 = Mother_x000D_
+2 = Father_x000D_
+3 = Sibling_x000D_
+4 = Other relative_x000D_
+5 = Other_x000D_
 9 = Unknown</t>
   </si>
   <si>
-    <t xml:space="preserve">Only similar item is Mortality: "Informant's Relationship (INFORMRELATE), which uses VRDR Decedent  contact.type.text   string (30 characters)
-VRCPL has:
-  - Patient-decedent-fetus, 
-  - Related Person - Parent Vital Records   
-  - RelatedPerson - Father Natural Vital Records         
-  - RelatedPerson - Father Vital Records         
-  - RelatedPerson - Mother Gestational Vital Records         
-  - RelatedPerson - Mother Vital Records
-NOTE that the IJE Code Structure Description here includes Sibling and others
-Saul notes: VRDR uses fields that can be from a controlled vocabulary or any arbitrary string (e.g., CERTL in  http://build.fhir.org/ig/HL7/vrdr/branches/master/StructureDefinition-vrdr-death-certification.html) with a consistent pattern (I think
+    <t xml:space="preserve">Only similar item is Mortality: "Informant's Relationship (INFORMRELATE), which uses VRDR Decedent  contact.type.text   string (30 characters)_x000D_
+VRCPL has:_x000D_
+  - Patient-decedent-fetus, _x000D_
+  - Related Person - Parent Vital Records   _x000D_
+  - RelatedPerson - Father Natural Vital Records         _x000D_
+  - RelatedPerson - Father Vital Records         _x000D_
+  - RelatedPerson - Mother Gestational Vital Records         _x000D_
+  - RelatedPerson - Mother Vital Records_x000D_
+NOTE that the IJE Code Structure Description here includes Sibling and others_x000D_
+Saul notes: VRDR uses fields that can be from a controlled vocabulary or any arbitrary string (e.g., CERTL in  http://build.fhir.org/ig/HL7/vrdr/branches/master/StructureDefinition-vrdr-death-certification.html) with a consistent pattern (I think_x000D_
 there are two such fields). </t>
   </si>
   <si>
@@ -7787,9 +7788,9 @@
     <t>Deprecated, see [VRFM]</t>
   </si>
   <si>
-    <t>Code used on 3 tabs: N, FD, &amp; BID
-Mortality (VRDR) uses   DeathCertificate  extension[replaceStatus].valuecodeable   [ReplaceStatusVS]
-VRDR addresses in the VRDR Messaging IG. 
+    <t>Code used on 3 tabs: N, FD, &amp; BID_x000D_
+Mortality (VRDR) uses   DeathCertificate  extension[replaceStatus].valuecodeable   [ReplaceStatusVS]_x000D_
+VRDR addresses in the VRDR Messaging IG. _x000D_
 Decision: Births should behave the same as deaths.</t>
   </si>
   <si>
@@ -7805,30 +7806,31 @@
     <t>State, U.S. Territory or Canadian Province of Birth (Infant) - code</t>
   </si>
   <si>
-    <t xml:space="preserve">
-NCHS Instruction Manual: Part 8
-ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY
-XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA
-YC = NEW YORK CITY
-For US Territories:
-   MP  NORTHERN MARIANAS
-   AS  AMERICAN SAMOA
-   GU  GUAM
-   VI   VIRGIN ISLANDS
-   PR  PUERTO RICO
-For Canadian Provinces:
-   AB  ALBERTA  
-   BC  BRITISH COLUMBIA 
-   MB  MANITOBA 
-   NB  NEW BRUNSWICK  
-   NL  NEWFOUNDLAND AND LABRADOR  
-   NS  NOVA SCOTIA 
-   NT  NORTHWEST TERRITORIES
-   NU  NUNAVUT
-   ON  ONTARIO
-   PE  PRINCE EDWARD ISLAND 
-   QC  QUEBEC  
-   SK  SASKATCHEWAN
+    <t>_x000D_
+NCHS Instruction Manual: Part 8_x000D_
+ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY_x000D_
+XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA_x000D_
+YC = NEW YORK CITY_x000D_
+_x000D_
+For US Territories:_x000D_
+   MP  NORTHERN MARIANAS_x000D_
+   AS  AMERICAN SAMOA_x000D_
+   GU  GUAM_x000D_
+   VI   VIRGIN ISLANDS_x000D_
+   PR  PUERTO RICO_x000D_
+For Canadian Provinces:_x000D_
+   AB  ALBERTA  _x000D_
+   BC  BRITISH COLUMBIA _x000D_
+   MB  MANITOBA _x000D_
+   NB  NEW BRUNSWICK  _x000D_
+   NL  NEWFOUNDLAND AND LABRADOR  _x000D_
+   NS  NOVA SCOTIA _x000D_
+   NT  NORTHWEST TERRITORIES_x000D_
+   NU  NUNAVUT_x000D_
+   ON  ONTARIO_x000D_
+   PE  PRINCE EDWARD ISLAND _x000D_
+   QC  QUEBEC  _x000D_
+   SK  SASKATCHEWAN_x000D_
    YT  YUKON</t>
   </si>
   <si>
@@ -7847,8 +7849,8 @@
     <t>identifier.extension[localFileNumber2].value</t>
   </si>
   <si>
-    <t>male = Male
-female = Female
+    <t>male = Male_x000D_
+female = Female_x000D_
 other = Other unknown = Unknown</t>
   </si>
   <si>
@@ -7864,8 +7866,8 @@
     <t>ISEX</t>
   </si>
   <si>
-    <t>M = Male
-F = Female
+    <t>M = Male_x000D_
+F = Female_x000D_
 N = Not Yet Determined</t>
   </si>
   <si>
@@ -7899,31 +7901,31 @@
     <t>4 digit year (&lt; year of birth of child);  9999 = unknown</t>
   </si>
   <si>
-    <t>0 = Edit Passed
+    <t>0 = Edit Passed_x000D_
 1 = Data Queried</t>
   </si>
   <si>
-    <t>NCHS Instruction Manual: Part 8
-   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY
-   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA           For U.S. Territories:
-   MP  NORTHERN MARIANAS
-   AS  AMERICAN SAMOA
-   GU  GUAM
-   VI   VIRGIN ISLANDS
-   PR  PUERTO RICO
-For Canadian Provinces:
-   AB  ALBERTA  
-   BC  BRITISH COLUMBIA 
-   MB  MANITOBA 
-   NB  NEW BRUNSWICK  
-   NL  NEWFOUNDLAND AND LABRADOR 
-   NS  NOVA SCOTIA 
-   NT  NORTHWEST TERRITORIES
-   NU  NUNAVUT
-   ON  ONTARIO
-   PE  PRINCE EDWARD ISLAND 
-   QC  QUEBEC  
-   SK  SASKATCHEWAN
+    <t>NCHS Instruction Manual: Part 8_x000D_
+   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY_x000D_
+   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA           For U.S. Territories:_x000D_
+   MP  NORTHERN MARIANAS_x000D_
+   AS  AMERICAN SAMOA_x000D_
+   GU  GUAM_x000D_
+   VI   VIRGIN ISLANDS_x000D_
+   PR  PUERTO RICO_x000D_
+For Canadian Provinces:_x000D_
+   AB  ALBERTA  _x000D_
+   BC  BRITISH COLUMBIA _x000D_
+   MB  MANITOBA _x000D_
+   NB  NEW BRUNSWICK  _x000D_
+   NL  NEWFOUNDLAND AND LABRADOR _x000D_
+   NS  NOVA SCOTIA _x000D_
+   NT  NORTHWEST TERRITORIES_x000D_
+   NU  NUNAVUT_x000D_
+   ON  ONTARIO_x000D_
+   PE  PRINCE EDWARD ISLAND _x000D_
+   QC  QUEBEC  _x000D_
+   SK  SASKATCHEWAN_x000D_
    YT  YUKON</t>
   </si>
   <si>
@@ -7933,27 +7935,27 @@
     <t>Residence of Mother--City</t>
   </si>
   <si>
-    <t>NCHS Instruction Manual: Part 8
-   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY
-   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA        For U.S. Territories:
-   MP  NORTHERN MARIANAS
-   AS  AMERICAN SAMOA
-   GU  GUAM
-   VI   VIRGIN ISLANDS
-   PR  PUERTO RICO
-For Canadian Provinces:
-   AB  ALBERTA  
-   BC  BRITISH COLUMBIA 
-   MB  MANITOBA 
-   NB  NEW BRUNSWICK  
-   NL  NEWFOUNDLAND AND LABRADOR 
-   NS  NOVA SCOTIA 
-   NT  NORTHWEST TERRITORIES
-   NU  NUNAVUT
-   ON  ONTARIO
-   PE  PRINCE EDWARD ISLAND 
-   QC  QUEBEC  
-   SK  SASKATCHEWAN
+    <t>NCHS Instruction Manual: Part 8_x000D_
+   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY_x000D_
+   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA        For U.S. Territories:_x000D_
+   MP  NORTHERN MARIANAS_x000D_
+   AS  AMERICAN SAMOA_x000D_
+   GU  GUAM_x000D_
+   VI   VIRGIN ISLANDS_x000D_
+   PR  PUERTO RICO_x000D_
+For Canadian Provinces:_x000D_
+   AB  ALBERTA  _x000D_
+   BC  BRITISH COLUMBIA _x000D_
+   MB  MANITOBA _x000D_
+   NB  NEW BRUNSWICK  _x000D_
+   NL  NEWFOUNDLAND AND LABRADOR _x000D_
+   NS  NOVA SCOTIA _x000D_
+   NT  NORTHWEST TERRITORIES_x000D_
+   NU  NUNAVUT_x000D_
+   ON  ONTARIO_x000D_
+   PE  PRINCE EDWARD ISLAND _x000D_
+   QC  QUEBEC  _x000D_
+   SK  SASKATCHEWAN_x000D_
    YT  YUKON</t>
   </si>
   <si>
@@ -7993,8 +7995,8 @@
     <t>Literal; blank</t>
   </si>
   <si>
-    <t xml:space="preserve">NCHS Appendix E
-(values for fields 62 - 77 returned from NCHS)
+    <t xml:space="preserve">NCHS Appendix E_x000D_
+(values for fields 62 - 77 returned from NCHS)_x000D_
 </t>
   </si>
   <si>
@@ -8004,7 +8006,7 @@
     <t>component[ThirdEditedCode].value, &lt;br /&gt;code=CodeSystemLocalObservationsCodesVitalRecords#codedraceandethnicityMother</t>
   </si>
   <si>
-    <t>NCHS Appendix E
+    <t>NCHS Appendix E_x000D_
 (values for fields 108 - 123 returned from NCHS)</t>
   </si>
   <si>
@@ -8026,11 +8028,11 @@
     <t>01-31 (based on month), 88=no care, 99=unknown</t>
   </si>
   <si>
-    <t xml:space="preserve">4 digit year; year of child's birth or
+    <t xml:space="preserve">4 digit year; year of child's birth or_x000D_
 (year of child's birth - 1), 8888=no care, 9999=unknown </t>
   </si>
   <si>
-    <t>4 digit year; year of child's birth or 
+    <t>4 digit year; year of child's birth or _x000D_
 (year of child's birth - 1), 8888=no care, 9999=unknown</t>
   </si>
   <si>
@@ -8061,7 +8063,7 @@
     <t>ObservationNumberOtherPregnancyOutcomes</t>
   </si>
   <si>
-    <t>4 digit year;(year of mother's birth + 10) through
+    <t>4 digit year;(year of mother's birth + 10) through_x000D_
 year of child's birth, 8888, 9999</t>
   </si>
   <si>
@@ -8083,13 +8085,13 @@
     <t>PAY</t>
   </si>
   <si>
-    <t>1 = Medicaid
-2 = Private Insurance
-3 = Self-pay
-4 = Indian Health Service
-5 = CHAMPUS/TRICARE
-6 = Other Government (Fed, State, Local) 
-8 = Other
+    <t>1 = Medicaid_x000D_
+2 = Private Insurance_x000D_
+3 = Self-pay_x000D_
+4 = Indian Health Service_x000D_
+5 = CHAMPUS/TRICARE_x000D_
+6 = Other Government (Fed, State, Local) _x000D_
+8 = Other_x000D_
 9 = Unknown</t>
   </si>
   <si>
@@ -8102,8 +8104,8 @@
     <t>[BirthAndFetalDeathFinancialClassVS] </t>
   </si>
   <si>
-    <t>4 digit year; year of child's birth 
-or (year of child's birth - 1)
+    <t>4 digit year; year of child's birth _x000D_
+or (year of child's birth - 1)_x000D_
 or (year of child's birth - 2), 9999</t>
   </si>
   <si>
@@ -8236,8 +8238,8 @@
     <t>See [note on missing characteristics of labor and delivery data]</t>
   </si>
   <si>
-    <t>Update L&amp;D (old Observation-characteristic-of-labor-and-delivery)
-STU 1 listed:
+    <t>Update L&amp;D (old Observation-characteristic-of-labor-and-delivery)_x000D_
+STU 1 listed:_x000D_
 IJE Natality Data Elements: INDL, AUGL, NVPR, STER, ANTB, CHOR, ESAN</t>
   </si>
   <si>
@@ -8292,9 +8294,9 @@
     <t>MECS</t>
   </si>
   <si>
-    <t>Update L&amp;D (old Observation-characteristic-of-labor-and-delivery)
-STU 1 listed:
-IJE Natality Data Elements: INDL, AUGL, NVPR, STER, ANTB, CHOR, ESAN
+    <t>Update L&amp;D (old Observation-characteristic-of-labor-and-delivery)_x000D_
+STU 1 listed:_x000D_
+IJE Natality Data Elements: INDL, AUGL, NVPR, STER, ANTB, CHOR, ESAN_x000D_
 (new) MECS</t>
   </si>
   <si>
@@ -8304,9 +8306,9 @@
     <t>FINT</t>
   </si>
   <si>
-    <t>Update L&amp;D (old Observation-characteristic-of-labor-and-delivery)
-STU 1 listed:
-IJE Natality Data Elements: INDL, AUGL, NVPR, STER, ANTB, CHOR, ESAN
+    <t>Update L&amp;D (old Observation-characteristic-of-labor-and-delivery)_x000D_
+STU 1 listed:_x000D_
+IJE Natality Data Elements: INDL, AUGL, NVPR, STER, ANTB, CHOR, ESAN_x000D_
 (new) FINT</t>
   </si>
   <si>
@@ -8352,8 +8354,8 @@
     <t>BW_BYPASS</t>
   </si>
   <si>
-    <t>0 = Off
-1 = Queried data correct, out of range
+    <t>0 = Off_x000D_
+1 = Queried data correct, out of range_x000D_
 2 = Queried, failed birthweight/gestation edit</t>
   </si>
   <si>
@@ -8393,8 +8395,8 @@
     <t>ObservationNumberLiveBirthsThisDelivery</t>
   </si>
   <si>
-    <t>0 = OFF
-1 = Queried, and Correct
+    <t>0 = OFF_x000D_
+1 = Queried, and Correct_x000D_
 2 = Plurality/Set Order Queried, Inconsistent</t>
   </si>
   <si>
@@ -8410,8 +8412,8 @@
     <t>See [note on missing abnormal conditions of newborn data]</t>
   </si>
   <si>
-    <t>Update abnormal conditions of  newborn (old Condition-abnormal-condition-of-newborn)
-STU 1 listed:
+    <t>Update abnormal conditions of  newborn (old Condition-abnormal-condition-of-newborn)_x000D_
+STU 1 listed:_x000D_
 IJE Natality Data Elements: AVEN1, AVEN6, NICU, SURF, ANTI, SEIZ, MCPH</t>
   </si>
   <si>
@@ -8469,9 +8471,9 @@
     <t>BINJ</t>
   </si>
   <si>
-    <t>Update abnormal conditions of  newborn (old Condition-abnormal-condition-of-newborn)
-STU 1 listed:
-IJE Natality Data Elements: AVEN1, AVEN6, NICU, SURF, ANTI, SEIZ, MCPH
+    <t>Update abnormal conditions of  newborn (old Condition-abnormal-condition-of-newborn)_x000D_
+STU 1 listed:_x000D_
+IJE Natality Data Elements: AVEN1, AVEN6, NICU, SURF, ANTI, SEIZ, MCPH_x000D_
 (new) BINJ</t>
   </si>
   <si>
@@ -8571,8 +8573,8 @@
     <t>ILIV</t>
   </si>
   <si>
-    <t>Y = Yes
-N = No
+    <t>Y = Yes_x000D_
+N = No_x000D_
 U = Infant transferred, Status Unknown</t>
   </si>
   <si>
@@ -8591,9 +8593,9 @@
     <t>leave blank</t>
   </si>
   <si>
-    <t>Code used on 3 tabs: N, FD, &amp; BID
-Code sent back to state VRO
-For R_YR, R_MO, R_DY, VRDR uses CodingStatusValues  parameter[receiptDate].value   date    See [PartialDatesAndTimes]
+    <t>Code used on 3 tabs: N, FD, &amp; BID_x000D_
+Code sent back to state VRO_x000D_
+For R_YR, R_MO, R_DY, VRDR uses CodingStatusValues  parameter[receiptDate].value   date    See [PartialDatesAndTimes]_x000D_
 Decision: Mimic VRDR</t>
   </si>
   <si>
@@ -8603,10 +8605,10 @@
     <t>Risk Factors--Infertility: Fertility Enhancing Drugs  (RECOMMENDED ADDITION EFFECTIVE 2004)</t>
   </si>
   <si>
-    <t>Y = Yes
-N = No
-X = Not Applicable
-U = Unknown
+    <t>Y = Yes_x000D_
+N = No_x000D_
+X = Not Applicable_x000D_
+U = Unknown_x000D_
 (BLANK IF NOT ADDED)</t>
   </si>
   <si>
@@ -8763,27 +8765,27 @@
     <t>Refer to NCHS Instruction Manual Part 19, Industry and Occupation Coding for Death Certificates, 2003. Leave blank if using a coding system other than this</t>
   </si>
   <si>
-    <t>NCHS Instruction Manual: Part 8
-   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY
-   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA           For U.S. Territories:
-   MP  NORTHERN MARIANAS
-   AS  AMERICAN SAMOA
-   GU  GUAM
-   VI   VIRGIN ISLANDS
-   PR  PUERTO RICO
-For Canadian Provinces:
-   AB  ALBERTA  
-   BC  BRITISH COLUMBIA 
-   MB  MANITOBA 
-   NB  NEW BRUNSWICK  
-   NL  NEWFOUNDLAND AND LABRADOR  
-   NS  NOVA SCOTIA 
-   NT  NORTHWEST TERRITORIES
-   NU  NUNAVUT
-   ON  ONTARIO
-   PE  PRINCE EDWARD ISLAND 
-   QC  QUEBEC  
-   SK  SASKATCHEWAN
+    <t>NCHS Instruction Manual: Part 8_x000D_
+   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY_x000D_
+   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA           For U.S. Territories:_x000D_
+   MP  NORTHERN MARIANAS_x000D_
+   AS  AMERICAN SAMOA_x000D_
+   GU  GUAM_x000D_
+   VI   VIRGIN ISLANDS_x000D_
+   PR  PUERTO RICO_x000D_
+For Canadian Provinces:_x000D_
+   AB  ALBERTA  _x000D_
+   BC  BRITISH COLUMBIA _x000D_
+   MB  MANITOBA _x000D_
+   NB  NEW BRUNSWICK  _x000D_
+   NL  NEWFOUNDLAND AND LABRADOR  _x000D_
+   NS  NOVA SCOTIA _x000D_
+   NT  NORTHWEST TERRITORIES_x000D_
+   NU  NUNAVUT_x000D_
+   ON  ONTARIO_x000D_
+   PE  PRINCE EDWARD ISLAND _x000D_
+   QC  QUEBEC  _x000D_
+   SK  SASKATCHEWAN_x000D_
    YT  YUKON</t>
   </si>
   <si>
@@ -8907,8 +8909,8 @@
     <t>SSN_MULT_BTH_CD</t>
   </si>
   <si>
-    <t>Y = Yes
-N = No
+    <t>Y = Yes_x000D_
+N = No_x000D_
 or blank</t>
   </si>
   <si>
@@ -8957,12 +8959,12 @@
     <t>CERTIF</t>
   </si>
   <si>
-    <t>1 = MD
-2 = DO
-3 = CNM/CM
-4 = Other midwife
-5 = Other (specify) 
-6 = Hospital Admin
+    <t>1 = MD_x000D_
+2 = DO_x000D_
+3 = CNM/CM_x000D_
+4 = Other midwife_x000D_
+5 = Other (specify) _x000D_
+6 = Hospital Admin_x000D_
 9 = Unknown</t>
   </si>
   <si>
@@ -9011,51 +9013,51 @@
     <t>Deprecated,  see [VRFM]</t>
   </si>
   <si>
-    <t>NCHS Instruction Manual: Part 8
-   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY
-   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA              For U.S. Territories:
-   MP  NORTHERN MARIANAS
-   AS  AMERICAN SAMOA
-   GU  GUAM
-   VI   VIRGIN ISLANDS
-   PR  PUERTO RICO
-For Canadian Provinces:
-   AB  ALBERTA  
-   BC  BRITISH COLUMBIA 
-   MB  MANITOBA 
-   NB  NEW BRUNSWICK  
-   NL  NEWFOUNDLAND AND LABRADOR 
-   NS  NOVA SCOTIA 
-   NT  NORTHWEST TERRITORIES
-   NU  NUNAVUT
-   ON  ONTARIO
-   PE  PRINCE EDWARD ISLAND 
-   QC  QUEBEC  
-   SK  SASKATCHEWAN
+    <t>NCHS Instruction Manual: Part 8_x000D_
+   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY_x000D_
+   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA              For U.S. Territories:_x000D_
+   MP  NORTHERN MARIANAS_x000D_
+   AS  AMERICAN SAMOA_x000D_
+   GU  GUAM_x000D_
+   VI   VIRGIN ISLANDS_x000D_
+   PR  PUERTO RICO_x000D_
+For Canadian Provinces:_x000D_
+   AB  ALBERTA  _x000D_
+   BC  BRITISH COLUMBIA _x000D_
+   MB  MANITOBA _x000D_
+   NB  NEW BRUNSWICK  _x000D_
+   NL  NEWFOUNDLAND AND LABRADOR _x000D_
+   NS  NOVA SCOTIA _x000D_
+   NT  NORTHWEST TERRITORIES_x000D_
+   NU  NUNAVUT_x000D_
+   ON  ONTARIO_x000D_
+   PE  PRINCE EDWARD ISLAND _x000D_
+   QC  QUEBEC  _x000D_
+   SK  SASKATCHEWAN_x000D_
    YT  YUKON</t>
   </si>
   <si>
-    <t>NCHS Instruction Manual: Part 8
-   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY
-   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA            For U.S. Territories:
-   MP  NORTHERN MARIANAS
-   AS  AMERICAN SAMOA
-   GU  GUAM
-   VI   VIRGIN ISLANDS
-   PR  PUERTO RICO
-For Canadian Provinces:
-   AB  ALBERTA  
-   BC  BRITISH COLUMBIA 
-   MB  MANITOBA 
-   NB  NEW BRUNSWICK  
-   NL  NEWFOUNDLAND AND LABRADOR 
-   NS  NOVA SCOTIA 
-   NT  NORTHWEST TERRITORIES
-   NU  NUNAVUT
-   ON  ONTARIO
-   PE  PRINCE EDWARD ISLAND 
-   QC  QUEBEC  
-   SK  SASKATCHEWAN
+    <t>NCHS Instruction Manual: Part 8_x000D_
+   ZZ = UNKNOWN OR BLANK U.S. STATE OR TERRITORY OR UNKNOWN/ UNCLASSIFIABLE COUNTRY_x000D_
+   XX = COUNTRY IS CANADA BUT UNKNOWN CANADIAN PROVINCE OR ANY COUNTRY THAT IS KNOWN, BUT NOT U.S. OR CANADA            For U.S. Territories:_x000D_
+   MP  NORTHERN MARIANAS_x000D_
+   AS  AMERICAN SAMOA_x000D_
+   GU  GUAM_x000D_
+   VI   VIRGIN ISLANDS_x000D_
+   PR  PUERTO RICO_x000D_
+For Canadian Provinces:_x000D_
+   AB  ALBERTA  _x000D_
+   BC  BRITISH COLUMBIA _x000D_
+   MB  MANITOBA _x000D_
+   NB  NEW BRUNSWICK  _x000D_
+   NL  NEWFOUNDLAND AND LABRADOR _x000D_
+   NS  NOVA SCOTIA _x000D_
+   NT  NORTHWEST TERRITORIES_x000D_
+   NU  NUNAVUT_x000D_
+   ON  ONTARIO_x000D_
+   PE  PRINCE EDWARD ISLAND _x000D_
+   QC  QUEBEC  _x000D_
+   SK  SASKATCHEWAN_x000D_
    YT  YUKON</t>
   </si>
   <si>
@@ -9131,7 +9133,7 @@
     <t>Residence Street number</t>
   </si>
   <si>
-    <t>For use of jurisdictions with domestic partnerships, other
+    <t>For use of jurisdictions with domestic partnerships, other_x000D_
 types of relationships.</t>
   </si>
   <si>
@@ -9156,26 +9158,26 @@
     <t>Death Jurisdiction - code</t>
   </si>
   <si>
-    <t>NCHS Instruction Manual Part 8A
- For U.S. Territories:
-   MP  NORTHERN MARIANAS
-   AS  AMERICAN SAMOA
-   GU  GUAM
-   VI   VIRGIN ISLANDS
-   PR  PUERTO RICO
- For Canadian Provinces:
-   AB  ALBERTA  
-   BC  BRITISH COLUMBIA 
-   MB  MANITOBA 
-   NB  NEW BRUNSWICK  
-   NL  NEWFOUNDLAND AND LABRADOR  
-   NS  NOVA SCOTIA 
-   NT  NORTHWEST TERRITORIES
-   NU  NUNAVUT
-   ON  ONTARIO
-   PE  PRINCE EDWARD ISLAND 
-   QC  QUEBEC  
-   SK  SASKATCHEWAN
+    <t>NCHS Instruction Manual Part 8A_x000D_
+ For U.S. Territories:_x000D_
+   MP  NORTHERN MARIANAS_x000D_
+   AS  AMERICAN SAMOA_x000D_
+   GU  GUAM_x000D_
+   VI   VIRGIN ISLANDS_x000D_
+   PR  PUERTO RICO_x000D_
+ For Canadian Provinces:_x000D_
+   AB  ALBERTA  _x000D_
+   BC  BRITISH COLUMBIA _x000D_
+   MB  MANITOBA _x000D_
+   NB  NEW BRUNSWICK  _x000D_
+   NL  NEWFOUNDLAND AND LABRADOR  _x000D_
+   NS  NOVA SCOTIA _x000D_
+   NT  NORTHWEST TERRITORIES_x000D_
+   NU  NUNAVUT_x000D_
+   ON  ONTARIO_x000D_
+   PE  PRINCE EDWARD ISLAND _x000D_
+   QC  QUEBEC  _x000D_
+   SK  SASKATCHEWAN_x000D_
    YT  YUKON</t>
   </si>
   <si>

</xml_diff>

<commit_message>
move autopsy perform indicator from vrcl
</commit_message>
<xml_diff>
--- a/input/images/IJE_File_Layouts_and_FHIR_Mapping_24-06-21.xlsx
+++ b/input/images/IJE_File_Layouts_and_FHIR_Mapping_24-06-21.xlsx
@@ -6058,7 +6058,10 @@
 P = Planned</t>
   </si>
   <si>
-    <t>ObservationAutopsyPerformedIndicatorVitalRecords</t>
+    <t>ObservationAutopsyPerformedIndicator</t>
+  </si>
+  <si>
+    <t>[PerformedNotPerformedPlannedVS]</t>
   </si>
   <si>
     <t>Was a Histological Placental Examination Performed?</t>
@@ -6068,9 +6071,6 @@
   </si>
   <si>
     <t>ObservationHistologicalPlacentalExamPerformed</t>
-  </si>
-  <si>
-    <t>[HistologicalPlacentalExaminationVS]</t>
   </si>
   <si>
     <t>Were Autopsy or Histological Placental Examination Results Used in Determining the Cause of Fetal Death?</t>
@@ -41256,7 +41256,7 @@
         <v>1827</v>
       </c>
       <c r="I153" t="s">
-        <v>205</v>
+        <v>939</v>
       </c>
       <c r="J153" t="s">
         <v>1828</v>
@@ -41268,7 +41268,7 @@
         <v>33</v>
       </c>
       <c r="M153" t="s">
-        <v>456</v>
+        <v>1829</v>
       </c>
       <c r="N153" s="1" t="s">
         <v>952</v>
@@ -41289,10 +41289,10 @@
         <v>1</v>
       </c>
       <c r="E154" s="1" t="s">
-        <v>1829</v>
+        <v>1830</v>
       </c>
       <c r="F154" s="4" t="s">
-        <v>1830</v>
+        <v>1831</v>
       </c>
       <c r="G154" s="1" t="s">
         <v>1827</v>
@@ -41301,7 +41301,7 @@
         <v>939</v>
       </c>
       <c r="J154" t="s">
-        <v>1831</v>
+        <v>1832</v>
       </c>
       <c r="K154" s="1" t="s">
         <v>24</v>
@@ -41310,7 +41310,7 @@
         <v>33</v>
       </c>
       <c r="M154" t="s">
-        <v>1832</v>
+        <v>1829</v>
       </c>
       <c r="N154" s="1" t="s">
         <v>952</v>

</xml_diff>

<commit_message>
adding back some stuff not in master sheets for dd
</commit_message>
<xml_diff>
--- a/input/images/IJE_File_Layouts_and_FHIR_Mapping_24-06-21.xlsx
+++ b/input/images/IJE_File_Layouts_and_FHIR_Mapping_24-06-21.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12180" uniqueCount="2785">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12178" uniqueCount="2785">
   <si>
     <t>This content was derived from the file IJE_File_Layouts_Version_2021_FHIR* and is automatically generated from the source file IJE_File_Layouts_and_FHIR_Mapping_24-06-21.csv.
 The CSV version of the file is used to drive the content of narrative generated for the Vital Records Implementation Guides (VRDR, BFDR, and VRCL).
@@ -5893,7 +5893,7 @@
     <t>code</t>
   </si>
   <si>
-    <t>See  [note on missing method of delivery data]</t>
+    <t>[DeliveryRoutesVS] unless unknown, &lt;br /&gt;See  [note on missing method of delivery data]</t>
   </si>
   <si>
     <t>Method of Delivery--Trial of Labor Attempted</t>
@@ -45909,9 +45909,6 @@
       <c r="L270" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="M270" t="s">
-        <v>104</v>
-      </c>
       <c r="N270" s="1" t="s">
         <v>953</v>
       </c>
@@ -45950,9 +45947,6 @@
       </c>
       <c r="L271" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="M271" t="s">
-        <v>104</v>
       </c>
       <c r="N271" s="1" t="s">
         <v>953</v>

</xml_diff>

<commit_message>
national reporting flagging updates
</commit_message>
<xml_diff>
--- a/input/images/IJE_File_Layouts_and_FHIR_Mapping_24-06-21.xlsx
+++ b/input/images/IJE_File_Layouts_and_FHIR_Mapping_24-06-21.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12797" uniqueCount="2788">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12768" uniqueCount="2788">
   <si>
     <t>This content was derived from the file IJE_File_Layouts_Version_2021_FHIR* and is automatically generated from the source file IJE_File_Layouts_and_FHIR_Mapping_24-06-21.csv.
 The CSV version of the file is used to drive the content of narrative generated for the Vital Records Implementation Guides (VRDR, BFDR, and VRCL).
@@ -10629,9 +10629,6 @@
       </c>
       <c r="N22" s="1"/>
       <c r="P22" s="1"/>
-      <c r="S22" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="23" spans="1:19">
       <c r="A23">
@@ -35911,9 +35908,6 @@
         <v>43</v>
       </c>
       <c r="P8" s="1"/>
-      <c r="S8" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="9" spans="1:19">
       <c r="A9">
@@ -40775,9 +40769,6 @@
         <v>43</v>
       </c>
       <c r="P123" s="1"/>
-      <c r="S123" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="124" spans="1:19">
       <c r="A124">
@@ -42351,9 +42342,6 @@
         <v>43</v>
       </c>
       <c r="P161" s="1"/>
-      <c r="S161" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="162" spans="1:19">
       <c r="A162">
@@ -42868,9 +42856,6 @@
       <c r="R175" t="s">
         <v>1884</v>
       </c>
-      <c r="S175" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="176" spans="1:19">
       <c r="A176">
@@ -42914,9 +42899,6 @@
       <c r="R176" t="s">
         <v>1884</v>
       </c>
-      <c r="S176" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="177" spans="1:19">
       <c r="A177">
@@ -42959,9 +42941,6 @@
       </c>
       <c r="R177" t="s">
         <v>1884</v>
-      </c>
-      <c r="S177" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="178" spans="1:19">
@@ -51226,9 +51205,6 @@
         <v>43</v>
       </c>
       <c r="P7" s="1"/>
-      <c r="S7" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="8" spans="1:19">
       <c r="A8">
@@ -54224,9 +54200,6 @@
         <v>1569</v>
       </c>
       <c r="P78" s="1"/>
-      <c r="S78" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="79" spans="1:19">
       <c r="A79">
@@ -54269,9 +54242,6 @@
         <v>1569</v>
       </c>
       <c r="P79" s="1"/>
-      <c r="S79" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="80" spans="1:19">
       <c r="A80">
@@ -54314,9 +54284,6 @@
         <v>1569</v>
       </c>
       <c r="P80" s="1"/>
-      <c r="S80" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="81" spans="1:19">
       <c r="A81">
@@ -54359,9 +54326,6 @@
         <v>1569</v>
       </c>
       <c r="P81" s="1"/>
-      <c r="S81" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="82" spans="1:19">
       <c r="A82">
@@ -54404,9 +54368,6 @@
         <v>1569</v>
       </c>
       <c r="P82" s="1"/>
-      <c r="S82" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="83" spans="1:19">
       <c r="A83">
@@ -54449,9 +54410,6 @@
         <v>1569</v>
       </c>
       <c r="P83" s="1"/>
-      <c r="S83" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="84" spans="1:19">
       <c r="A84">
@@ -54494,9 +54452,6 @@
         <v>1569</v>
       </c>
       <c r="P84" s="1"/>
-      <c r="S84" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="85" spans="1:19">
       <c r="A85">
@@ -54539,9 +54494,6 @@
         <v>1569</v>
       </c>
       <c r="P85" s="1"/>
-      <c r="S85" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="86" spans="1:19">
       <c r="A86">
@@ -54584,9 +54536,6 @@
         <v>1569</v>
       </c>
       <c r="P86" s="1"/>
-      <c r="S86" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="87" spans="1:19">
       <c r="A87">
@@ -54629,9 +54578,6 @@
         <v>1569</v>
       </c>
       <c r="P87" s="1"/>
-      <c r="S87" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="88" spans="1:19">
       <c r="A88">
@@ -54674,9 +54620,6 @@
         <v>1569</v>
       </c>
       <c r="P88" s="1"/>
-      <c r="S88" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="89" spans="1:19">
       <c r="A89">
@@ -54719,9 +54662,6 @@
         <v>1569</v>
       </c>
       <c r="P89" s="1"/>
-      <c r="S89" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="90" spans="1:19">
       <c r="A90">
@@ -54764,9 +54704,6 @@
         <v>1569</v>
       </c>
       <c r="P90" s="1"/>
-      <c r="S90" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="91" spans="1:19">
       <c r="A91">
@@ -54809,9 +54746,6 @@
         <v>1569</v>
       </c>
       <c r="P91" s="1"/>
-      <c r="S91" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="92" spans="1:19">
       <c r="A92">
@@ -54854,9 +54788,6 @@
         <v>1569</v>
       </c>
       <c r="P92" s="1"/>
-      <c r="S92" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="93" spans="1:19">
       <c r="A93">
@@ -54899,9 +54830,6 @@
         <v>1569</v>
       </c>
       <c r="P93" s="1"/>
-      <c r="S93" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="94" spans="1:19">
       <c r="A94">
@@ -60711,9 +60639,6 @@
         <v>43</v>
       </c>
       <c r="P226" s="1"/>
-      <c r="S226" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="227" spans="1:19">
       <c r="A227">
@@ -61826,9 +61751,6 @@
       <c r="R250" t="s">
         <v>1884</v>
       </c>
-      <c r="S250" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="251" spans="1:19">
       <c r="A251">
@@ -61872,9 +61794,6 @@
       <c r="R251" t="s">
         <v>1884</v>
       </c>
-      <c r="S251" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="252" spans="1:19">
       <c r="A252">
@@ -61918,9 +61837,6 @@
       <c r="R252" t="s">
         <v>1884</v>
       </c>
-      <c r="S252" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="253" spans="1:19">
       <c r="A253">
@@ -62376,9 +62292,6 @@
       </c>
       <c r="P262" s="1" t="s">
         <v>2630</v>
-      </c>
-      <c r="S262" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="263" spans="1:19">

</xml_diff>

<commit_message>
updates to national flagging dd
</commit_message>
<xml_diff>
--- a/input/images/IJE_File_Layouts_and_FHIR_Mapping_24-06-21.xlsx
+++ b/input/images/IJE_File_Layouts_and_FHIR_Mapping_24-06-21.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12768" uniqueCount="2788">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12836" uniqueCount="2788">
   <si>
     <t>This content was derived from the file IJE_File_Layouts_Version_2021_FHIR* and is automatically generated from the source file IJE_File_Layouts_and_FHIR_Mapping_24-06-21.csv.
 The CSV version of the file is used to drive the content of narrative generated for the Vital Records Implementation Guides (VRDR, BFDR, and VRCL).
@@ -1075,6 +1075,9 @@
     <t>component[FirstEditedCode].value, &lt;br /&gt;code=CodeSystemLocalObservationsCodesVitalRecords#codedraceandethnicityDecedent</t>
   </si>
   <si>
+    <t>[ValueSetRaceCodeVitalRecords]</t>
+  </si>
+  <si>
     <t>Second Edited Code</t>
   </si>
   <si>
@@ -1085,9 +1088,6 @@
   </si>
   <si>
     <t>component[SecondEditedCode].value, &lt;br /&gt;code=CodeSystemLocalObservationsCodesVitalRecords#codedraceandethnicityDecedent</t>
-  </si>
-  <si>
-    <t>[ValueSetRaceCodeVitalRecords]</t>
   </si>
   <si>
     <t>Third Edited Code</t>
@@ -13053,9 +13053,11 @@
       <c r="K75" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="L75" s="1"/>
+      <c r="L75" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="M75" t="s">
-        <v>43</v>
+        <v>305</v>
       </c>
       <c r="N75" s="1"/>
       <c r="P75" s="1"/>
@@ -13074,13 +13076,13 @@
         <v>3</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="F76" s="4" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="I76" t="s">
         <v>208</v>
@@ -13089,13 +13091,13 @@
         <v>303</v>
       </c>
       <c r="K76" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="L76" s="1" t="s">
         <v>35</v>
       </c>
       <c r="M76" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N76" s="1"/>
       <c r="P76" s="1"/>
@@ -13120,7 +13122,7 @@
         <v>311</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="I77" t="s">
         <v>208</v>
@@ -13135,7 +13137,7 @@
         <v>35</v>
       </c>
       <c r="M77" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N77" s="1"/>
       <c r="P77" s="1"/>
@@ -13160,7 +13162,7 @@
         <v>314</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="I78" t="s">
         <v>208</v>
@@ -13175,7 +13177,7 @@
         <v>35</v>
       </c>
       <c r="M78" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N78" s="1"/>
       <c r="P78" s="1"/>
@@ -13200,7 +13202,7 @@
         <v>317</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="I79" t="s">
         <v>208</v>
@@ -13215,7 +13217,7 @@
         <v>35</v>
       </c>
       <c r="M79" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N79" s="1"/>
       <c r="P79" s="1"/>
@@ -13240,7 +13242,7 @@
         <v>320</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="I80" t="s">
         <v>208</v>
@@ -13255,7 +13257,7 @@
         <v>35</v>
       </c>
       <c r="M80" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N80" s="1"/>
       <c r="P80" s="1"/>
@@ -13280,7 +13282,7 @@
         <v>323</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="I81" t="s">
         <v>208</v>
@@ -13295,7 +13297,7 @@
         <v>35</v>
       </c>
       <c r="M81" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N81" s="1"/>
       <c r="P81" s="1"/>
@@ -13320,7 +13322,7 @@
         <v>326</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="I82" t="s">
         <v>208</v>
@@ -13335,7 +13337,7 @@
         <v>35</v>
       </c>
       <c r="M82" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N82" s="1"/>
       <c r="P82" s="1"/>
@@ -13360,7 +13362,7 @@
         <v>329</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="I83" t="s">
         <v>208</v>
@@ -13375,7 +13377,7 @@
         <v>35</v>
       </c>
       <c r="M83" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N83" s="1"/>
       <c r="P83" s="1"/>
@@ -13400,7 +13402,7 @@
         <v>332</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="I84" t="s">
         <v>208</v>
@@ -13415,7 +13417,7 @@
         <v>35</v>
       </c>
       <c r="M84" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N84" s="1"/>
       <c r="P84" s="1"/>
@@ -13440,7 +13442,7 @@
         <v>335</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="I85" t="s">
         <v>208</v>
@@ -13455,7 +13457,7 @@
         <v>35</v>
       </c>
       <c r="M85" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N85" s="1"/>
       <c r="P85" s="1"/>
@@ -13480,7 +13482,7 @@
         <v>338</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="I86" t="s">
         <v>208</v>
@@ -13495,7 +13497,7 @@
         <v>35</v>
       </c>
       <c r="M86" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N86" s="1"/>
       <c r="P86" s="1"/>
@@ -13520,7 +13522,7 @@
         <v>341</v>
       </c>
       <c r="G87" s="1" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="I87" t="s">
         <v>208</v>
@@ -13535,7 +13537,7 @@
         <v>35</v>
       </c>
       <c r="M87" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N87" s="1"/>
       <c r="P87" s="1"/>
@@ -13560,7 +13562,7 @@
         <v>344</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="I88" t="s">
         <v>208</v>
@@ -13575,7 +13577,7 @@
         <v>35</v>
       </c>
       <c r="M88" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N88" s="1"/>
       <c r="P88" s="1"/>
@@ -13600,7 +13602,7 @@
         <v>347</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="I89" t="s">
         <v>208</v>
@@ -13615,7 +13617,7 @@
         <v>35</v>
       </c>
       <c r="M89" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N89" s="1"/>
       <c r="P89" s="1"/>
@@ -13640,7 +13642,7 @@
         <v>350</v>
       </c>
       <c r="G90" s="1" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="I90" t="s">
         <v>208</v>
@@ -13655,7 +13657,7 @@
         <v>35</v>
       </c>
       <c r="M90" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N90" s="1"/>
       <c r="P90" s="1"/>
@@ -13699,6 +13701,9 @@
       </c>
       <c r="N91" s="1"/>
       <c r="P91" s="1"/>
+      <c r="S91" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="92" spans="1:19">
       <c r="A92">
@@ -15286,6 +15291,9 @@
       </c>
       <c r="N129" s="1"/>
       <c r="P129" s="1"/>
+      <c r="S129" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="130" spans="1:19">
       <c r="A130">
@@ -15440,6 +15448,9 @@
         <v>28</v>
       </c>
       <c r="P133" s="1"/>
+      <c r="S133" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="134" spans="1:19">
       <c r="A134">
@@ -15768,6 +15779,9 @@
       </c>
       <c r="N141" s="1"/>
       <c r="P141" s="1"/>
+      <c r="S141" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="142" spans="1:19">
       <c r="A142">
@@ -15811,6 +15825,9 @@
       </c>
       <c r="N142" s="1"/>
       <c r="P142" s="1"/>
+      <c r="S142" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="143" spans="1:19">
       <c r="A143">
@@ -15852,6 +15869,9 @@
       </c>
       <c r="N143" s="1"/>
       <c r="P143" s="1"/>
+      <c r="S143" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="144" spans="1:19">
       <c r="A144">
@@ -15893,6 +15913,9 @@
       </c>
       <c r="N144" s="1"/>
       <c r="P144" s="1"/>
+      <c r="S144" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="145" spans="1:19">
       <c r="A145">
@@ -15934,6 +15957,9 @@
       </c>
       <c r="N145" s="1"/>
       <c r="P145" s="1"/>
+      <c r="S145" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="146" spans="1:19">
       <c r="A146">
@@ -15975,6 +16001,9 @@
       </c>
       <c r="N146" s="1"/>
       <c r="P146" s="1"/>
+      <c r="S146" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="147" spans="1:19">
       <c r="A147">
@@ -16016,6 +16045,9 @@
       </c>
       <c r="N147" s="1"/>
       <c r="P147" s="1"/>
+      <c r="S147" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="148" spans="1:19">
       <c r="A148">
@@ -16059,6 +16091,9 @@
       </c>
       <c r="N148" s="1"/>
       <c r="P148" s="1"/>
+      <c r="S148" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="149" spans="1:19">
       <c r="A149">
@@ -16102,6 +16137,9 @@
       </c>
       <c r="N149" s="1"/>
       <c r="P149" s="1"/>
+      <c r="S149" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="150" spans="1:19">
       <c r="A150">
@@ -16145,6 +16183,9 @@
       </c>
       <c r="N150" s="1"/>
       <c r="P150" s="1"/>
+      <c r="S150" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="151" spans="1:19">
       <c r="A151">
@@ -16188,6 +16229,9 @@
       </c>
       <c r="N151" s="1"/>
       <c r="P151" s="1"/>
+      <c r="S151" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="152" spans="1:19">
       <c r="A152">
@@ -16231,6 +16275,9 @@
       </c>
       <c r="N152" s="1"/>
       <c r="P152" s="1"/>
+      <c r="S152" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="153" spans="1:19">
       <c r="A153">
@@ -16983,6 +17030,9 @@
         <v>28</v>
       </c>
       <c r="P169" s="1"/>
+      <c r="S169" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="170" spans="1:19">
       <c r="A170">
@@ -38511,7 +38561,7 @@
         <v>35</v>
       </c>
       <c r="M69" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N69" s="1" t="s">
         <v>1569</v>
@@ -38553,7 +38603,7 @@
         <v>35</v>
       </c>
       <c r="M70" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N70" s="1" t="s">
         <v>1569</v>
@@ -38595,7 +38645,7 @@
         <v>35</v>
       </c>
       <c r="M71" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N71" s="1" t="s">
         <v>1569</v>
@@ -38637,7 +38687,7 @@
         <v>35</v>
       </c>
       <c r="M72" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N72" s="1" t="s">
         <v>1569</v>
@@ -38679,7 +38729,7 @@
         <v>35</v>
       </c>
       <c r="M73" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N73" s="1" t="s">
         <v>1569</v>
@@ -38721,7 +38771,7 @@
         <v>35</v>
       </c>
       <c r="M74" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N74" s="1" t="s">
         <v>1569</v>
@@ -38763,7 +38813,7 @@
         <v>35</v>
       </c>
       <c r="M75" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N75" s="1" t="s">
         <v>1569</v>
@@ -38805,7 +38855,7 @@
         <v>35</v>
       </c>
       <c r="M76" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N76" s="1" t="s">
         <v>1569</v>
@@ -38847,7 +38897,7 @@
         <v>35</v>
       </c>
       <c r="M77" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N77" s="1" t="s">
         <v>1569</v>
@@ -38889,7 +38939,7 @@
         <v>35</v>
       </c>
       <c r="M78" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N78" s="1" t="s">
         <v>1569</v>
@@ -38931,7 +38981,7 @@
         <v>35</v>
       </c>
       <c r="M79" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N79" s="1" t="s">
         <v>1569</v>
@@ -38973,7 +39023,7 @@
         <v>35</v>
       </c>
       <c r="M80" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N80" s="1" t="s">
         <v>1569</v>
@@ -39015,7 +39065,7 @@
         <v>35</v>
       </c>
       <c r="M81" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N81" s="1" t="s">
         <v>1569</v>
@@ -39057,7 +39107,7 @@
         <v>35</v>
       </c>
       <c r="M82" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N82" s="1" t="s">
         <v>1569</v>
@@ -39099,7 +39149,7 @@
         <v>35</v>
       </c>
       <c r="M83" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N83" s="1" t="s">
         <v>1569</v>
@@ -39141,7 +39191,7 @@
         <v>35</v>
       </c>
       <c r="M84" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N84" s="1" t="s">
         <v>1569</v>
@@ -44986,7 +45036,7 @@
       </c>
       <c r="P224" s="1"/>
     </row>
-    <row r="225" spans="1:16">
+    <row r="225" spans="1:19">
       <c r="A225">
         <v>1035</v>
       </c>
@@ -45021,7 +45071,7 @@
       </c>
       <c r="P225" s="1"/>
     </row>
-    <row r="226" spans="1:16">
+    <row r="226" spans="1:19">
       <c r="A226">
         <v>1036</v>
       </c>
@@ -45063,7 +45113,7 @@
       </c>
       <c r="P226" s="1"/>
     </row>
-    <row r="227" spans="1:16">
+    <row r="227" spans="1:19">
       <c r="A227">
         <v>1037</v>
       </c>
@@ -45105,7 +45155,7 @@
       </c>
       <c r="P227" s="1"/>
     </row>
-    <row r="228" spans="1:16">
+    <row r="228" spans="1:19">
       <c r="A228">
         <v>1038</v>
       </c>
@@ -45147,7 +45197,7 @@
       </c>
       <c r="P228" s="1"/>
     </row>
-    <row r="229" spans="1:16">
+    <row r="229" spans="1:19">
       <c r="A229">
         <v>1039</v>
       </c>
@@ -45186,7 +45236,7 @@
       </c>
       <c r="P229" s="1"/>
     </row>
-    <row r="230" spans="1:16">
+    <row r="230" spans="1:19">
       <c r="A230">
         <v>1040</v>
       </c>
@@ -45221,7 +45271,7 @@
       </c>
       <c r="P230" s="1"/>
     </row>
-    <row r="231" spans="1:16">
+    <row r="231" spans="1:19">
       <c r="A231">
         <v>1041</v>
       </c>
@@ -45260,7 +45310,7 @@
       </c>
       <c r="P231" s="1"/>
     </row>
-    <row r="232" spans="1:16">
+    <row r="232" spans="1:19">
       <c r="A232">
         <v>1042</v>
       </c>
@@ -45298,8 +45348,11 @@
         <v>955</v>
       </c>
       <c r="P232" s="1"/>
-    </row>
-    <row r="233" spans="1:16">
+      <c r="S232" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="233" spans="1:19">
       <c r="A233">
         <v>1043</v>
       </c>
@@ -45337,8 +45390,11 @@
         <v>955</v>
       </c>
       <c r="P233" s="1"/>
-    </row>
-    <row r="234" spans="1:16">
+      <c r="S233" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="234" spans="1:19">
       <c r="A234">
         <v>1044</v>
       </c>
@@ -45376,8 +45432,11 @@
         <v>955</v>
       </c>
       <c r="P234" s="1"/>
-    </row>
-    <row r="235" spans="1:16">
+      <c r="S234" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="235" spans="1:19">
       <c r="A235">
         <v>1045</v>
       </c>
@@ -45415,8 +45474,11 @@
         <v>955</v>
       </c>
       <c r="P235" s="1"/>
-    </row>
-    <row r="236" spans="1:16">
+      <c r="S235" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="236" spans="1:19">
       <c r="A236">
         <v>1046</v>
       </c>
@@ -45454,8 +45516,11 @@
         <v>955</v>
       </c>
       <c r="P236" s="1"/>
-    </row>
-    <row r="237" spans="1:16">
+      <c r="S236" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="237" spans="1:19">
       <c r="A237">
         <v>1047</v>
       </c>
@@ -45493,8 +45558,11 @@
         <v>955</v>
       </c>
       <c r="P237" s="1"/>
-    </row>
-    <row r="238" spans="1:16">
+      <c r="S237" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="238" spans="1:19">
       <c r="A238">
         <v>1048</v>
       </c>
@@ -45532,8 +45600,11 @@
         <v>955</v>
       </c>
       <c r="P238" s="1"/>
-    </row>
-    <row r="239" spans="1:16">
+      <c r="S238" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="239" spans="1:19">
       <c r="A239">
         <v>1049</v>
       </c>
@@ -45571,8 +45642,11 @@
         <v>955</v>
       </c>
       <c r="P239" s="1"/>
-    </row>
-    <row r="240" spans="1:16">
+      <c r="S239" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="240" spans="1:19">
       <c r="A240">
         <v>1050</v>
       </c>
@@ -45610,6 +45684,9 @@
         <v>955</v>
       </c>
       <c r="P240" s="1"/>
+      <c r="S240" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="241" spans="1:19">
       <c r="A241">
@@ -45649,6 +45726,9 @@
         <v>955</v>
       </c>
       <c r="P241" s="1"/>
+      <c r="S241" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="242" spans="1:19">
       <c r="A242">
@@ -45691,6 +45771,9 @@
         <v>955</v>
       </c>
       <c r="P242" s="1"/>
+      <c r="S242" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="243" spans="1:19">
       <c r="A243">
@@ -45733,6 +45816,9 @@
         <v>955</v>
       </c>
       <c r="P243" s="1"/>
+      <c r="S243" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="244" spans="1:19">
       <c r="A244">
@@ -46899,7 +46985,7 @@
       </c>
       <c r="P272" s="1"/>
     </row>
-    <row r="273" spans="1:18">
+    <row r="273" spans="1:19">
       <c r="A273">
         <v>1083</v>
       </c>
@@ -46938,7 +47024,7 @@
       </c>
       <c r="P273" s="1"/>
     </row>
-    <row r="274" spans="1:18">
+    <row r="274" spans="1:19">
       <c r="A274">
         <v>1084</v>
       </c>
@@ -46973,7 +47059,7 @@
       </c>
       <c r="P274" s="1"/>
     </row>
-    <row r="275" spans="1:18">
+    <row r="275" spans="1:19">
       <c r="A275">
         <v>1085</v>
       </c>
@@ -47008,7 +47094,7 @@
       </c>
       <c r="P275" s="1"/>
     </row>
-    <row r="276" spans="1:18">
+    <row r="276" spans="1:19">
       <c r="A276">
         <v>1086</v>
       </c>
@@ -47052,7 +47138,7 @@
         <v>2143</v>
       </c>
     </row>
-    <row r="277" spans="1:18">
+    <row r="277" spans="1:19">
       <c r="A277">
         <v>1087</v>
       </c>
@@ -47085,7 +47171,7 @@
       </c>
       <c r="P277" s="1"/>
     </row>
-    <row r="278" spans="1:18">
+    <row r="278" spans="1:19">
       <c r="A278">
         <v>1088</v>
       </c>
@@ -47129,7 +47215,7 @@
         <v>2143</v>
       </c>
     </row>
-    <row r="279" spans="1:18">
+    <row r="279" spans="1:19">
       <c r="A279">
         <v>1089</v>
       </c>
@@ -47162,7 +47248,7 @@
       </c>
       <c r="P279" s="1"/>
     </row>
-    <row r="280" spans="1:18">
+    <row r="280" spans="1:19">
       <c r="A280">
         <v>1090</v>
       </c>
@@ -47207,7 +47293,7 @@
         <v>2143</v>
       </c>
     </row>
-    <row r="281" spans="1:18">
+    <row r="281" spans="1:19">
       <c r="A281">
         <v>1091</v>
       </c>
@@ -47240,7 +47326,7 @@
       </c>
       <c r="P281" s="1"/>
     </row>
-    <row r="282" spans="1:18">
+    <row r="282" spans="1:19">
       <c r="A282">
         <v>1092</v>
       </c>
@@ -47284,7 +47370,7 @@
         <v>2143</v>
       </c>
     </row>
-    <row r="283" spans="1:18">
+    <row r="283" spans="1:19">
       <c r="A283">
         <v>1093</v>
       </c>
@@ -47317,7 +47403,7 @@
       </c>
       <c r="P283" s="1"/>
     </row>
-    <row r="284" spans="1:18">
+    <row r="284" spans="1:19">
       <c r="A284">
         <v>1094</v>
       </c>
@@ -47358,8 +47444,11 @@
         <v>955</v>
       </c>
       <c r="P284" s="1"/>
-    </row>
-    <row r="285" spans="1:18">
+      <c r="S284" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="285" spans="1:19">
       <c r="A285">
         <v>1095</v>
       </c>
@@ -47400,8 +47489,11 @@
         <v>955</v>
       </c>
       <c r="P285" s="1"/>
-    </row>
-    <row r="286" spans="1:18">
+      <c r="S285" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="286" spans="1:19">
       <c r="A286">
         <v>1096</v>
       </c>
@@ -47442,8 +47534,11 @@
         <v>955</v>
       </c>
       <c r="P286" s="1"/>
-    </row>
-    <row r="287" spans="1:18">
+      <c r="S286" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="287" spans="1:19">
       <c r="A287">
         <v>1097</v>
       </c>
@@ -47484,8 +47579,11 @@
         <v>955</v>
       </c>
       <c r="P287" s="1"/>
-    </row>
-    <row r="288" spans="1:18">
+      <c r="S287" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="288" spans="1:19">
       <c r="A288">
         <v>1098</v>
       </c>
@@ -47526,8 +47624,11 @@
         <v>955</v>
       </c>
       <c r="P288" s="1"/>
-    </row>
-    <row r="289" spans="1:16">
+      <c r="S288" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="289" spans="1:19">
       <c r="A289">
         <v>1099</v>
       </c>
@@ -47568,8 +47669,11 @@
         <v>955</v>
       </c>
       <c r="P289" s="1"/>
-    </row>
-    <row r="290" spans="1:16">
+      <c r="S289" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="290" spans="1:19">
       <c r="A290">
         <v>1100</v>
       </c>
@@ -47611,7 +47715,7 @@
       </c>
       <c r="P290" s="1"/>
     </row>
-    <row r="291" spans="1:16">
+    <row r="291" spans="1:19">
       <c r="A291">
         <v>1101</v>
       </c>
@@ -47653,7 +47757,7 @@
       </c>
       <c r="P291" s="1"/>
     </row>
-    <row r="292" spans="1:16">
+    <row r="292" spans="1:19">
       <c r="A292">
         <v>1102</v>
       </c>
@@ -47695,7 +47799,7 @@
       </c>
       <c r="P292" s="1"/>
     </row>
-    <row r="293" spans="1:16">
+    <row r="293" spans="1:19">
       <c r="A293">
         <v>1103</v>
       </c>
@@ -47737,7 +47841,7 @@
       </c>
       <c r="P293" s="1"/>
     </row>
-    <row r="294" spans="1:16">
+    <row r="294" spans="1:19">
       <c r="A294">
         <v>1104</v>
       </c>
@@ -47779,7 +47883,7 @@
       </c>
       <c r="P294" s="1"/>
     </row>
-    <row r="295" spans="1:16">
+    <row r="295" spans="1:19">
       <c r="A295">
         <v>1105</v>
       </c>
@@ -47821,7 +47925,7 @@
       </c>
       <c r="P295" s="1"/>
     </row>
-    <row r="296" spans="1:16">
+    <row r="296" spans="1:19">
       <c r="A296">
         <v>1106</v>
       </c>
@@ -47860,7 +47964,7 @@
       </c>
       <c r="P296" s="1"/>
     </row>
-    <row r="297" spans="1:16">
+    <row r="297" spans="1:19">
       <c r="A297">
         <v>1107</v>
       </c>
@@ -47899,7 +48003,7 @@
       </c>
       <c r="P297" s="1"/>
     </row>
-    <row r="298" spans="1:16">
+    <row r="298" spans="1:19">
       <c r="A298">
         <v>1108</v>
       </c>
@@ -47938,7 +48042,7 @@
       </c>
       <c r="P298" s="1"/>
     </row>
-    <row r="299" spans="1:16">
+    <row r="299" spans="1:19">
       <c r="A299">
         <v>1109</v>
       </c>
@@ -47977,7 +48081,7 @@
       </c>
       <c r="P299" s="1"/>
     </row>
-    <row r="300" spans="1:16">
+    <row r="300" spans="1:19">
       <c r="A300">
         <v>1110</v>
       </c>
@@ -48016,7 +48120,7 @@
       </c>
       <c r="P300" s="1"/>
     </row>
-    <row r="301" spans="1:16">
+    <row r="301" spans="1:19">
       <c r="A301">
         <v>1111</v>
       </c>
@@ -48055,7 +48159,7 @@
       </c>
       <c r="P301" s="1"/>
     </row>
-    <row r="302" spans="1:16">
+    <row r="302" spans="1:19">
       <c r="A302">
         <v>1112</v>
       </c>
@@ -48094,7 +48198,7 @@
       </c>
       <c r="P302" s="1"/>
     </row>
-    <row r="303" spans="1:16">
+    <row r="303" spans="1:19">
       <c r="A303">
         <v>1113</v>
       </c>
@@ -48133,7 +48237,7 @@
       </c>
       <c r="P303" s="1"/>
     </row>
-    <row r="304" spans="1:16">
+    <row r="304" spans="1:19">
       <c r="A304">
         <v>1114</v>
       </c>
@@ -48792,7 +48896,7 @@
         <v>35</v>
       </c>
       <c r="M320" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N320" s="1" t="s">
         <v>1569</v>
@@ -48834,7 +48938,7 @@
         <v>35</v>
       </c>
       <c r="M321" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N321" s="1" t="s">
         <v>1569</v>
@@ -48876,7 +48980,7 @@
         <v>35</v>
       </c>
       <c r="M322" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N322" s="1" t="s">
         <v>1569</v>
@@ -48918,7 +49022,7 @@
         <v>35</v>
       </c>
       <c r="M323" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N323" s="1" t="s">
         <v>1569</v>
@@ -48960,7 +49064,7 @@
         <v>35</v>
       </c>
       <c r="M324" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N324" s="1" t="s">
         <v>1569</v>
@@ -49002,7 +49106,7 @@
         <v>35</v>
       </c>
       <c r="M325" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N325" s="1" t="s">
         <v>1569</v>
@@ -49044,7 +49148,7 @@
         <v>35</v>
       </c>
       <c r="M326" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N326" s="1" t="s">
         <v>1569</v>
@@ -49086,7 +49190,7 @@
         <v>35</v>
       </c>
       <c r="M327" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N327" s="1" t="s">
         <v>1569</v>
@@ -49128,7 +49232,7 @@
         <v>35</v>
       </c>
       <c r="M328" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N328" s="1" t="s">
         <v>1569</v>
@@ -49170,7 +49274,7 @@
         <v>35</v>
       </c>
       <c r="M329" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N329" s="1" t="s">
         <v>1569</v>
@@ -49212,7 +49316,7 @@
         <v>35</v>
       </c>
       <c r="M330" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N330" s="1" t="s">
         <v>1569</v>
@@ -49254,7 +49358,7 @@
         <v>35</v>
       </c>
       <c r="M331" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N331" s="1" t="s">
         <v>1569</v>
@@ -49296,7 +49400,7 @@
         <v>35</v>
       </c>
       <c r="M332" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N332" s="1" t="s">
         <v>1569</v>
@@ -49338,7 +49442,7 @@
         <v>35</v>
       </c>
       <c r="M333" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N333" s="1" t="s">
         <v>1569</v>
@@ -49380,7 +49484,7 @@
         <v>35</v>
       </c>
       <c r="M334" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N334" s="1" t="s">
         <v>1569</v>
@@ -49422,7 +49526,7 @@
         <v>35</v>
       </c>
       <c r="M335" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N335" s="1" t="s">
         <v>1569</v>
@@ -49471,7 +49575,7 @@
       </c>
       <c r="P336" s="1"/>
     </row>
-    <row r="337" spans="1:16">
+    <row r="337" spans="1:19">
       <c r="A337">
         <v>1147</v>
       </c>
@@ -49513,7 +49617,7 @@
       </c>
       <c r="P337" s="1"/>
     </row>
-    <row r="338" spans="1:16">
+    <row r="338" spans="1:19">
       <c r="A338">
         <v>1148</v>
       </c>
@@ -49548,7 +49652,7 @@
       </c>
       <c r="P338" s="1"/>
     </row>
-    <row r="339" spans="1:16">
+    <row r="339" spans="1:19">
       <c r="A339">
         <v>1149</v>
       </c>
@@ -49590,7 +49694,7 @@
       </c>
       <c r="P339" s="1"/>
     </row>
-    <row r="340" spans="1:16">
+    <row r="340" spans="1:19">
       <c r="A340">
         <v>1150</v>
       </c>
@@ -49632,7 +49736,7 @@
       </c>
       <c r="P340" s="1"/>
     </row>
-    <row r="341" spans="1:16">
+    <row r="341" spans="1:19">
       <c r="A341">
         <v>1151</v>
       </c>
@@ -49667,7 +49771,7 @@
       </c>
       <c r="P341" s="1"/>
     </row>
-    <row r="342" spans="1:16">
+    <row r="342" spans="1:19">
       <c r="A342">
         <v>1152</v>
       </c>
@@ -49702,7 +49806,7 @@
       </c>
       <c r="P342" s="1"/>
     </row>
-    <row r="343" spans="1:16">
+    <row r="343" spans="1:19">
       <c r="A343">
         <v>1153</v>
       </c>
@@ -49737,7 +49841,7 @@
       </c>
       <c r="P343" s="1"/>
     </row>
-    <row r="344" spans="1:16">
+    <row r="344" spans="1:19">
       <c r="A344">
         <v>1154</v>
       </c>
@@ -49772,7 +49876,7 @@
       </c>
       <c r="P344" s="1"/>
     </row>
-    <row r="345" spans="1:16">
+    <row r="345" spans="1:19">
       <c r="A345">
         <v>1155</v>
       </c>
@@ -49807,7 +49911,7 @@
       </c>
       <c r="P345" s="1"/>
     </row>
-    <row r="346" spans="1:16">
+    <row r="346" spans="1:19">
       <c r="A346">
         <v>1156</v>
       </c>
@@ -49846,7 +49950,7 @@
       </c>
       <c r="P346" s="1"/>
     </row>
-    <row r="347" spans="1:16">
+    <row r="347" spans="1:19">
       <c r="A347">
         <v>1157</v>
       </c>
@@ -49884,8 +49988,11 @@
         <v>955</v>
       </c>
       <c r="P347" s="1"/>
-    </row>
-    <row r="348" spans="1:16">
+      <c r="S347" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="348" spans="1:19">
       <c r="A348">
         <v>1158</v>
       </c>
@@ -49923,8 +50030,11 @@
         <v>955</v>
       </c>
       <c r="P348" s="1"/>
-    </row>
-    <row r="349" spans="1:16">
+      <c r="S348" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="349" spans="1:19">
       <c r="A349">
         <v>1159</v>
       </c>
@@ -49965,8 +50075,11 @@
         <v>955</v>
       </c>
       <c r="P349" s="1"/>
-    </row>
-    <row r="350" spans="1:16">
+      <c r="S349" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="350" spans="1:19">
       <c r="A350">
         <v>1160</v>
       </c>
@@ -49999,7 +50112,7 @@
       </c>
       <c r="P350" s="1"/>
     </row>
-    <row r="351" spans="1:16">
+    <row r="351" spans="1:19">
       <c r="A351">
         <v>1161</v>
       </c>
@@ -50032,7 +50145,7 @@
       </c>
       <c r="P351" s="1"/>
     </row>
-    <row r="352" spans="1:16">
+    <row r="352" spans="1:19">
       <c r="A352">
         <v>1162</v>
       </c>
@@ -50145,6 +50258,9 @@
         <v>955</v>
       </c>
       <c r="P354" s="1"/>
+      <c r="S354" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="355" spans="1:19">
       <c r="A355">
@@ -50187,6 +50303,9 @@
         <v>955</v>
       </c>
       <c r="P355" s="1"/>
+      <c r="S355" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="356" spans="1:19">
       <c r="A356">
@@ -50229,6 +50348,9 @@
         <v>955</v>
       </c>
       <c r="P356" s="1"/>
+      <c r="S356" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="357" spans="1:19">
       <c r="A357">
@@ -54194,7 +54316,7 @@
         <v>35</v>
       </c>
       <c r="M78" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N78" s="1" t="s">
         <v>1569</v>
@@ -54236,7 +54358,7 @@
         <v>35</v>
       </c>
       <c r="M79" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N79" s="1" t="s">
         <v>1569</v>
@@ -54278,7 +54400,7 @@
         <v>35</v>
       </c>
       <c r="M80" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N80" s="1" t="s">
         <v>1569</v>
@@ -54320,7 +54442,7 @@
         <v>35</v>
       </c>
       <c r="M81" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N81" s="1" t="s">
         <v>1569</v>
@@ -54362,7 +54484,7 @@
         <v>35</v>
       </c>
       <c r="M82" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N82" s="1" t="s">
         <v>1569</v>
@@ -54404,7 +54526,7 @@
         <v>35</v>
       </c>
       <c r="M83" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N83" s="1" t="s">
         <v>1569</v>
@@ -54446,7 +54568,7 @@
         <v>35</v>
       </c>
       <c r="M84" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N84" s="1" t="s">
         <v>1569</v>
@@ -54488,7 +54610,7 @@
         <v>35</v>
       </c>
       <c r="M85" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N85" s="1" t="s">
         <v>1569</v>
@@ -54530,7 +54652,7 @@
         <v>35</v>
       </c>
       <c r="M86" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N86" s="1" t="s">
         <v>1569</v>
@@ -54572,7 +54694,7 @@
         <v>35</v>
       </c>
       <c r="M87" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N87" s="1" t="s">
         <v>1569</v>
@@ -54614,7 +54736,7 @@
         <v>35</v>
       </c>
       <c r="M88" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N88" s="1" t="s">
         <v>1569</v>
@@ -54656,7 +54778,7 @@
         <v>35</v>
       </c>
       <c r="M89" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N89" s="1" t="s">
         <v>1569</v>
@@ -54698,7 +54820,7 @@
         <v>35</v>
       </c>
       <c r="M90" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N90" s="1" t="s">
         <v>1569</v>
@@ -54740,7 +54862,7 @@
         <v>35</v>
       </c>
       <c r="M91" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N91" s="1" t="s">
         <v>1569</v>
@@ -54782,7 +54904,7 @@
         <v>35</v>
       </c>
       <c r="M92" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N92" s="1" t="s">
         <v>1569</v>
@@ -54824,7 +54946,7 @@
         <v>35</v>
       </c>
       <c r="M93" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N93" s="1" t="s">
         <v>1569</v>
@@ -56144,7 +56266,7 @@
         <v>35</v>
       </c>
       <c r="M124" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N124" s="1" t="s">
         <v>1569</v>
@@ -56189,7 +56311,7 @@
         <v>35</v>
       </c>
       <c r="M125" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N125" s="1" t="s">
         <v>1569</v>
@@ -56234,7 +56356,7 @@
         <v>35</v>
       </c>
       <c r="M126" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N126" s="1" t="s">
         <v>1569</v>
@@ -56279,7 +56401,7 @@
         <v>35</v>
       </c>
       <c r="M127" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N127" s="1" t="s">
         <v>1569</v>
@@ -56324,7 +56446,7 @@
         <v>35</v>
       </c>
       <c r="M128" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N128" s="1" t="s">
         <v>1569</v>
@@ -56369,7 +56491,7 @@
         <v>35</v>
       </c>
       <c r="M129" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N129" s="1" t="s">
         <v>1569</v>
@@ -56414,7 +56536,7 @@
         <v>35</v>
       </c>
       <c r="M130" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N130" s="1" t="s">
         <v>1569</v>
@@ -56459,7 +56581,7 @@
         <v>35</v>
       </c>
       <c r="M131" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N131" s="1" t="s">
         <v>1569</v>
@@ -56504,7 +56626,7 @@
         <v>35</v>
       </c>
       <c r="M132" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N132" s="1" t="s">
         <v>1569</v>
@@ -56549,7 +56671,7 @@
         <v>35</v>
       </c>
       <c r="M133" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N133" s="1" t="s">
         <v>1569</v>
@@ -56594,7 +56716,7 @@
         <v>35</v>
       </c>
       <c r="M134" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N134" s="1" t="s">
         <v>1569</v>
@@ -56639,7 +56761,7 @@
         <v>35</v>
       </c>
       <c r="M135" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N135" s="1" t="s">
         <v>1569</v>
@@ -56684,7 +56806,7 @@
         <v>35</v>
       </c>
       <c r="M136" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N136" s="1" t="s">
         <v>1569</v>
@@ -56729,7 +56851,7 @@
         <v>35</v>
       </c>
       <c r="M137" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N137" s="1" t="s">
         <v>1569</v>
@@ -56774,7 +56896,7 @@
         <v>35</v>
       </c>
       <c r="M138" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N138" s="1" t="s">
         <v>1569</v>
@@ -56819,7 +56941,7 @@
         <v>35</v>
       </c>
       <c r="M139" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="N139" s="1" t="s">
         <v>1569</v>
@@ -62497,6 +62619,9 @@
         <v>955</v>
       </c>
       <c r="P267" s="1"/>
+      <c r="S267" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="268" spans="1:19">
       <c r="A268">
@@ -62536,6 +62661,9 @@
         <v>955</v>
       </c>
       <c r="P268" s="1"/>
+      <c r="S268" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="269" spans="1:19">
       <c r="A269">
@@ -63984,7 +64112,7 @@
         <v>2143</v>
       </c>
     </row>
-    <row r="305" spans="1:16">
+    <row r="305" spans="1:19">
       <c r="A305">
         <v>753</v>
       </c>
@@ -64019,7 +64147,7 @@
       </c>
       <c r="P305" s="1"/>
     </row>
-    <row r="306" spans="1:16">
+    <row r="306" spans="1:19">
       <c r="A306">
         <v>754</v>
       </c>
@@ -64060,8 +64188,11 @@
         <v>955</v>
       </c>
       <c r="P306" s="1"/>
-    </row>
-    <row r="307" spans="1:16">
+      <c r="S306" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="307" spans="1:19">
       <c r="A307">
         <v>755</v>
       </c>
@@ -64102,8 +64233,11 @@
         <v>955</v>
       </c>
       <c r="P307" s="1"/>
-    </row>
-    <row r="308" spans="1:16">
+      <c r="S307" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="308" spans="1:19">
       <c r="A308">
         <v>756</v>
       </c>
@@ -64145,7 +64279,7 @@
       </c>
       <c r="P308" s="1"/>
     </row>
-    <row r="309" spans="1:16">
+    <row r="309" spans="1:19">
       <c r="A309">
         <v>757</v>
       </c>
@@ -64187,7 +64321,7 @@
       </c>
       <c r="P309" s="1"/>
     </row>
-    <row r="310" spans="1:16">
+    <row r="310" spans="1:19">
       <c r="A310">
         <v>758</v>
       </c>
@@ -64222,7 +64356,7 @@
       </c>
       <c r="P310" s="1"/>
     </row>
-    <row r="311" spans="1:16">
+    <row r="311" spans="1:19">
       <c r="A311">
         <v>759</v>
       </c>
@@ -64264,7 +64398,7 @@
       </c>
       <c r="P311" s="1"/>
     </row>
-    <row r="312" spans="1:16">
+    <row r="312" spans="1:19">
       <c r="A312">
         <v>760</v>
       </c>
@@ -64306,7 +64440,7 @@
       </c>
       <c r="P312" s="1"/>
     </row>
-    <row r="313" spans="1:16">
+    <row r="313" spans="1:19">
       <c r="A313">
         <v>761</v>
       </c>
@@ -64341,7 +64475,7 @@
       </c>
       <c r="P313" s="1"/>
     </row>
-    <row r="314" spans="1:16">
+    <row r="314" spans="1:19">
       <c r="A314">
         <v>762</v>
       </c>
@@ -64376,7 +64510,7 @@
       </c>
       <c r="P314" s="1"/>
     </row>
-    <row r="315" spans="1:16">
+    <row r="315" spans="1:19">
       <c r="A315">
         <v>763</v>
       </c>
@@ -64411,7 +64545,7 @@
       </c>
       <c r="P315" s="1"/>
     </row>
-    <row r="316" spans="1:16">
+    <row r="316" spans="1:19">
       <c r="A316">
         <v>764</v>
       </c>
@@ -64446,7 +64580,7 @@
       </c>
       <c r="P316" s="1"/>
     </row>
-    <row r="317" spans="1:16">
+    <row r="317" spans="1:19">
       <c r="A317">
         <v>765</v>
       </c>
@@ -64481,7 +64615,7 @@
       </c>
       <c r="P317" s="1"/>
     </row>
-    <row r="318" spans="1:16">
+    <row r="318" spans="1:19">
       <c r="A318">
         <v>766</v>
       </c>
@@ -64520,7 +64654,7 @@
       </c>
       <c r="P318" s="1"/>
     </row>
-    <row r="319" spans="1:16">
+    <row r="319" spans="1:19">
       <c r="A319">
         <v>767</v>
       </c>
@@ -64559,7 +64693,7 @@
       </c>
       <c r="P319" s="1"/>
     </row>
-    <row r="320" spans="1:16">
+    <row r="320" spans="1:19">
       <c r="A320">
         <v>768</v>
       </c>
@@ -64597,8 +64731,11 @@
         <v>955</v>
       </c>
       <c r="P320" s="1"/>
-    </row>
-    <row r="321" spans="1:16">
+      <c r="S320" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="321" spans="1:19">
       <c r="A321">
         <v>769</v>
       </c>
@@ -64639,8 +64776,11 @@
         <v>955</v>
       </c>
       <c r="P321" s="1"/>
-    </row>
-    <row r="322" spans="1:16">
+      <c r="S321" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="322" spans="1:19">
       <c r="A322">
         <v>770</v>
       </c>
@@ -64681,8 +64821,11 @@
         <v>955</v>
       </c>
       <c r="P322" s="1"/>
-    </row>
-    <row r="323" spans="1:16">
+      <c r="S322" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="323" spans="1:19">
       <c r="A323">
         <v>771</v>
       </c>
@@ -64723,8 +64866,11 @@
         <v>955</v>
       </c>
       <c r="P323" s="1"/>
-    </row>
-    <row r="324" spans="1:16">
+      <c r="S323" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="324" spans="1:19">
       <c r="A324">
         <v>772</v>
       </c>
@@ -64765,8 +64911,11 @@
         <v>955</v>
       </c>
       <c r="P324" s="1"/>
-    </row>
-    <row r="325" spans="1:16">
+      <c r="S324" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="325" spans="1:19">
       <c r="A325">
         <v>773</v>
       </c>
@@ -64804,8 +64953,11 @@
         <v>955</v>
       </c>
       <c r="P325" s="1"/>
-    </row>
-    <row r="326" spans="1:16">
+      <c r="S325" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="326" spans="1:19">
       <c r="A326">
         <v>774</v>
       </c>
@@ -64843,8 +64995,11 @@
         <v>955</v>
       </c>
       <c r="P326" s="1"/>
-    </row>
-    <row r="327" spans="1:16">
+      <c r="S326" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="327" spans="1:19">
       <c r="A327">
         <v>775</v>
       </c>
@@ -64882,8 +65037,11 @@
         <v>955</v>
       </c>
       <c r="P327" s="1"/>
-    </row>
-    <row r="328" spans="1:16">
+      <c r="S327" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="328" spans="1:19">
       <c r="A328">
         <v>776</v>
       </c>
@@ -64921,8 +65079,11 @@
         <v>955</v>
       </c>
       <c r="P328" s="1"/>
-    </row>
-    <row r="329" spans="1:16">
+      <c r="S328" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="329" spans="1:19">
       <c r="A329">
         <v>777</v>
       </c>
@@ -64960,8 +65121,11 @@
         <v>955</v>
       </c>
       <c r="P329" s="1"/>
-    </row>
-    <row r="330" spans="1:16">
+      <c r="S329" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="330" spans="1:19">
       <c r="A330">
         <v>778</v>
       </c>
@@ -64999,8 +65163,11 @@
         <v>955</v>
       </c>
       <c r="P330" s="1"/>
-    </row>
-    <row r="331" spans="1:16">
+      <c r="S330" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="331" spans="1:19">
       <c r="A331">
         <v>779</v>
       </c>
@@ -65038,8 +65205,11 @@
         <v>955</v>
       </c>
       <c r="P331" s="1"/>
-    </row>
-    <row r="332" spans="1:16">
+      <c r="S331" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="332" spans="1:19">
       <c r="A332">
         <v>780</v>
       </c>
@@ -65077,8 +65247,11 @@
         <v>955</v>
       </c>
       <c r="P332" s="1"/>
-    </row>
-    <row r="333" spans="1:16">
+      <c r="S332" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="333" spans="1:19">
       <c r="A333">
         <v>781</v>
       </c>
@@ -65116,8 +65289,11 @@
         <v>955</v>
       </c>
       <c r="P333" s="1"/>
-    </row>
-    <row r="334" spans="1:16">
+      <c r="S333" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="334" spans="1:19">
       <c r="A334">
         <v>782</v>
       </c>
@@ -65155,8 +65331,11 @@
         <v>955</v>
       </c>
       <c r="P334" s="1"/>
-    </row>
-    <row r="335" spans="1:16">
+      <c r="S334" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="335" spans="1:19">
       <c r="A335">
         <v>783</v>
       </c>
@@ -65197,8 +65376,11 @@
         <v>955</v>
       </c>
       <c r="P335" s="1"/>
-    </row>
-    <row r="336" spans="1:16">
+      <c r="S335" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="336" spans="1:19">
       <c r="A336">
         <v>784</v>
       </c>
@@ -65239,8 +65421,11 @@
         <v>955</v>
       </c>
       <c r="P336" s="1"/>
-    </row>
-    <row r="337" spans="1:16">
+      <c r="S336" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="337" spans="1:19">
       <c r="A337">
         <v>785</v>
       </c>
@@ -65279,7 +65464,7 @@
       </c>
       <c r="P337" s="1"/>
     </row>
-    <row r="338" spans="1:16">
+    <row r="338" spans="1:19">
       <c r="A338">
         <v>786</v>
       </c>
@@ -65314,7 +65499,7 @@
       </c>
       <c r="P338" s="1"/>
     </row>
-    <row r="339" spans="1:16">
+    <row r="339" spans="1:19">
       <c r="A339">
         <v>787</v>
       </c>
@@ -65349,7 +65534,7 @@
       </c>
       <c r="P339" s="1"/>
     </row>
-    <row r="340" spans="1:16">
+    <row r="340" spans="1:19">
       <c r="A340">
         <v>788</v>
       </c>
@@ -65384,7 +65569,7 @@
       </c>
       <c r="P340" s="1"/>
     </row>
-    <row r="341" spans="1:16">
+    <row r="341" spans="1:19">
       <c r="A341">
         <v>789</v>
       </c>
@@ -65419,7 +65604,7 @@
       </c>
       <c r="P341" s="1"/>
     </row>
-    <row r="342" spans="1:16">
+    <row r="342" spans="1:19">
       <c r="A342">
         <v>790</v>
       </c>
@@ -65457,8 +65642,11 @@
         <v>955</v>
       </c>
       <c r="P342" s="1"/>
-    </row>
-    <row r="343" spans="1:16">
+      <c r="S342" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="343" spans="1:19">
       <c r="A343">
         <v>791</v>
       </c>
@@ -65496,8 +65684,11 @@
         <v>955</v>
       </c>
       <c r="P343" s="1"/>
-    </row>
-    <row r="344" spans="1:16">
+      <c r="S343" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="344" spans="1:19">
       <c r="A344">
         <v>792</v>
       </c>
@@ -65535,8 +65726,11 @@
         <v>955</v>
       </c>
       <c r="P344" s="1"/>
-    </row>
-    <row r="345" spans="1:16">
+      <c r="S344" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="345" spans="1:19">
       <c r="A345">
         <v>793</v>
       </c>
@@ -65574,8 +65768,11 @@
         <v>955</v>
       </c>
       <c r="P345" s="1"/>
-    </row>
-    <row r="346" spans="1:16">
+      <c r="S345" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="346" spans="1:19">
       <c r="A346">
         <v>794</v>
       </c>
@@ -65616,8 +65813,11 @@
         <v>955</v>
       </c>
       <c r="P346" s="1"/>
-    </row>
-    <row r="347" spans="1:16">
+      <c r="S346" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="347" spans="1:19">
       <c r="A347">
         <v>795</v>
       </c>
@@ -65655,8 +65855,11 @@
         <v>955</v>
       </c>
       <c r="P347" s="1"/>
-    </row>
-    <row r="348" spans="1:16">
+      <c r="S347" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="348" spans="1:19">
       <c r="A348">
         <v>796</v>
       </c>
@@ -65695,7 +65898,7 @@
       </c>
       <c r="P348" s="1"/>
     </row>
-    <row r="349" spans="1:16">
+    <row r="349" spans="1:19">
       <c r="A349">
         <v>797</v>
       </c>
@@ -65734,7 +65937,7 @@
       </c>
       <c r="P349" s="1"/>
     </row>
-    <row r="350" spans="1:16">
+    <row r="350" spans="1:19">
       <c r="A350">
         <v>798</v>
       </c>
@@ -65776,7 +65979,7 @@
       </c>
       <c r="P350" s="1"/>
     </row>
-    <row r="351" spans="1:16">
+    <row r="351" spans="1:19">
       <c r="A351">
         <v>799</v>
       </c>
@@ -65818,7 +66021,7 @@
       </c>
       <c r="P351" s="1"/>
     </row>
-    <row r="352" spans="1:16">
+    <row r="352" spans="1:19">
       <c r="A352">
         <v>800</v>
       </c>

</xml_diff>

<commit_message>
regenerate dd with national flagging updates
</commit_message>
<xml_diff>
--- a/input/images/IJE_File_Layouts_and_FHIR_Mapping_24-06-21.xlsx
+++ b/input/images/IJE_File_Layouts_and_FHIR_Mapping_24-06-21.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12836" uniqueCount="2788">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12784" uniqueCount="2788">
   <si>
     <t>This content was derived from the file IJE_File_Layouts_Version_2021_FHIR* and is automatically generated from the source file IJE_File_Layouts_and_FHIR_Mapping_24-06-21.csv.
 The CSV version of the file is used to drive the content of narrative generated for the Vital Records Implementation Guides (VRDR, BFDR, and VRCL).
@@ -13701,9 +13701,6 @@
       </c>
       <c r="N91" s="1"/>
       <c r="P91" s="1"/>
-      <c r="S91" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="92" spans="1:19">
       <c r="A92">
@@ -45036,7 +45033,7 @@
       </c>
       <c r="P224" s="1"/>
     </row>
-    <row r="225" spans="1:19">
+    <row r="225" spans="1:16">
       <c r="A225">
         <v>1035</v>
       </c>
@@ -45071,7 +45068,7 @@
       </c>
       <c r="P225" s="1"/>
     </row>
-    <row r="226" spans="1:19">
+    <row r="226" spans="1:16">
       <c r="A226">
         <v>1036</v>
       </c>
@@ -45113,7 +45110,7 @@
       </c>
       <c r="P226" s="1"/>
     </row>
-    <row r="227" spans="1:19">
+    <row r="227" spans="1:16">
       <c r="A227">
         <v>1037</v>
       </c>
@@ -45155,7 +45152,7 @@
       </c>
       <c r="P227" s="1"/>
     </row>
-    <row r="228" spans="1:19">
+    <row r="228" spans="1:16">
       <c r="A228">
         <v>1038</v>
       </c>
@@ -45197,7 +45194,7 @@
       </c>
       <c r="P228" s="1"/>
     </row>
-    <row r="229" spans="1:19">
+    <row r="229" spans="1:16">
       <c r="A229">
         <v>1039</v>
       </c>
@@ -45236,7 +45233,7 @@
       </c>
       <c r="P229" s="1"/>
     </row>
-    <row r="230" spans="1:19">
+    <row r="230" spans="1:16">
       <c r="A230">
         <v>1040</v>
       </c>
@@ -45271,7 +45268,7 @@
       </c>
       <c r="P230" s="1"/>
     </row>
-    <row r="231" spans="1:19">
+    <row r="231" spans="1:16">
       <c r="A231">
         <v>1041</v>
       </c>
@@ -45310,7 +45307,7 @@
       </c>
       <c r="P231" s="1"/>
     </row>
-    <row r="232" spans="1:19">
+    <row r="232" spans="1:16">
       <c r="A232">
         <v>1042</v>
       </c>
@@ -45348,11 +45345,8 @@
         <v>955</v>
       </c>
       <c r="P232" s="1"/>
-      <c r="S232" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="233" spans="1:19">
+    </row>
+    <row r="233" spans="1:16">
       <c r="A233">
         <v>1043</v>
       </c>
@@ -45390,11 +45384,8 @@
         <v>955</v>
       </c>
       <c r="P233" s="1"/>
-      <c r="S233" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="234" spans="1:19">
+    </row>
+    <row r="234" spans="1:16">
       <c r="A234">
         <v>1044</v>
       </c>
@@ -45432,11 +45423,8 @@
         <v>955</v>
       </c>
       <c r="P234" s="1"/>
-      <c r="S234" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="235" spans="1:19">
+    </row>
+    <row r="235" spans="1:16">
       <c r="A235">
         <v>1045</v>
       </c>
@@ -45474,11 +45462,8 @@
         <v>955</v>
       </c>
       <c r="P235" s="1"/>
-      <c r="S235" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="236" spans="1:19">
+    </row>
+    <row r="236" spans="1:16">
       <c r="A236">
         <v>1046</v>
       </c>
@@ -45516,11 +45501,8 @@
         <v>955</v>
       </c>
       <c r="P236" s="1"/>
-      <c r="S236" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="237" spans="1:19">
+    </row>
+    <row r="237" spans="1:16">
       <c r="A237">
         <v>1047</v>
       </c>
@@ -45558,11 +45540,8 @@
         <v>955</v>
       </c>
       <c r="P237" s="1"/>
-      <c r="S237" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="238" spans="1:19">
+    </row>
+    <row r="238" spans="1:16">
       <c r="A238">
         <v>1048</v>
       </c>
@@ -45600,11 +45579,8 @@
         <v>955</v>
       </c>
       <c r="P238" s="1"/>
-      <c r="S238" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="239" spans="1:19">
+    </row>
+    <row r="239" spans="1:16">
       <c r="A239">
         <v>1049</v>
       </c>
@@ -45642,11 +45618,8 @@
         <v>955</v>
       </c>
       <c r="P239" s="1"/>
-      <c r="S239" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="240" spans="1:19">
+    </row>
+    <row r="240" spans="1:16">
       <c r="A240">
         <v>1050</v>
       </c>
@@ -45684,9 +45657,6 @@
         <v>955</v>
       </c>
       <c r="P240" s="1"/>
-      <c r="S240" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="241" spans="1:19">
       <c r="A241">
@@ -45726,9 +45696,6 @@
         <v>955</v>
       </c>
       <c r="P241" s="1"/>
-      <c r="S241" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="242" spans="1:19">
       <c r="A242">
@@ -45771,9 +45738,6 @@
         <v>955</v>
       </c>
       <c r="P242" s="1"/>
-      <c r="S242" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="243" spans="1:19">
       <c r="A243">
@@ -45816,9 +45780,6 @@
         <v>955</v>
       </c>
       <c r="P243" s="1"/>
-      <c r="S243" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="244" spans="1:19">
       <c r="A244">
@@ -46985,7 +46946,7 @@
       </c>
       <c r="P272" s="1"/>
     </row>
-    <row r="273" spans="1:19">
+    <row r="273" spans="1:18">
       <c r="A273">
         <v>1083</v>
       </c>
@@ -47024,7 +46985,7 @@
       </c>
       <c r="P273" s="1"/>
     </row>
-    <row r="274" spans="1:19">
+    <row r="274" spans="1:18">
       <c r="A274">
         <v>1084</v>
       </c>
@@ -47059,7 +47020,7 @@
       </c>
       <c r="P274" s="1"/>
     </row>
-    <row r="275" spans="1:19">
+    <row r="275" spans="1:18">
       <c r="A275">
         <v>1085</v>
       </c>
@@ -47094,7 +47055,7 @@
       </c>
       <c r="P275" s="1"/>
     </row>
-    <row r="276" spans="1:19">
+    <row r="276" spans="1:18">
       <c r="A276">
         <v>1086</v>
       </c>
@@ -47138,7 +47099,7 @@
         <v>2143</v>
       </c>
     </row>
-    <row r="277" spans="1:19">
+    <row r="277" spans="1:18">
       <c r="A277">
         <v>1087</v>
       </c>
@@ -47171,7 +47132,7 @@
       </c>
       <c r="P277" s="1"/>
     </row>
-    <row r="278" spans="1:19">
+    <row r="278" spans="1:18">
       <c r="A278">
         <v>1088</v>
       </c>
@@ -47215,7 +47176,7 @@
         <v>2143</v>
       </c>
     </row>
-    <row r="279" spans="1:19">
+    <row r="279" spans="1:18">
       <c r="A279">
         <v>1089</v>
       </c>
@@ -47248,7 +47209,7 @@
       </c>
       <c r="P279" s="1"/>
     </row>
-    <row r="280" spans="1:19">
+    <row r="280" spans="1:18">
       <c r="A280">
         <v>1090</v>
       </c>
@@ -47293,7 +47254,7 @@
         <v>2143</v>
       </c>
     </row>
-    <row r="281" spans="1:19">
+    <row r="281" spans="1:18">
       <c r="A281">
         <v>1091</v>
       </c>
@@ -47326,7 +47287,7 @@
       </c>
       <c r="P281" s="1"/>
     </row>
-    <row r="282" spans="1:19">
+    <row r="282" spans="1:18">
       <c r="A282">
         <v>1092</v>
       </c>
@@ -47370,7 +47331,7 @@
         <v>2143</v>
       </c>
     </row>
-    <row r="283" spans="1:19">
+    <row r="283" spans="1:18">
       <c r="A283">
         <v>1093</v>
       </c>
@@ -47403,7 +47364,7 @@
       </c>
       <c r="P283" s="1"/>
     </row>
-    <row r="284" spans="1:19">
+    <row r="284" spans="1:18">
       <c r="A284">
         <v>1094</v>
       </c>
@@ -47444,11 +47405,8 @@
         <v>955</v>
       </c>
       <c r="P284" s="1"/>
-      <c r="S284" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="285" spans="1:19">
+    </row>
+    <row r="285" spans="1:18">
       <c r="A285">
         <v>1095</v>
       </c>
@@ -47489,11 +47447,8 @@
         <v>955</v>
       </c>
       <c r="P285" s="1"/>
-      <c r="S285" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="286" spans="1:19">
+    </row>
+    <row r="286" spans="1:18">
       <c r="A286">
         <v>1096</v>
       </c>
@@ -47534,11 +47489,8 @@
         <v>955</v>
       </c>
       <c r="P286" s="1"/>
-      <c r="S286" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="287" spans="1:19">
+    </row>
+    <row r="287" spans="1:18">
       <c r="A287">
         <v>1097</v>
       </c>
@@ -47579,11 +47531,8 @@
         <v>955</v>
       </c>
       <c r="P287" s="1"/>
-      <c r="S287" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="288" spans="1:19">
+    </row>
+    <row r="288" spans="1:18">
       <c r="A288">
         <v>1098</v>
       </c>
@@ -47624,11 +47573,8 @@
         <v>955</v>
       </c>
       <c r="P288" s="1"/>
-      <c r="S288" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="289" spans="1:19">
+    </row>
+    <row r="289" spans="1:16">
       <c r="A289">
         <v>1099</v>
       </c>
@@ -47669,11 +47615,8 @@
         <v>955</v>
       </c>
       <c r="P289" s="1"/>
-      <c r="S289" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="290" spans="1:19">
+    </row>
+    <row r="290" spans="1:16">
       <c r="A290">
         <v>1100</v>
       </c>
@@ -47715,7 +47658,7 @@
       </c>
       <c r="P290" s="1"/>
     </row>
-    <row r="291" spans="1:19">
+    <row r="291" spans="1:16">
       <c r="A291">
         <v>1101</v>
       </c>
@@ -47757,7 +47700,7 @@
       </c>
       <c r="P291" s="1"/>
     </row>
-    <row r="292" spans="1:19">
+    <row r="292" spans="1:16">
       <c r="A292">
         <v>1102</v>
       </c>
@@ -47799,7 +47742,7 @@
       </c>
       <c r="P292" s="1"/>
     </row>
-    <row r="293" spans="1:19">
+    <row r="293" spans="1:16">
       <c r="A293">
         <v>1103</v>
       </c>
@@ -47841,7 +47784,7 @@
       </c>
       <c r="P293" s="1"/>
     </row>
-    <row r="294" spans="1:19">
+    <row r="294" spans="1:16">
       <c r="A294">
         <v>1104</v>
       </c>
@@ -47883,7 +47826,7 @@
       </c>
       <c r="P294" s="1"/>
     </row>
-    <row r="295" spans="1:19">
+    <row r="295" spans="1:16">
       <c r="A295">
         <v>1105</v>
       </c>
@@ -47925,7 +47868,7 @@
       </c>
       <c r="P295" s="1"/>
     </row>
-    <row r="296" spans="1:19">
+    <row r="296" spans="1:16">
       <c r="A296">
         <v>1106</v>
       </c>
@@ -47964,7 +47907,7 @@
       </c>
       <c r="P296" s="1"/>
     </row>
-    <row r="297" spans="1:19">
+    <row r="297" spans="1:16">
       <c r="A297">
         <v>1107</v>
       </c>
@@ -48003,7 +47946,7 @@
       </c>
       <c r="P297" s="1"/>
     </row>
-    <row r="298" spans="1:19">
+    <row r="298" spans="1:16">
       <c r="A298">
         <v>1108</v>
       </c>
@@ -48042,7 +47985,7 @@
       </c>
       <c r="P298" s="1"/>
     </row>
-    <row r="299" spans="1:19">
+    <row r="299" spans="1:16">
       <c r="A299">
         <v>1109</v>
       </c>
@@ -48081,7 +48024,7 @@
       </c>
       <c r="P299" s="1"/>
     </row>
-    <row r="300" spans="1:19">
+    <row r="300" spans="1:16">
       <c r="A300">
         <v>1110</v>
       </c>
@@ -48120,7 +48063,7 @@
       </c>
       <c r="P300" s="1"/>
     </row>
-    <row r="301" spans="1:19">
+    <row r="301" spans="1:16">
       <c r="A301">
         <v>1111</v>
       </c>
@@ -48159,7 +48102,7 @@
       </c>
       <c r="P301" s="1"/>
     </row>
-    <row r="302" spans="1:19">
+    <row r="302" spans="1:16">
       <c r="A302">
         <v>1112</v>
       </c>
@@ -48198,7 +48141,7 @@
       </c>
       <c r="P302" s="1"/>
     </row>
-    <row r="303" spans="1:19">
+    <row r="303" spans="1:16">
       <c r="A303">
         <v>1113</v>
       </c>
@@ -48237,7 +48180,7 @@
       </c>
       <c r="P303" s="1"/>
     </row>
-    <row r="304" spans="1:19">
+    <row r="304" spans="1:16">
       <c r="A304">
         <v>1114</v>
       </c>
@@ -49575,7 +49518,7 @@
       </c>
       <c r="P336" s="1"/>
     </row>
-    <row r="337" spans="1:19">
+    <row r="337" spans="1:16">
       <c r="A337">
         <v>1147</v>
       </c>
@@ -49617,7 +49560,7 @@
       </c>
       <c r="P337" s="1"/>
     </row>
-    <row r="338" spans="1:19">
+    <row r="338" spans="1:16">
       <c r="A338">
         <v>1148</v>
       </c>
@@ -49652,7 +49595,7 @@
       </c>
       <c r="P338" s="1"/>
     </row>
-    <row r="339" spans="1:19">
+    <row r="339" spans="1:16">
       <c r="A339">
         <v>1149</v>
       </c>
@@ -49694,7 +49637,7 @@
       </c>
       <c r="P339" s="1"/>
     </row>
-    <row r="340" spans="1:19">
+    <row r="340" spans="1:16">
       <c r="A340">
         <v>1150</v>
       </c>
@@ -49736,7 +49679,7 @@
       </c>
       <c r="P340" s="1"/>
     </row>
-    <row r="341" spans="1:19">
+    <row r="341" spans="1:16">
       <c r="A341">
         <v>1151</v>
       </c>
@@ -49771,7 +49714,7 @@
       </c>
       <c r="P341" s="1"/>
     </row>
-    <row r="342" spans="1:19">
+    <row r="342" spans="1:16">
       <c r="A342">
         <v>1152</v>
       </c>
@@ -49806,7 +49749,7 @@
       </c>
       <c r="P342" s="1"/>
     </row>
-    <row r="343" spans="1:19">
+    <row r="343" spans="1:16">
       <c r="A343">
         <v>1153</v>
       </c>
@@ -49841,7 +49784,7 @@
       </c>
       <c r="P343" s="1"/>
     </row>
-    <row r="344" spans="1:19">
+    <row r="344" spans="1:16">
       <c r="A344">
         <v>1154</v>
       </c>
@@ -49876,7 +49819,7 @@
       </c>
       <c r="P344" s="1"/>
     </row>
-    <row r="345" spans="1:19">
+    <row r="345" spans="1:16">
       <c r="A345">
         <v>1155</v>
       </c>
@@ -49911,7 +49854,7 @@
       </c>
       <c r="P345" s="1"/>
     </row>
-    <row r="346" spans="1:19">
+    <row r="346" spans="1:16">
       <c r="A346">
         <v>1156</v>
       </c>
@@ -49950,7 +49893,7 @@
       </c>
       <c r="P346" s="1"/>
     </row>
-    <row r="347" spans="1:19">
+    <row r="347" spans="1:16">
       <c r="A347">
         <v>1157</v>
       </c>
@@ -49988,11 +49931,8 @@
         <v>955</v>
       </c>
       <c r="P347" s="1"/>
-      <c r="S347" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="348" spans="1:19">
+    </row>
+    <row r="348" spans="1:16">
       <c r="A348">
         <v>1158</v>
       </c>
@@ -50030,11 +49970,8 @@
         <v>955</v>
       </c>
       <c r="P348" s="1"/>
-      <c r="S348" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="349" spans="1:19">
+    </row>
+    <row r="349" spans="1:16">
       <c r="A349">
         <v>1159</v>
       </c>
@@ -50075,11 +50012,8 @@
         <v>955</v>
       </c>
       <c r="P349" s="1"/>
-      <c r="S349" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="350" spans="1:19">
+    </row>
+    <row r="350" spans="1:16">
       <c r="A350">
         <v>1160</v>
       </c>
@@ -50112,7 +50046,7 @@
       </c>
       <c r="P350" s="1"/>
     </row>
-    <row r="351" spans="1:19">
+    <row r="351" spans="1:16">
       <c r="A351">
         <v>1161</v>
       </c>
@@ -50145,7 +50079,7 @@
       </c>
       <c r="P351" s="1"/>
     </row>
-    <row r="352" spans="1:19">
+    <row r="352" spans="1:16">
       <c r="A352">
         <v>1162</v>
       </c>
@@ -50258,9 +50192,6 @@
         <v>955</v>
       </c>
       <c r="P354" s="1"/>
-      <c r="S354" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="355" spans="1:19">
       <c r="A355">
@@ -50303,9 +50234,6 @@
         <v>955</v>
       </c>
       <c r="P355" s="1"/>
-      <c r="S355" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="356" spans="1:19">
       <c r="A356">
@@ -50348,9 +50276,6 @@
         <v>955</v>
       </c>
       <c r="P356" s="1"/>
-      <c r="S356" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="357" spans="1:19">
       <c r="A357">
@@ -62619,9 +62544,6 @@
         <v>955</v>
       </c>
       <c r="P267" s="1"/>
-      <c r="S267" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="268" spans="1:19">
       <c r="A268">
@@ -62661,9 +62583,6 @@
         <v>955</v>
       </c>
       <c r="P268" s="1"/>
-      <c r="S268" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="269" spans="1:19">
       <c r="A269">
@@ -64112,7 +64031,7 @@
         <v>2143</v>
       </c>
     </row>
-    <row r="305" spans="1:19">
+    <row r="305" spans="1:16">
       <c r="A305">
         <v>753</v>
       </c>
@@ -64147,7 +64066,7 @@
       </c>
       <c r="P305" s="1"/>
     </row>
-    <row r="306" spans="1:19">
+    <row r="306" spans="1:16">
       <c r="A306">
         <v>754</v>
       </c>
@@ -64188,11 +64107,8 @@
         <v>955</v>
       </c>
       <c r="P306" s="1"/>
-      <c r="S306" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="307" spans="1:19">
+    </row>
+    <row r="307" spans="1:16">
       <c r="A307">
         <v>755</v>
       </c>
@@ -64233,11 +64149,8 @@
         <v>955</v>
       </c>
       <c r="P307" s="1"/>
-      <c r="S307" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="308" spans="1:19">
+    </row>
+    <row r="308" spans="1:16">
       <c r="A308">
         <v>756</v>
       </c>
@@ -64279,7 +64192,7 @@
       </c>
       <c r="P308" s="1"/>
     </row>
-    <row r="309" spans="1:19">
+    <row r="309" spans="1:16">
       <c r="A309">
         <v>757</v>
       </c>
@@ -64321,7 +64234,7 @@
       </c>
       <c r="P309" s="1"/>
     </row>
-    <row r="310" spans="1:19">
+    <row r="310" spans="1:16">
       <c r="A310">
         <v>758</v>
       </c>
@@ -64356,7 +64269,7 @@
       </c>
       <c r="P310" s="1"/>
     </row>
-    <row r="311" spans="1:19">
+    <row r="311" spans="1:16">
       <c r="A311">
         <v>759</v>
       </c>
@@ -64398,7 +64311,7 @@
       </c>
       <c r="P311" s="1"/>
     </row>
-    <row r="312" spans="1:19">
+    <row r="312" spans="1:16">
       <c r="A312">
         <v>760</v>
       </c>
@@ -64440,7 +64353,7 @@
       </c>
       <c r="P312" s="1"/>
     </row>
-    <row r="313" spans="1:19">
+    <row r="313" spans="1:16">
       <c r="A313">
         <v>761</v>
       </c>
@@ -64475,7 +64388,7 @@
       </c>
       <c r="P313" s="1"/>
     </row>
-    <row r="314" spans="1:19">
+    <row r="314" spans="1:16">
       <c r="A314">
         <v>762</v>
       </c>
@@ -64510,7 +64423,7 @@
       </c>
       <c r="P314" s="1"/>
     </row>
-    <row r="315" spans="1:19">
+    <row r="315" spans="1:16">
       <c r="A315">
         <v>763</v>
       </c>
@@ -64545,7 +64458,7 @@
       </c>
       <c r="P315" s="1"/>
     </row>
-    <row r="316" spans="1:19">
+    <row r="316" spans="1:16">
       <c r="A316">
         <v>764</v>
       </c>
@@ -64580,7 +64493,7 @@
       </c>
       <c r="P316" s="1"/>
     </row>
-    <row r="317" spans="1:19">
+    <row r="317" spans="1:16">
       <c r="A317">
         <v>765</v>
       </c>
@@ -64615,7 +64528,7 @@
       </c>
       <c r="P317" s="1"/>
     </row>
-    <row r="318" spans="1:19">
+    <row r="318" spans="1:16">
       <c r="A318">
         <v>766</v>
       </c>
@@ -64654,7 +64567,7 @@
       </c>
       <c r="P318" s="1"/>
     </row>
-    <row r="319" spans="1:19">
+    <row r="319" spans="1:16">
       <c r="A319">
         <v>767</v>
       </c>
@@ -64693,7 +64606,7 @@
       </c>
       <c r="P319" s="1"/>
     </row>
-    <row r="320" spans="1:19">
+    <row r="320" spans="1:16">
       <c r="A320">
         <v>768</v>
       </c>
@@ -64731,11 +64644,8 @@
         <v>955</v>
       </c>
       <c r="P320" s="1"/>
-      <c r="S320" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="321" spans="1:19">
+    </row>
+    <row r="321" spans="1:16">
       <c r="A321">
         <v>769</v>
       </c>
@@ -64776,11 +64686,8 @@
         <v>955</v>
       </c>
       <c r="P321" s="1"/>
-      <c r="S321" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="322" spans="1:19">
+    </row>
+    <row r="322" spans="1:16">
       <c r="A322">
         <v>770</v>
       </c>
@@ -64821,11 +64728,8 @@
         <v>955</v>
       </c>
       <c r="P322" s="1"/>
-      <c r="S322" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="323" spans="1:19">
+    </row>
+    <row r="323" spans="1:16">
       <c r="A323">
         <v>771</v>
       </c>
@@ -64866,11 +64770,8 @@
         <v>955</v>
       </c>
       <c r="P323" s="1"/>
-      <c r="S323" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="324" spans="1:19">
+    </row>
+    <row r="324" spans="1:16">
       <c r="A324">
         <v>772</v>
       </c>
@@ -64911,11 +64812,8 @@
         <v>955</v>
       </c>
       <c r="P324" s="1"/>
-      <c r="S324" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="325" spans="1:19">
+    </row>
+    <row r="325" spans="1:16">
       <c r="A325">
         <v>773</v>
       </c>
@@ -64953,11 +64851,8 @@
         <v>955</v>
       </c>
       <c r="P325" s="1"/>
-      <c r="S325" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="326" spans="1:19">
+    </row>
+    <row r="326" spans="1:16">
       <c r="A326">
         <v>774</v>
       </c>
@@ -64995,11 +64890,8 @@
         <v>955</v>
       </c>
       <c r="P326" s="1"/>
-      <c r="S326" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="327" spans="1:19">
+    </row>
+    <row r="327" spans="1:16">
       <c r="A327">
         <v>775</v>
       </c>
@@ -65037,11 +64929,8 @@
         <v>955</v>
       </c>
       <c r="P327" s="1"/>
-      <c r="S327" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="328" spans="1:19">
+    </row>
+    <row r="328" spans="1:16">
       <c r="A328">
         <v>776</v>
       </c>
@@ -65079,11 +64968,8 @@
         <v>955</v>
       </c>
       <c r="P328" s="1"/>
-      <c r="S328" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="329" spans="1:19">
+    </row>
+    <row r="329" spans="1:16">
       <c r="A329">
         <v>777</v>
       </c>
@@ -65121,11 +65007,8 @@
         <v>955</v>
       </c>
       <c r="P329" s="1"/>
-      <c r="S329" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="330" spans="1:19">
+    </row>
+    <row r="330" spans="1:16">
       <c r="A330">
         <v>778</v>
       </c>
@@ -65163,11 +65046,8 @@
         <v>955</v>
       </c>
       <c r="P330" s="1"/>
-      <c r="S330" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="331" spans="1:19">
+    </row>
+    <row r="331" spans="1:16">
       <c r="A331">
         <v>779</v>
       </c>
@@ -65205,11 +65085,8 @@
         <v>955</v>
       </c>
       <c r="P331" s="1"/>
-      <c r="S331" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="332" spans="1:19">
+    </row>
+    <row r="332" spans="1:16">
       <c r="A332">
         <v>780</v>
       </c>
@@ -65247,11 +65124,8 @@
         <v>955</v>
       </c>
       <c r="P332" s="1"/>
-      <c r="S332" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="333" spans="1:19">
+    </row>
+    <row r="333" spans="1:16">
       <c r="A333">
         <v>781</v>
       </c>
@@ -65289,11 +65163,8 @@
         <v>955</v>
       </c>
       <c r="P333" s="1"/>
-      <c r="S333" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="334" spans="1:19">
+    </row>
+    <row r="334" spans="1:16">
       <c r="A334">
         <v>782</v>
       </c>
@@ -65331,11 +65202,8 @@
         <v>955</v>
       </c>
       <c r="P334" s="1"/>
-      <c r="S334" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="335" spans="1:19">
+    </row>
+    <row r="335" spans="1:16">
       <c r="A335">
         <v>783</v>
       </c>
@@ -65376,11 +65244,8 @@
         <v>955</v>
       </c>
       <c r="P335" s="1"/>
-      <c r="S335" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="336" spans="1:19">
+    </row>
+    <row r="336" spans="1:16">
       <c r="A336">
         <v>784</v>
       </c>
@@ -65421,11 +65286,8 @@
         <v>955</v>
       </c>
       <c r="P336" s="1"/>
-      <c r="S336" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="337" spans="1:19">
+    </row>
+    <row r="337" spans="1:16">
       <c r="A337">
         <v>785</v>
       </c>
@@ -65464,7 +65326,7 @@
       </c>
       <c r="P337" s="1"/>
     </row>
-    <row r="338" spans="1:19">
+    <row r="338" spans="1:16">
       <c r="A338">
         <v>786</v>
       </c>
@@ -65499,7 +65361,7 @@
       </c>
       <c r="P338" s="1"/>
     </row>
-    <row r="339" spans="1:19">
+    <row r="339" spans="1:16">
       <c r="A339">
         <v>787</v>
       </c>
@@ -65534,7 +65396,7 @@
       </c>
       <c r="P339" s="1"/>
     </row>
-    <row r="340" spans="1:19">
+    <row r="340" spans="1:16">
       <c r="A340">
         <v>788</v>
       </c>
@@ -65569,7 +65431,7 @@
       </c>
       <c r="P340" s="1"/>
     </row>
-    <row r="341" spans="1:19">
+    <row r="341" spans="1:16">
       <c r="A341">
         <v>789</v>
       </c>
@@ -65604,7 +65466,7 @@
       </c>
       <c r="P341" s="1"/>
     </row>
-    <row r="342" spans="1:19">
+    <row r="342" spans="1:16">
       <c r="A342">
         <v>790</v>
       </c>
@@ -65642,11 +65504,8 @@
         <v>955</v>
       </c>
       <c r="P342" s="1"/>
-      <c r="S342" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="343" spans="1:19">
+    </row>
+    <row r="343" spans="1:16">
       <c r="A343">
         <v>791</v>
       </c>
@@ -65684,11 +65543,8 @@
         <v>955</v>
       </c>
       <c r="P343" s="1"/>
-      <c r="S343" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="344" spans="1:19">
+    </row>
+    <row r="344" spans="1:16">
       <c r="A344">
         <v>792</v>
       </c>
@@ -65726,11 +65582,8 @@
         <v>955</v>
       </c>
       <c r="P344" s="1"/>
-      <c r="S344" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="345" spans="1:19">
+    </row>
+    <row r="345" spans="1:16">
       <c r="A345">
         <v>793</v>
       </c>
@@ -65768,11 +65621,8 @@
         <v>955</v>
       </c>
       <c r="P345" s="1"/>
-      <c r="S345" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="346" spans="1:19">
+    </row>
+    <row r="346" spans="1:16">
       <c r="A346">
         <v>794</v>
       </c>
@@ -65813,11 +65663,8 @@
         <v>955</v>
       </c>
       <c r="P346" s="1"/>
-      <c r="S346" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="347" spans="1:19">
+    </row>
+    <row r="347" spans="1:16">
       <c r="A347">
         <v>795</v>
       </c>
@@ -65855,11 +65702,8 @@
         <v>955</v>
       </c>
       <c r="P347" s="1"/>
-      <c r="S347" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="348" spans="1:19">
+    </row>
+    <row r="348" spans="1:16">
       <c r="A348">
         <v>796</v>
       </c>
@@ -65898,7 +65742,7 @@
       </c>
       <c r="P348" s="1"/>
     </row>
-    <row r="349" spans="1:19">
+    <row r="349" spans="1:16">
       <c r="A349">
         <v>797</v>
       </c>
@@ -65937,7 +65781,7 @@
       </c>
       <c r="P349" s="1"/>
     </row>
-    <row r="350" spans="1:19">
+    <row r="350" spans="1:16">
       <c r="A350">
         <v>798</v>
       </c>
@@ -65979,7 +65823,7 @@
       </c>
       <c r="P350" s="1"/>
     </row>
-    <row r="351" spans="1:19">
+    <row r="351" spans="1:16">
       <c r="A351">
         <v>799</v>
       </c>
@@ -66021,7 +65865,7 @@
       </c>
       <c r="P351" s="1"/>
     </row>
-    <row r="352" spans="1:19">
+    <row r="352" spans="1:16">
       <c r="A352">
         <v>800</v>
       </c>

</xml_diff>